<commit_message>
Tweak XLSX template after Marcus' feedback - large project name, background colour on headings
#3286

git-svn-id: file:///mnt/ramdisk/d4-svn/trunk@10341 484df14f-75d2-4b3f-8ba0-490e05069a01
</commit_message>
<xml_diff>
--- a/businessintelligenceplugin/default-transformation-templates/ticket-list/report-template.xlsx
+++ b/businessintelligenceplugin/default-transformation-templates/ticket-list/report-template.xlsx
@@ -21,7 +21,7 @@
   </definedNames>
   <calcPr calcId="145621" iterateDelta="1E-4"/>
   <pivotCaches>
-    <pivotCache cacheId="7" r:id="rId3"/>
+    <pivotCache cacheId="22" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
@@ -120,7 +120,7 @@
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -154,10 +154,31 @@
       <sz val="11"/>
       <color indexed="12"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="28"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -171,6 +192,12 @@
     </fill>
     <fill>
       <patternFill patternType="none">
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -212,8 +239,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -222,34 +247,23 @@
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="2">
     <dxf>
       <font>
         <color theme="5" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
       </font>
     </dxf>
     <dxf>
@@ -351,11 +365,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="111194112"/>
-        <c:axId val="111195648"/>
+        <c:axId val="112390528"/>
+        <c:axId val="232361984"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="111194112"/>
+        <c:axId val="112390528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -364,7 +378,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="111195648"/>
+        <c:crossAx val="232361984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -372,7 +386,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="111195648"/>
+        <c:axId val="232361984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -383,7 +397,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="111194112"/>
+        <c:crossAx val="112390528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -421,14 +435,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>255661</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>80311</xdr:rowOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>4111</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>125372</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>57151</xdr:rowOff>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -444,7 +458,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="255661" y="651811"/>
-          <a:ext cx="307861" cy="167340"/>
+          <a:ext cx="344414" cy="157814"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -466,8 +480,8 @@
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>379428</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>333375</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -678,7 +692,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="Piper, Nick" refreshedDate="41417.552109259261" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="243">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="Piper, Nick" refreshedDate="41417.604668981483" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="243">
   <cacheSource type="worksheet">
     <worksheetSource ref="A7:O10000" sheet="Tickets"/>
   </cacheSource>
@@ -4887,7 +4901,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="22" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="B4:D7" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="15">
     <pivotField showAll="0"/>
@@ -5323,7 +5337,7 @@
   <dimension ref="A1:AML249"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5348,1888 +5362,1888 @@
   <sheetData>
     <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1"/>
-      <c r="G1" s="13"/>
-    </row>
-    <row r="2" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G1" s="11"/>
+    </row>
+    <row r="2" spans="1:16" s="2" customFormat="1" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="C2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="4"/>
+      <c r="D2" s="16"/>
       <c r="E2" s="5"/>
-      <c r="G2" s="13"/>
+      <c r="G2" s="11"/>
     </row>
     <row r="3" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="8"/>
+      <c r="D3" s="6"/>
       <c r="E3" s="5"/>
-      <c r="G3" s="13"/>
+      <c r="G3" s="11"/>
     </row>
     <row r="4" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C4" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="4"/>
-      <c r="G4" s="13"/>
+      <c r="G4" s="11"/>
     </row>
     <row r="5" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="G5" s="13"/>
+      <c r="G5" s="11"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="M6" s="11"/>
-      <c r="N6" s="11"/>
-      <c r="O6" s="11"/>
-    </row>
-    <row r="7" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
+    </row>
+    <row r="7" spans="1:16" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="14" t="s">
         <v>8</v>
       </c>
       <c r="G7" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I7" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J7" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="K7" t="s">
+      <c r="K7" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="L7" t="s">
+      <c r="L7" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="M7" t="s">
+      <c r="M7" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="N7" t="s">
+      <c r="N7" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="O7" t="s">
+      <c r="O7" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="P7" t="s">
+      <c r="P7" s="14" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
-      <c r="L8" s="9"/>
-      <c r="M8" s="10"/>
-      <c r="N8" s="10"/>
-      <c r="O8" s="10"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="8"/>
+      <c r="N8" s="8"/>
+      <c r="O8" s="8"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="9"/>
-      <c r="L9" s="9"/>
-      <c r="M9" s="10"/>
-      <c r="N9" s="10"/>
-      <c r="O9" s="10"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="8"/>
+      <c r="O9" s="8"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="9"/>
-      <c r="M10" s="10"/>
-      <c r="N10" s="10"/>
-      <c r="O10" s="10"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="8"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="9"/>
-      <c r="L11" s="9"/>
-      <c r="M11" s="10"/>
-      <c r="N11" s="10"/>
-      <c r="O11" s="10"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="8"/>
+      <c r="O11" s="8"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
-      <c r="L12" s="9"/>
-      <c r="M12" s="10"/>
-      <c r="N12" s="10"/>
-      <c r="O12" s="10"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="8"/>
+      <c r="O12" s="8"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="9"/>
-      <c r="L13" s="9"/>
-      <c r="M13" s="10"/>
-      <c r="N13" s="10"/>
-      <c r="O13" s="10"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="8"/>
+      <c r="O13" s="8"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
-      <c r="J14" s="9"/>
-      <c r="K14" s="9"/>
-      <c r="L14" s="9"/>
-      <c r="M14" s="10"/>
-      <c r="N14" s="10"/>
-      <c r="O14" s="10"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
+      <c r="O14" s="8"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
-      <c r="J15" s="9"/>
-      <c r="K15" s="9"/>
-      <c r="L15" s="9"/>
-      <c r="M15" s="10"/>
-      <c r="N15" s="10"/>
-      <c r="O15" s="10"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="8"/>
+      <c r="O15" s="8"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
-      <c r="J16" s="9"/>
-      <c r="K16" s="9"/>
-      <c r="L16" s="9"/>
-      <c r="M16" s="10"/>
-      <c r="N16" s="10"/>
-      <c r="O16" s="10"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="8"/>
+      <c r="O16" s="8"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
-      <c r="J17" s="9"/>
-      <c r="K17" s="9"/>
-      <c r="L17" s="9"/>
-      <c r="M17" s="10"/>
-      <c r="N17" s="10"/>
-      <c r="O17" s="10"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="7"/>
+      <c r="M17" s="8"/>
+      <c r="N17" s="8"/>
+      <c r="O17" s="8"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
-      <c r="J18" s="9"/>
-      <c r="K18" s="9"/>
-      <c r="L18" s="9"/>
-      <c r="M18" s="10"/>
-      <c r="N18" s="10"/>
-      <c r="O18" s="10"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
+      <c r="L18" s="7"/>
+      <c r="M18" s="8"/>
+      <c r="N18" s="8"/>
+      <c r="O18" s="8"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
-      <c r="J19" s="9"/>
-      <c r="K19" s="9"/>
-      <c r="L19" s="9"/>
-      <c r="M19" s="10"/>
-      <c r="N19" s="10"/>
-      <c r="O19" s="10"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="8"/>
+      <c r="N19" s="8"/>
+      <c r="O19" s="8"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
-      <c r="J20" s="9"/>
-      <c r="K20" s="9"/>
-      <c r="L20" s="9"/>
-      <c r="M20" s="10"/>
-      <c r="N20" s="10"/>
-      <c r="O20" s="10"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
+      <c r="M20" s="8"/>
+      <c r="N20" s="8"/>
+      <c r="O20" s="8"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
-      <c r="J21" s="9"/>
-      <c r="K21" s="9"/>
-      <c r="L21" s="9"/>
-      <c r="M21" s="10"/>
-      <c r="N21" s="10"/>
-      <c r="O21" s="10"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="7"/>
+      <c r="L21" s="7"/>
+      <c r="M21" s="8"/>
+      <c r="N21" s="8"/>
+      <c r="O21" s="8"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
-      <c r="J22" s="9"/>
-      <c r="K22" s="9"/>
-      <c r="L22" s="9"/>
-      <c r="M22" s="10"/>
-      <c r="N22" s="10"/>
-      <c r="O22" s="10"/>
+      <c r="J22" s="7"/>
+      <c r="K22" s="7"/>
+      <c r="L22" s="7"/>
+      <c r="M22" s="8"/>
+      <c r="N22" s="8"/>
+      <c r="O22" s="8"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
-      <c r="J23" s="9"/>
-      <c r="K23" s="9"/>
-      <c r="L23" s="9"/>
-      <c r="M23" s="10"/>
-      <c r="N23" s="10"/>
-      <c r="O23" s="10"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="7"/>
+      <c r="M23" s="8"/>
+      <c r="N23" s="8"/>
+      <c r="O23" s="8"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
-      <c r="J24" s="9"/>
-      <c r="K24" s="9"/>
-      <c r="L24" s="9"/>
-      <c r="M24" s="10"/>
-      <c r="N24" s="10"/>
-      <c r="O24" s="10"/>
+      <c r="J24" s="7"/>
+      <c r="K24" s="7"/>
+      <c r="L24" s="7"/>
+      <c r="M24" s="8"/>
+      <c r="N24" s="8"/>
+      <c r="O24" s="8"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
-      <c r="J25" s="9"/>
-      <c r="K25" s="9"/>
-      <c r="L25" s="9"/>
-      <c r="M25" s="10"/>
-      <c r="N25" s="10"/>
-      <c r="O25" s="10"/>
+      <c r="J25" s="7"/>
+      <c r="K25" s="7"/>
+      <c r="L25" s="7"/>
+      <c r="M25" s="8"/>
+      <c r="N25" s="8"/>
+      <c r="O25" s="8"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
-      <c r="J26" s="9"/>
-      <c r="K26" s="9"/>
-      <c r="L26" s="9"/>
-      <c r="M26" s="10"/>
-      <c r="N26" s="10"/>
-      <c r="O26" s="10"/>
+      <c r="J26" s="7"/>
+      <c r="K26" s="7"/>
+      <c r="L26" s="7"/>
+      <c r="M26" s="8"/>
+      <c r="N26" s="8"/>
+      <c r="O26" s="8"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
-      <c r="J27" s="9"/>
-      <c r="K27" s="9"/>
-      <c r="L27" s="9"/>
-      <c r="M27" s="10"/>
-      <c r="N27" s="10"/>
-      <c r="O27" s="10"/>
+      <c r="J27" s="7"/>
+      <c r="K27" s="7"/>
+      <c r="L27" s="7"/>
+      <c r="M27" s="8"/>
+      <c r="N27" s="8"/>
+      <c r="O27" s="8"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
-      <c r="J28" s="9"/>
-      <c r="K28" s="9"/>
-      <c r="L28" s="9"/>
-      <c r="M28" s="10"/>
-      <c r="N28" s="10"/>
-      <c r="O28" s="10"/>
+      <c r="J28" s="7"/>
+      <c r="K28" s="7"/>
+      <c r="L28" s="7"/>
+      <c r="M28" s="8"/>
+      <c r="N28" s="8"/>
+      <c r="O28" s="8"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
-      <c r="J29" s="9"/>
-      <c r="K29" s="9"/>
-      <c r="L29" s="9"/>
-      <c r="M29" s="10"/>
-      <c r="N29" s="10"/>
-      <c r="O29" s="10"/>
+      <c r="J29" s="7"/>
+      <c r="K29" s="7"/>
+      <c r="L29" s="7"/>
+      <c r="M29" s="8"/>
+      <c r="N29" s="8"/>
+      <c r="O29" s="8"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
-      <c r="J30" s="9"/>
-      <c r="K30" s="9"/>
-      <c r="L30" s="9"/>
-      <c r="M30" s="10"/>
-      <c r="N30" s="10"/>
-      <c r="O30" s="10"/>
+      <c r="J30" s="7"/>
+      <c r="K30" s="7"/>
+      <c r="L30" s="7"/>
+      <c r="M30" s="8"/>
+      <c r="N30" s="8"/>
+      <c r="O30" s="8"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
-      <c r="J31" s="9"/>
-      <c r="K31" s="9"/>
-      <c r="L31" s="9"/>
-      <c r="M31" s="10"/>
-      <c r="N31" s="10"/>
-      <c r="O31" s="10"/>
+      <c r="J31" s="7"/>
+      <c r="K31" s="7"/>
+      <c r="L31" s="7"/>
+      <c r="M31" s="8"/>
+      <c r="N31" s="8"/>
+      <c r="O31" s="8"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
-      <c r="J32" s="9"/>
-      <c r="K32" s="9"/>
-      <c r="L32" s="9"/>
-      <c r="M32" s="10"/>
-      <c r="N32" s="10"/>
-      <c r="O32" s="10"/>
+      <c r="J32" s="7"/>
+      <c r="K32" s="7"/>
+      <c r="L32" s="7"/>
+      <c r="M32" s="8"/>
+      <c r="N32" s="8"/>
+      <c r="O32" s="8"/>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
-      <c r="J33" s="9"/>
-      <c r="K33" s="9"/>
-      <c r="L33" s="9"/>
-      <c r="M33" s="10"/>
-      <c r="N33" s="10"/>
-      <c r="O33" s="10"/>
+      <c r="J33" s="7"/>
+      <c r="K33" s="7"/>
+      <c r="L33" s="7"/>
+      <c r="M33" s="8"/>
+      <c r="N33" s="8"/>
+      <c r="O33" s="8"/>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
-      <c r="J34" s="9"/>
-      <c r="K34" s="9"/>
-      <c r="L34" s="9"/>
-      <c r="M34" s="10"/>
-      <c r="N34" s="10"/>
-      <c r="O34" s="10"/>
+      <c r="J34" s="7"/>
+      <c r="K34" s="7"/>
+      <c r="L34" s="7"/>
+      <c r="M34" s="8"/>
+      <c r="N34" s="8"/>
+      <c r="O34" s="8"/>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
-      <c r="J35" s="9"/>
-      <c r="K35" s="9"/>
-      <c r="L35" s="9"/>
-      <c r="M35" s="10"/>
-      <c r="N35" s="10"/>
-      <c r="O35" s="10"/>
+      <c r="J35" s="7"/>
+      <c r="K35" s="7"/>
+      <c r="L35" s="7"/>
+      <c r="M35" s="8"/>
+      <c r="N35" s="8"/>
+      <c r="O35" s="8"/>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
-      <c r="J36" s="9"/>
-      <c r="K36" s="9"/>
-      <c r="L36" s="9"/>
-      <c r="M36" s="10"/>
-      <c r="N36" s="10"/>
-      <c r="O36" s="10"/>
+      <c r="J36" s="7"/>
+      <c r="K36" s="7"/>
+      <c r="L36" s="7"/>
+      <c r="M36" s="8"/>
+      <c r="N36" s="8"/>
+      <c r="O36" s="8"/>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
-      <c r="J37" s="9"/>
-      <c r="K37" s="9"/>
-      <c r="L37" s="9"/>
-      <c r="M37" s="10"/>
-      <c r="N37" s="10"/>
-      <c r="O37" s="10"/>
+      <c r="J37" s="7"/>
+      <c r="K37" s="7"/>
+      <c r="L37" s="7"/>
+      <c r="M37" s="8"/>
+      <c r="N37" s="8"/>
+      <c r="O37" s="8"/>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
-      <c r="J38" s="9"/>
-      <c r="K38" s="9"/>
-      <c r="L38" s="9"/>
-      <c r="M38" s="10"/>
-      <c r="N38" s="10"/>
-      <c r="O38" s="10"/>
+      <c r="J38" s="7"/>
+      <c r="K38" s="7"/>
+      <c r="L38" s="7"/>
+      <c r="M38" s="8"/>
+      <c r="N38" s="8"/>
+      <c r="O38" s="8"/>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
-      <c r="J39" s="9"/>
-      <c r="K39" s="9"/>
-      <c r="L39" s="9"/>
-      <c r="M39" s="10"/>
-      <c r="N39" s="10"/>
-      <c r="O39" s="10"/>
+      <c r="J39" s="7"/>
+      <c r="K39" s="7"/>
+      <c r="L39" s="7"/>
+      <c r="M39" s="8"/>
+      <c r="N39" s="8"/>
+      <c r="O39" s="8"/>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
-      <c r="J40" s="9"/>
-      <c r="K40" s="9"/>
-      <c r="L40" s="9"/>
-      <c r="M40" s="10"/>
-      <c r="N40" s="10"/>
-      <c r="O40" s="10"/>
+      <c r="J40" s="7"/>
+      <c r="K40" s="7"/>
+      <c r="L40" s="7"/>
+      <c r="M40" s="8"/>
+      <c r="N40" s="8"/>
+      <c r="O40" s="8"/>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
-      <c r="J41" s="9"/>
-      <c r="K41" s="9"/>
-      <c r="L41" s="9"/>
-      <c r="M41" s="10"/>
-      <c r="N41" s="10"/>
-      <c r="O41" s="10"/>
+      <c r="J41" s="7"/>
+      <c r="K41" s="7"/>
+      <c r="L41" s="7"/>
+      <c r="M41" s="8"/>
+      <c r="N41" s="8"/>
+      <c r="O41" s="8"/>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
-      <c r="J42" s="9"/>
-      <c r="K42" s="9"/>
-      <c r="L42" s="9"/>
-      <c r="M42" s="10"/>
-      <c r="N42" s="10"/>
-      <c r="O42" s="10"/>
+      <c r="J42" s="7"/>
+      <c r="K42" s="7"/>
+      <c r="L42" s="7"/>
+      <c r="M42" s="8"/>
+      <c r="N42" s="8"/>
+      <c r="O42" s="8"/>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
-      <c r="J43" s="9"/>
-      <c r="K43" s="9"/>
-      <c r="L43" s="9"/>
-      <c r="M43" s="10"/>
-      <c r="N43" s="10"/>
-      <c r="O43" s="10"/>
+      <c r="J43" s="7"/>
+      <c r="K43" s="7"/>
+      <c r="L43" s="7"/>
+      <c r="M43" s="8"/>
+      <c r="N43" s="8"/>
+      <c r="O43" s="8"/>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
-      <c r="J44" s="9"/>
-      <c r="K44" s="9"/>
-      <c r="L44" s="9"/>
-      <c r="M44" s="10"/>
-      <c r="N44" s="10"/>
-      <c r="O44" s="10"/>
+      <c r="J44" s="7"/>
+      <c r="K44" s="7"/>
+      <c r="L44" s="7"/>
+      <c r="M44" s="8"/>
+      <c r="N44" s="8"/>
+      <c r="O44" s="8"/>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
-      <c r="J45" s="9"/>
-      <c r="K45" s="9"/>
-      <c r="L45" s="9"/>
-      <c r="M45" s="10"/>
-      <c r="N45" s="10"/>
-      <c r="O45" s="10"/>
+      <c r="J45" s="7"/>
+      <c r="K45" s="7"/>
+      <c r="L45" s="7"/>
+      <c r="M45" s="8"/>
+      <c r="N45" s="8"/>
+      <c r="O45" s="8"/>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
-      <c r="J46" s="9"/>
-      <c r="K46" s="9"/>
-      <c r="L46" s="9"/>
-      <c r="M46" s="10"/>
-      <c r="N46" s="10"/>
-      <c r="O46" s="10"/>
+      <c r="J46" s="7"/>
+      <c r="K46" s="7"/>
+      <c r="L46" s="7"/>
+      <c r="M46" s="8"/>
+      <c r="N46" s="8"/>
+      <c r="O46" s="8"/>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
-      <c r="J47" s="9"/>
-      <c r="K47" s="9"/>
-      <c r="L47" s="9"/>
-      <c r="M47" s="10"/>
-      <c r="N47" s="10"/>
-      <c r="O47" s="10"/>
+      <c r="J47" s="7"/>
+      <c r="K47" s="7"/>
+      <c r="L47" s="7"/>
+      <c r="M47" s="8"/>
+      <c r="N47" s="8"/>
+      <c r="O47" s="8"/>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
-      <c r="J48" s="9"/>
-      <c r="K48" s="9"/>
-      <c r="L48" s="9"/>
-      <c r="M48" s="10"/>
-      <c r="N48" s="10"/>
-      <c r="O48" s="10"/>
+      <c r="J48" s="7"/>
+      <c r="K48" s="7"/>
+      <c r="L48" s="7"/>
+      <c r="M48" s="8"/>
+      <c r="N48" s="8"/>
+      <c r="O48" s="8"/>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
-      <c r="J49" s="9"/>
-      <c r="K49" s="9"/>
-      <c r="L49" s="9"/>
-      <c r="M49" s="10"/>
-      <c r="N49" s="10"/>
-      <c r="O49" s="10"/>
+      <c r="J49" s="7"/>
+      <c r="K49" s="7"/>
+      <c r="L49" s="7"/>
+      <c r="M49" s="8"/>
+      <c r="N49" s="8"/>
+      <c r="O49" s="8"/>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
-      <c r="J50" s="9"/>
-      <c r="K50" s="9"/>
-      <c r="L50" s="9"/>
-      <c r="M50" s="10"/>
-      <c r="N50" s="10"/>
-      <c r="O50" s="10"/>
+      <c r="J50" s="7"/>
+      <c r="K50" s="7"/>
+      <c r="L50" s="7"/>
+      <c r="M50" s="8"/>
+      <c r="N50" s="8"/>
+      <c r="O50" s="8"/>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
-      <c r="J51" s="9"/>
-      <c r="K51" s="9"/>
-      <c r="L51" s="9"/>
-      <c r="M51" s="10"/>
-      <c r="N51" s="10"/>
-      <c r="O51" s="10"/>
+      <c r="J51" s="7"/>
+      <c r="K51" s="7"/>
+      <c r="L51" s="7"/>
+      <c r="M51" s="8"/>
+      <c r="N51" s="8"/>
+      <c r="O51" s="8"/>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
-      <c r="J52" s="9"/>
-      <c r="K52" s="9"/>
-      <c r="L52" s="9"/>
-      <c r="M52" s="10"/>
-      <c r="N52" s="10"/>
-      <c r="O52" s="10"/>
+      <c r="J52" s="7"/>
+      <c r="K52" s="7"/>
+      <c r="L52" s="7"/>
+      <c r="M52" s="8"/>
+      <c r="N52" s="8"/>
+      <c r="O52" s="8"/>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
-      <c r="J53" s="9"/>
-      <c r="K53" s="9"/>
-      <c r="L53" s="9"/>
-      <c r="M53" s="10"/>
-      <c r="N53" s="10"/>
-      <c r="O53" s="10"/>
+      <c r="J53" s="7"/>
+      <c r="K53" s="7"/>
+      <c r="L53" s="7"/>
+      <c r="M53" s="8"/>
+      <c r="N53" s="8"/>
+      <c r="O53" s="8"/>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
-      <c r="J54" s="9"/>
-      <c r="K54" s="9"/>
-      <c r="L54" s="9"/>
-      <c r="M54" s="10"/>
-      <c r="N54" s="10"/>
-      <c r="O54" s="10"/>
+      <c r="J54" s="7"/>
+      <c r="K54" s="7"/>
+      <c r="L54" s="7"/>
+      <c r="M54" s="8"/>
+      <c r="N54" s="8"/>
+      <c r="O54" s="8"/>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
-      <c r="J55" s="9"/>
-      <c r="K55" s="9"/>
-      <c r="L55" s="9"/>
-      <c r="M55" s="10"/>
-      <c r="N55" s="10"/>
-      <c r="O55" s="10"/>
+      <c r="J55" s="7"/>
+      <c r="K55" s="7"/>
+      <c r="L55" s="7"/>
+      <c r="M55" s="8"/>
+      <c r="N55" s="8"/>
+      <c r="O55" s="8"/>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
-      <c r="J56" s="9"/>
-      <c r="K56" s="9"/>
-      <c r="L56" s="9"/>
-      <c r="M56" s="10"/>
-      <c r="N56" s="10"/>
-      <c r="O56" s="10"/>
+      <c r="J56" s="7"/>
+      <c r="K56" s="7"/>
+      <c r="L56" s="7"/>
+      <c r="M56" s="8"/>
+      <c r="N56" s="8"/>
+      <c r="O56" s="8"/>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
-      <c r="J57" s="9"/>
-      <c r="K57" s="9"/>
-      <c r="L57" s="9"/>
-      <c r="M57" s="10"/>
-      <c r="N57" s="10"/>
-      <c r="O57" s="10"/>
+      <c r="J57" s="7"/>
+      <c r="K57" s="7"/>
+      <c r="L57" s="7"/>
+      <c r="M57" s="8"/>
+      <c r="N57" s="8"/>
+      <c r="O57" s="8"/>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
-      <c r="J58" s="9"/>
-      <c r="K58" s="9"/>
-      <c r="L58" s="9"/>
-      <c r="M58" s="10"/>
-      <c r="N58" s="10"/>
-      <c r="O58" s="10"/>
+      <c r="J58" s="7"/>
+      <c r="K58" s="7"/>
+      <c r="L58" s="7"/>
+      <c r="M58" s="8"/>
+      <c r="N58" s="8"/>
+      <c r="O58" s="8"/>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
-      <c r="J59" s="9"/>
-      <c r="K59" s="9"/>
-      <c r="L59" s="9"/>
-      <c r="M59" s="10"/>
-      <c r="N59" s="10"/>
-      <c r="O59" s="10"/>
+      <c r="J59" s="7"/>
+      <c r="K59" s="7"/>
+      <c r="L59" s="7"/>
+      <c r="M59" s="8"/>
+      <c r="N59" s="8"/>
+      <c r="O59" s="8"/>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
-      <c r="J60" s="9"/>
-      <c r="K60" s="9"/>
-      <c r="L60" s="9"/>
-      <c r="M60" s="10"/>
-      <c r="N60" s="10"/>
-      <c r="O60" s="10"/>
+      <c r="J60" s="7"/>
+      <c r="K60" s="7"/>
+      <c r="L60" s="7"/>
+      <c r="M60" s="8"/>
+      <c r="N60" s="8"/>
+      <c r="O60" s="8"/>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
-      <c r="J61" s="9"/>
-      <c r="K61" s="9"/>
-      <c r="L61" s="9"/>
-      <c r="M61" s="10"/>
-      <c r="N61" s="10"/>
-      <c r="O61" s="10"/>
+      <c r="J61" s="7"/>
+      <c r="K61" s="7"/>
+      <c r="L61" s="7"/>
+      <c r="M61" s="8"/>
+      <c r="N61" s="8"/>
+      <c r="O61" s="8"/>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
-      <c r="J62" s="9"/>
-      <c r="K62" s="9"/>
-      <c r="L62" s="9"/>
-      <c r="M62" s="10"/>
-      <c r="N62" s="10"/>
-      <c r="O62" s="10"/>
+      <c r="J62" s="7"/>
+      <c r="K62" s="7"/>
+      <c r="L62" s="7"/>
+      <c r="M62" s="8"/>
+      <c r="N62" s="8"/>
+      <c r="O62" s="8"/>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
-      <c r="J63" s="9"/>
-      <c r="K63" s="9"/>
-      <c r="L63" s="9"/>
-      <c r="M63" s="10"/>
-      <c r="N63" s="10"/>
-      <c r="O63" s="10"/>
+      <c r="J63" s="7"/>
+      <c r="K63" s="7"/>
+      <c r="L63" s="7"/>
+      <c r="M63" s="8"/>
+      <c r="N63" s="8"/>
+      <c r="O63" s="8"/>
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
-      <c r="J64" s="9"/>
-      <c r="K64" s="9"/>
-      <c r="L64" s="9"/>
-      <c r="M64" s="10"/>
-      <c r="N64" s="10"/>
-      <c r="O64" s="10"/>
+      <c r="J64" s="7"/>
+      <c r="K64" s="7"/>
+      <c r="L64" s="7"/>
+      <c r="M64" s="8"/>
+      <c r="N64" s="8"/>
+      <c r="O64" s="8"/>
     </row>
     <row r="65" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
-      <c r="J65" s="9"/>
-      <c r="K65" s="9"/>
-      <c r="L65" s="9"/>
-      <c r="M65" s="10"/>
-      <c r="N65" s="10"/>
-      <c r="O65" s="10"/>
+      <c r="J65" s="7"/>
+      <c r="K65" s="7"/>
+      <c r="L65" s="7"/>
+      <c r="M65" s="8"/>
+      <c r="N65" s="8"/>
+      <c r="O65" s="8"/>
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
-      <c r="J66" s="9"/>
-      <c r="K66" s="9"/>
-      <c r="L66" s="9"/>
-      <c r="M66" s="10"/>
-      <c r="N66" s="10"/>
-      <c r="O66" s="10"/>
+      <c r="J66" s="7"/>
+      <c r="K66" s="7"/>
+      <c r="L66" s="7"/>
+      <c r="M66" s="8"/>
+      <c r="N66" s="8"/>
+      <c r="O66" s="8"/>
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
-      <c r="J67" s="9"/>
-      <c r="K67" s="9"/>
-      <c r="L67" s="9"/>
-      <c r="M67" s="10"/>
-      <c r="N67" s="10"/>
-      <c r="O67" s="10"/>
+      <c r="J67" s="7"/>
+      <c r="K67" s="7"/>
+      <c r="L67" s="7"/>
+      <c r="M67" s="8"/>
+      <c r="N67" s="8"/>
+      <c r="O67" s="8"/>
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
-      <c r="J68" s="9"/>
-      <c r="K68" s="9"/>
-      <c r="L68" s="9"/>
-      <c r="M68" s="10"/>
-      <c r="N68" s="10"/>
-      <c r="O68" s="10"/>
+      <c r="J68" s="7"/>
+      <c r="K68" s="7"/>
+      <c r="L68" s="7"/>
+      <c r="M68" s="8"/>
+      <c r="N68" s="8"/>
+      <c r="O68" s="8"/>
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
-      <c r="J69" s="9"/>
-      <c r="K69" s="9"/>
-      <c r="L69" s="9"/>
-      <c r="M69" s="10"/>
-      <c r="N69" s="10"/>
-      <c r="O69" s="10"/>
+      <c r="J69" s="7"/>
+      <c r="K69" s="7"/>
+      <c r="L69" s="7"/>
+      <c r="M69" s="8"/>
+      <c r="N69" s="8"/>
+      <c r="O69" s="8"/>
     </row>
     <row r="70" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
-      <c r="J70" s="9"/>
-      <c r="K70" s="9"/>
-      <c r="L70" s="9"/>
-      <c r="M70" s="10"/>
-      <c r="N70" s="10"/>
-      <c r="O70" s="10"/>
+      <c r="J70" s="7"/>
+      <c r="K70" s="7"/>
+      <c r="L70" s="7"/>
+      <c r="M70" s="8"/>
+      <c r="N70" s="8"/>
+      <c r="O70" s="8"/>
     </row>
     <row r="71" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
-      <c r="J71" s="9"/>
-      <c r="K71" s="9"/>
-      <c r="L71" s="9"/>
-      <c r="M71" s="10"/>
-      <c r="N71" s="10"/>
-      <c r="O71" s="10"/>
+      <c r="J71" s="7"/>
+      <c r="K71" s="7"/>
+      <c r="L71" s="7"/>
+      <c r="M71" s="8"/>
+      <c r="N71" s="8"/>
+      <c r="O71" s="8"/>
     </row>
     <row r="72" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
-      <c r="J72" s="9"/>
-      <c r="K72" s="9"/>
-      <c r="L72" s="9"/>
-      <c r="M72" s="10"/>
-      <c r="N72" s="10"/>
-      <c r="O72" s="10"/>
+      <c r="J72" s="7"/>
+      <c r="K72" s="7"/>
+      <c r="L72" s="7"/>
+      <c r="M72" s="8"/>
+      <c r="N72" s="8"/>
+      <c r="O72" s="8"/>
     </row>
     <row r="73" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
-      <c r="J73" s="9"/>
-      <c r="K73" s="9"/>
-      <c r="L73" s="9"/>
-      <c r="M73" s="10"/>
-      <c r="N73" s="10"/>
-      <c r="O73" s="10"/>
+      <c r="J73" s="7"/>
+      <c r="K73" s="7"/>
+      <c r="L73" s="7"/>
+      <c r="M73" s="8"/>
+      <c r="N73" s="8"/>
+      <c r="O73" s="8"/>
     </row>
     <row r="74" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
-      <c r="J74" s="9"/>
-      <c r="K74" s="9"/>
-      <c r="L74" s="9"/>
-      <c r="M74" s="10"/>
-      <c r="N74" s="10"/>
-      <c r="O74" s="10"/>
+      <c r="J74" s="7"/>
+      <c r="K74" s="7"/>
+      <c r="L74" s="7"/>
+      <c r="M74" s="8"/>
+      <c r="N74" s="8"/>
+      <c r="O74" s="8"/>
     </row>
     <row r="75" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
-      <c r="J75" s="9"/>
-      <c r="K75" s="9"/>
-      <c r="L75" s="9"/>
-      <c r="M75" s="10"/>
-      <c r="N75" s="10"/>
-      <c r="O75" s="10"/>
+      <c r="J75" s="7"/>
+      <c r="K75" s="7"/>
+      <c r="L75" s="7"/>
+      <c r="M75" s="8"/>
+      <c r="N75" s="8"/>
+      <c r="O75" s="8"/>
     </row>
     <row r="76" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
-      <c r="J76" s="9"/>
-      <c r="K76" s="9"/>
-      <c r="L76" s="9"/>
-      <c r="M76" s="10"/>
-      <c r="N76" s="10"/>
-      <c r="O76" s="10"/>
+      <c r="J76" s="7"/>
+      <c r="K76" s="7"/>
+      <c r="L76" s="7"/>
+      <c r="M76" s="8"/>
+      <c r="N76" s="8"/>
+      <c r="O76" s="8"/>
     </row>
     <row r="77" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
-      <c r="J77" s="9"/>
-      <c r="K77" s="9"/>
-      <c r="L77" s="9"/>
-      <c r="M77" s="10"/>
-      <c r="N77" s="10"/>
-      <c r="O77" s="10"/>
+      <c r="J77" s="7"/>
+      <c r="K77" s="7"/>
+      <c r="L77" s="7"/>
+      <c r="M77" s="8"/>
+      <c r="N77" s="8"/>
+      <c r="O77" s="8"/>
     </row>
     <row r="78" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
-      <c r="J78" s="9"/>
-      <c r="K78" s="9"/>
-      <c r="L78" s="9"/>
-      <c r="M78" s="10"/>
-      <c r="N78" s="10"/>
-      <c r="O78" s="10"/>
+      <c r="J78" s="7"/>
+      <c r="K78" s="7"/>
+      <c r="L78" s="7"/>
+      <c r="M78" s="8"/>
+      <c r="N78" s="8"/>
+      <c r="O78" s="8"/>
     </row>
     <row r="79" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
-      <c r="J79" s="9"/>
-      <c r="K79" s="9"/>
-      <c r="L79" s="9"/>
-      <c r="M79" s="10"/>
-      <c r="N79" s="10"/>
-      <c r="O79" s="10"/>
+      <c r="J79" s="7"/>
+      <c r="K79" s="7"/>
+      <c r="L79" s="7"/>
+      <c r="M79" s="8"/>
+      <c r="N79" s="8"/>
+      <c r="O79" s="8"/>
     </row>
     <row r="80" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
-      <c r="J80" s="9"/>
-      <c r="K80" s="9"/>
-      <c r="L80" s="9"/>
-      <c r="M80" s="10"/>
-      <c r="N80" s="10"/>
-      <c r="O80" s="10"/>
+      <c r="J80" s="7"/>
+      <c r="K80" s="7"/>
+      <c r="L80" s="7"/>
+      <c r="M80" s="8"/>
+      <c r="N80" s="8"/>
+      <c r="O80" s="8"/>
     </row>
     <row r="81" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
-      <c r="J81" s="9"/>
-      <c r="K81" s="9"/>
-      <c r="L81" s="9"/>
-      <c r="M81" s="10"/>
-      <c r="N81" s="10"/>
-      <c r="O81" s="10"/>
+      <c r="J81" s="7"/>
+      <c r="K81" s="7"/>
+      <c r="L81" s="7"/>
+      <c r="M81" s="8"/>
+      <c r="N81" s="8"/>
+      <c r="O81" s="8"/>
     </row>
     <row r="82" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
-      <c r="J82" s="9"/>
-      <c r="K82" s="9"/>
-      <c r="L82" s="9"/>
-      <c r="M82" s="10"/>
-      <c r="N82" s="10"/>
-      <c r="O82" s="10"/>
+      <c r="J82" s="7"/>
+      <c r="K82" s="7"/>
+      <c r="L82" s="7"/>
+      <c r="M82" s="8"/>
+      <c r="N82" s="8"/>
+      <c r="O82" s="8"/>
     </row>
     <row r="83" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
-      <c r="J83" s="9"/>
-      <c r="K83" s="9"/>
-      <c r="L83" s="9"/>
-      <c r="M83" s="10"/>
-      <c r="N83" s="10"/>
-      <c r="O83" s="10"/>
+      <c r="J83" s="7"/>
+      <c r="K83" s="7"/>
+      <c r="L83" s="7"/>
+      <c r="M83" s="8"/>
+      <c r="N83" s="8"/>
+      <c r="O83" s="8"/>
     </row>
     <row r="84" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
-      <c r="J84" s="9"/>
-      <c r="K84" s="9"/>
-      <c r="L84" s="9"/>
-      <c r="M84" s="10"/>
-      <c r="N84" s="10"/>
-      <c r="O84" s="10"/>
+      <c r="J84" s="7"/>
+      <c r="K84" s="7"/>
+      <c r="L84" s="7"/>
+      <c r="M84" s="8"/>
+      <c r="N84" s="8"/>
+      <c r="O84" s="8"/>
     </row>
     <row r="85" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
-      <c r="J85" s="9"/>
-      <c r="K85" s="9"/>
-      <c r="L85" s="9"/>
-      <c r="M85" s="10"/>
-      <c r="N85" s="10"/>
-      <c r="O85" s="10"/>
+      <c r="J85" s="7"/>
+      <c r="K85" s="7"/>
+      <c r="L85" s="7"/>
+      <c r="M85" s="8"/>
+      <c r="N85" s="8"/>
+      <c r="O85" s="8"/>
     </row>
     <row r="86" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
-      <c r="J86" s="9"/>
-      <c r="K86" s="9"/>
-      <c r="L86" s="9"/>
-      <c r="M86" s="10"/>
-      <c r="N86" s="10"/>
-      <c r="O86" s="10"/>
+      <c r="J86" s="7"/>
+      <c r="K86" s="7"/>
+      <c r="L86" s="7"/>
+      <c r="M86" s="8"/>
+      <c r="N86" s="8"/>
+      <c r="O86" s="8"/>
     </row>
     <row r="87" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
-      <c r="J87" s="9"/>
-      <c r="K87" s="9"/>
-      <c r="L87" s="9"/>
-      <c r="M87" s="10"/>
-      <c r="N87" s="10"/>
-      <c r="O87" s="10"/>
+      <c r="J87" s="7"/>
+      <c r="K87" s="7"/>
+      <c r="L87" s="7"/>
+      <c r="M87" s="8"/>
+      <c r="N87" s="8"/>
+      <c r="O87" s="8"/>
     </row>
     <row r="88" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
-      <c r="J88" s="9"/>
-      <c r="K88" s="9"/>
-      <c r="L88" s="9"/>
-      <c r="M88" s="10"/>
-      <c r="N88" s="10"/>
-      <c r="O88" s="10"/>
+      <c r="J88" s="7"/>
+      <c r="K88" s="7"/>
+      <c r="L88" s="7"/>
+      <c r="M88" s="8"/>
+      <c r="N88" s="8"/>
+      <c r="O88" s="8"/>
     </row>
     <row r="89" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
-      <c r="J89" s="9"/>
-      <c r="K89" s="9"/>
-      <c r="L89" s="9"/>
-      <c r="M89" s="10"/>
-      <c r="N89" s="10"/>
-      <c r="O89" s="10"/>
+      <c r="J89" s="7"/>
+      <c r="K89" s="7"/>
+      <c r="L89" s="7"/>
+      <c r="M89" s="8"/>
+      <c r="N89" s="8"/>
+      <c r="O89" s="8"/>
     </row>
     <row r="90" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
-      <c r="J90" s="9"/>
-      <c r="K90" s="9"/>
-      <c r="L90" s="9"/>
-      <c r="M90" s="10"/>
-      <c r="N90" s="10"/>
-      <c r="O90" s="10"/>
+      <c r="J90" s="7"/>
+      <c r="K90" s="7"/>
+      <c r="L90" s="7"/>
+      <c r="M90" s="8"/>
+      <c r="N90" s="8"/>
+      <c r="O90" s="8"/>
     </row>
     <row r="91" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
-      <c r="J91" s="9"/>
-      <c r="K91" s="9"/>
-      <c r="L91" s="9"/>
-      <c r="M91" s="10"/>
-      <c r="N91" s="10"/>
-      <c r="O91" s="10"/>
+      <c r="J91" s="7"/>
+      <c r="K91" s="7"/>
+      <c r="L91" s="7"/>
+      <c r="M91" s="8"/>
+      <c r="N91" s="8"/>
+      <c r="O91" s="8"/>
     </row>
     <row r="92" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
-      <c r="J92" s="9"/>
-      <c r="K92" s="9"/>
-      <c r="L92" s="9"/>
-      <c r="M92" s="10"/>
-      <c r="N92" s="10"/>
-      <c r="O92" s="10"/>
+      <c r="J92" s="7"/>
+      <c r="K92" s="7"/>
+      <c r="L92" s="7"/>
+      <c r="M92" s="8"/>
+      <c r="N92" s="8"/>
+      <c r="O92" s="8"/>
     </row>
     <row r="93" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
-      <c r="J93" s="9"/>
-      <c r="K93" s="9"/>
-      <c r="L93" s="9"/>
-      <c r="M93" s="10"/>
-      <c r="N93" s="10"/>
-      <c r="O93" s="10"/>
+      <c r="J93" s="7"/>
+      <c r="K93" s="7"/>
+      <c r="L93" s="7"/>
+      <c r="M93" s="8"/>
+      <c r="N93" s="8"/>
+      <c r="O93" s="8"/>
     </row>
     <row r="94" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
-      <c r="J94" s="9"/>
-      <c r="K94" s="9"/>
-      <c r="L94" s="9"/>
-      <c r="M94" s="10"/>
-      <c r="N94" s="10"/>
-      <c r="O94" s="10"/>
+      <c r="J94" s="7"/>
+      <c r="K94" s="7"/>
+      <c r="L94" s="7"/>
+      <c r="M94" s="8"/>
+      <c r="N94" s="8"/>
+      <c r="O94" s="8"/>
     </row>
     <row r="95" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
-      <c r="J95" s="9"/>
-      <c r="K95" s="9"/>
-      <c r="L95" s="9"/>
-      <c r="M95" s="10"/>
-      <c r="N95" s="10"/>
-      <c r="O95" s="10"/>
+      <c r="J95" s="7"/>
+      <c r="K95" s="7"/>
+      <c r="L95" s="7"/>
+      <c r="M95" s="8"/>
+      <c r="N95" s="8"/>
+      <c r="O95" s="8"/>
     </row>
     <row r="96" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
-      <c r="J96" s="9"/>
-      <c r="K96" s="9"/>
-      <c r="L96" s="9"/>
-      <c r="M96" s="10"/>
-      <c r="N96" s="10"/>
-      <c r="O96" s="10"/>
+      <c r="J96" s="7"/>
+      <c r="K96" s="7"/>
+      <c r="L96" s="7"/>
+      <c r="M96" s="8"/>
+      <c r="N96" s="8"/>
+      <c r="O96" s="8"/>
     </row>
     <row r="97" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
-      <c r="J97" s="9"/>
-      <c r="K97" s="9"/>
-      <c r="L97" s="9"/>
-      <c r="M97" s="10"/>
-      <c r="N97" s="10"/>
-      <c r="O97" s="10"/>
+      <c r="J97" s="7"/>
+      <c r="K97" s="7"/>
+      <c r="L97" s="7"/>
+      <c r="M97" s="8"/>
+      <c r="N97" s="8"/>
+      <c r="O97" s="8"/>
     </row>
     <row r="98" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A98" s="1"/>
-      <c r="J98" s="9"/>
-      <c r="K98" s="9"/>
-      <c r="L98" s="9"/>
-      <c r="M98" s="10"/>
-      <c r="N98" s="10"/>
-      <c r="O98" s="10"/>
+      <c r="J98" s="7"/>
+      <c r="K98" s="7"/>
+      <c r="L98" s="7"/>
+      <c r="M98" s="8"/>
+      <c r="N98" s="8"/>
+      <c r="O98" s="8"/>
     </row>
     <row r="99" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A99" s="1"/>
-      <c r="J99" s="9"/>
-      <c r="K99" s="9"/>
-      <c r="L99" s="9"/>
-      <c r="M99" s="10"/>
-      <c r="N99" s="10"/>
-      <c r="O99" s="10"/>
+      <c r="J99" s="7"/>
+      <c r="K99" s="7"/>
+      <c r="L99" s="7"/>
+      <c r="M99" s="8"/>
+      <c r="N99" s="8"/>
+      <c r="O99" s="8"/>
     </row>
     <row r="100" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
-      <c r="J100" s="9"/>
-      <c r="K100" s="9"/>
-      <c r="L100" s="9"/>
-      <c r="M100" s="10"/>
-      <c r="N100" s="10"/>
-      <c r="O100" s="10"/>
+      <c r="J100" s="7"/>
+      <c r="K100" s="7"/>
+      <c r="L100" s="7"/>
+      <c r="M100" s="8"/>
+      <c r="N100" s="8"/>
+      <c r="O100" s="8"/>
     </row>
     <row r="101" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A101" s="1"/>
-      <c r="J101" s="9"/>
-      <c r="K101" s="9"/>
-      <c r="L101" s="9"/>
-      <c r="M101" s="10"/>
-      <c r="N101" s="10"/>
-      <c r="O101" s="10"/>
+      <c r="J101" s="7"/>
+      <c r="K101" s="7"/>
+      <c r="L101" s="7"/>
+      <c r="M101" s="8"/>
+      <c r="N101" s="8"/>
+      <c r="O101" s="8"/>
     </row>
     <row r="102" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A102" s="1"/>
-      <c r="J102" s="9"/>
-      <c r="K102" s="9"/>
-      <c r="L102" s="9"/>
-      <c r="M102" s="10"/>
-      <c r="N102" s="10"/>
-      <c r="O102" s="10"/>
+      <c r="J102" s="7"/>
+      <c r="K102" s="7"/>
+      <c r="L102" s="7"/>
+      <c r="M102" s="8"/>
+      <c r="N102" s="8"/>
+      <c r="O102" s="8"/>
     </row>
     <row r="103" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A103" s="1"/>
-      <c r="J103" s="9"/>
-      <c r="K103" s="9"/>
-      <c r="L103" s="9"/>
-      <c r="M103" s="10"/>
-      <c r="N103" s="10"/>
-      <c r="O103" s="10"/>
+      <c r="J103" s="7"/>
+      <c r="K103" s="7"/>
+      <c r="L103" s="7"/>
+      <c r="M103" s="8"/>
+      <c r="N103" s="8"/>
+      <c r="O103" s="8"/>
     </row>
     <row r="104" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A104" s="1"/>
-      <c r="J104" s="9"/>
-      <c r="K104" s="9"/>
-      <c r="L104" s="9"/>
-      <c r="M104" s="10"/>
-      <c r="N104" s="10"/>
-      <c r="O104" s="10"/>
+      <c r="J104" s="7"/>
+      <c r="K104" s="7"/>
+      <c r="L104" s="7"/>
+      <c r="M104" s="8"/>
+      <c r="N104" s="8"/>
+      <c r="O104" s="8"/>
     </row>
     <row r="105" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A105" s="1"/>
-      <c r="J105" s="9"/>
-      <c r="K105" s="9"/>
-      <c r="L105" s="9"/>
-      <c r="M105" s="10"/>
-      <c r="N105" s="10"/>
-      <c r="O105" s="10"/>
+      <c r="J105" s="7"/>
+      <c r="K105" s="7"/>
+      <c r="L105" s="7"/>
+      <c r="M105" s="8"/>
+      <c r="N105" s="8"/>
+      <c r="O105" s="8"/>
     </row>
     <row r="106" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A106" s="1"/>
-      <c r="J106" s="9"/>
-      <c r="K106" s="9"/>
-      <c r="L106" s="9"/>
-      <c r="M106" s="10"/>
-      <c r="N106" s="10"/>
-      <c r="O106" s="10"/>
+      <c r="J106" s="7"/>
+      <c r="K106" s="7"/>
+      <c r="L106" s="7"/>
+      <c r="M106" s="8"/>
+      <c r="N106" s="8"/>
+      <c r="O106" s="8"/>
     </row>
     <row r="107" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A107" s="1"/>
-      <c r="J107" s="9"/>
-      <c r="K107" s="9"/>
-      <c r="L107" s="9"/>
-      <c r="M107" s="10"/>
-      <c r="N107" s="10"/>
-      <c r="O107" s="10"/>
+      <c r="J107" s="7"/>
+      <c r="K107" s="7"/>
+      <c r="L107" s="7"/>
+      <c r="M107" s="8"/>
+      <c r="N107" s="8"/>
+      <c r="O107" s="8"/>
     </row>
     <row r="108" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A108" s="1"/>
-      <c r="J108" s="9"/>
-      <c r="K108" s="9"/>
-      <c r="L108" s="9"/>
-      <c r="M108" s="10"/>
-      <c r="N108" s="10"/>
-      <c r="O108" s="10"/>
+      <c r="J108" s="7"/>
+      <c r="K108" s="7"/>
+      <c r="L108" s="7"/>
+      <c r="M108" s="8"/>
+      <c r="N108" s="8"/>
+      <c r="O108" s="8"/>
     </row>
     <row r="109" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A109" s="1"/>
-      <c r="J109" s="9"/>
-      <c r="K109" s="9"/>
-      <c r="L109" s="9"/>
-      <c r="M109" s="10"/>
-      <c r="N109" s="10"/>
-      <c r="O109" s="10"/>
+      <c r="J109" s="7"/>
+      <c r="K109" s="7"/>
+      <c r="L109" s="7"/>
+      <c r="M109" s="8"/>
+      <c r="N109" s="8"/>
+      <c r="O109" s="8"/>
     </row>
     <row r="110" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A110" s="1"/>
-      <c r="J110" s="9"/>
-      <c r="K110" s="9"/>
-      <c r="L110" s="9"/>
-      <c r="M110" s="10"/>
-      <c r="N110" s="10"/>
-      <c r="O110" s="10"/>
+      <c r="J110" s="7"/>
+      <c r="K110" s="7"/>
+      <c r="L110" s="7"/>
+      <c r="M110" s="8"/>
+      <c r="N110" s="8"/>
+      <c r="O110" s="8"/>
     </row>
     <row r="111" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A111" s="1"/>
-      <c r="J111" s="9"/>
-      <c r="K111" s="9"/>
-      <c r="L111" s="9"/>
-      <c r="M111" s="10"/>
-      <c r="N111" s="10"/>
-      <c r="O111" s="10"/>
+      <c r="J111" s="7"/>
+      <c r="K111" s="7"/>
+      <c r="L111" s="7"/>
+      <c r="M111" s="8"/>
+      <c r="N111" s="8"/>
+      <c r="O111" s="8"/>
     </row>
     <row r="112" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A112" s="1"/>
-      <c r="J112" s="9"/>
-      <c r="K112" s="9"/>
-      <c r="L112" s="9"/>
-      <c r="M112" s="10"/>
-      <c r="N112" s="10"/>
-      <c r="O112" s="10"/>
+      <c r="J112" s="7"/>
+      <c r="K112" s="7"/>
+      <c r="L112" s="7"/>
+      <c r="M112" s="8"/>
+      <c r="N112" s="8"/>
+      <c r="O112" s="8"/>
     </row>
     <row r="113" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A113" s="1"/>
-      <c r="J113" s="9"/>
-      <c r="K113" s="9"/>
-      <c r="L113" s="9"/>
-      <c r="M113" s="10"/>
-      <c r="N113" s="10"/>
-      <c r="O113" s="10"/>
+      <c r="J113" s="7"/>
+      <c r="K113" s="7"/>
+      <c r="L113" s="7"/>
+      <c r="M113" s="8"/>
+      <c r="N113" s="8"/>
+      <c r="O113" s="8"/>
     </row>
     <row r="114" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A114" s="1"/>
-      <c r="J114" s="9"/>
-      <c r="K114" s="9"/>
-      <c r="L114" s="9"/>
-      <c r="M114" s="10"/>
-      <c r="N114" s="10"/>
-      <c r="O114" s="10"/>
+      <c r="J114" s="7"/>
+      <c r="K114" s="7"/>
+      <c r="L114" s="7"/>
+      <c r="M114" s="8"/>
+      <c r="N114" s="8"/>
+      <c r="O114" s="8"/>
     </row>
     <row r="115" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A115" s="1"/>
-      <c r="J115" s="9"/>
-      <c r="K115" s="9"/>
-      <c r="L115" s="9"/>
-      <c r="M115" s="10"/>
-      <c r="N115" s="10"/>
-      <c r="O115" s="10"/>
+      <c r="J115" s="7"/>
+      <c r="K115" s="7"/>
+      <c r="L115" s="7"/>
+      <c r="M115" s="8"/>
+      <c r="N115" s="8"/>
+      <c r="O115" s="8"/>
     </row>
     <row r="116" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A116" s="1"/>
-      <c r="J116" s="9"/>
-      <c r="K116" s="9"/>
-      <c r="L116" s="9"/>
-      <c r="M116" s="10"/>
-      <c r="N116" s="10"/>
-      <c r="O116" s="10"/>
+      <c r="J116" s="7"/>
+      <c r="K116" s="7"/>
+      <c r="L116" s="7"/>
+      <c r="M116" s="8"/>
+      <c r="N116" s="8"/>
+      <c r="O116" s="8"/>
     </row>
     <row r="117" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A117" s="1"/>
-      <c r="J117" s="9"/>
-      <c r="K117" s="9"/>
-      <c r="L117" s="9"/>
-      <c r="M117" s="10"/>
-      <c r="N117" s="10"/>
-      <c r="O117" s="10"/>
+      <c r="J117" s="7"/>
+      <c r="K117" s="7"/>
+      <c r="L117" s="7"/>
+      <c r="M117" s="8"/>
+      <c r="N117" s="8"/>
+      <c r="O117" s="8"/>
     </row>
     <row r="118" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A118" s="1"/>
-      <c r="J118" s="9"/>
-      <c r="K118" s="9"/>
-      <c r="L118" s="9"/>
-      <c r="M118" s="10"/>
-      <c r="N118" s="10"/>
-      <c r="O118" s="10"/>
+      <c r="J118" s="7"/>
+      <c r="K118" s="7"/>
+      <c r="L118" s="7"/>
+      <c r="M118" s="8"/>
+      <c r="N118" s="8"/>
+      <c r="O118" s="8"/>
     </row>
     <row r="119" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A119" s="1"/>
-      <c r="J119" s="9"/>
-      <c r="K119" s="9"/>
-      <c r="L119" s="9"/>
-      <c r="M119" s="10"/>
-      <c r="N119" s="10"/>
-      <c r="O119" s="10"/>
+      <c r="J119" s="7"/>
+      <c r="K119" s="7"/>
+      <c r="L119" s="7"/>
+      <c r="M119" s="8"/>
+      <c r="N119" s="8"/>
+      <c r="O119" s="8"/>
     </row>
     <row r="120" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A120" s="1"/>
-      <c r="J120" s="9"/>
-      <c r="K120" s="9"/>
-      <c r="L120" s="9"/>
-      <c r="M120" s="10"/>
-      <c r="N120" s="10"/>
-      <c r="O120" s="10"/>
+      <c r="J120" s="7"/>
+      <c r="K120" s="7"/>
+      <c r="L120" s="7"/>
+      <c r="M120" s="8"/>
+      <c r="N120" s="8"/>
+      <c r="O120" s="8"/>
     </row>
     <row r="121" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A121" s="1"/>
-      <c r="J121" s="9"/>
-      <c r="K121" s="9"/>
-      <c r="L121" s="9"/>
-      <c r="M121" s="10"/>
-      <c r="N121" s="10"/>
-      <c r="O121" s="10"/>
+      <c r="J121" s="7"/>
+      <c r="K121" s="7"/>
+      <c r="L121" s="7"/>
+      <c r="M121" s="8"/>
+      <c r="N121" s="8"/>
+      <c r="O121" s="8"/>
     </row>
     <row r="122" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A122" s="1"/>
-      <c r="J122" s="9"/>
-      <c r="K122" s="9"/>
-      <c r="L122" s="9"/>
-      <c r="M122" s="10"/>
-      <c r="N122" s="10"/>
-      <c r="O122" s="10"/>
+      <c r="J122" s="7"/>
+      <c r="K122" s="7"/>
+      <c r="L122" s="7"/>
+      <c r="M122" s="8"/>
+      <c r="N122" s="8"/>
+      <c r="O122" s="8"/>
     </row>
     <row r="123" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A123" s="1"/>
-      <c r="J123" s="9"/>
-      <c r="K123" s="9"/>
-      <c r="L123" s="9"/>
-      <c r="M123" s="10"/>
-      <c r="N123" s="10"/>
-      <c r="O123" s="10"/>
+      <c r="J123" s="7"/>
+      <c r="K123" s="7"/>
+      <c r="L123" s="7"/>
+      <c r="M123" s="8"/>
+      <c r="N123" s="8"/>
+      <c r="O123" s="8"/>
     </row>
     <row r="124" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A124" s="1"/>
-      <c r="J124" s="9"/>
-      <c r="K124" s="9"/>
-      <c r="L124" s="9"/>
-      <c r="M124" s="10"/>
-      <c r="N124" s="10"/>
-      <c r="O124" s="10"/>
+      <c r="J124" s="7"/>
+      <c r="K124" s="7"/>
+      <c r="L124" s="7"/>
+      <c r="M124" s="8"/>
+      <c r="N124" s="8"/>
+      <c r="O124" s="8"/>
     </row>
     <row r="125" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A125" s="1"/>
-      <c r="J125" s="9"/>
-      <c r="K125" s="9"/>
-      <c r="L125" s="9"/>
-      <c r="M125" s="10"/>
-      <c r="N125" s="10"/>
-      <c r="O125" s="10"/>
+      <c r="J125" s="7"/>
+      <c r="K125" s="7"/>
+      <c r="L125" s="7"/>
+      <c r="M125" s="8"/>
+      <c r="N125" s="8"/>
+      <c r="O125" s="8"/>
     </row>
     <row r="126" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A126" s="1"/>
-      <c r="J126" s="9"/>
-      <c r="K126" s="9"/>
-      <c r="L126" s="9"/>
-      <c r="M126" s="10"/>
-      <c r="N126" s="10"/>
-      <c r="O126" s="10"/>
+      <c r="J126" s="7"/>
+      <c r="K126" s="7"/>
+      <c r="L126" s="7"/>
+      <c r="M126" s="8"/>
+      <c r="N126" s="8"/>
+      <c r="O126" s="8"/>
     </row>
     <row r="127" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A127" s="1"/>
-      <c r="J127" s="9"/>
-      <c r="K127" s="9"/>
-      <c r="L127" s="9"/>
-      <c r="M127" s="10"/>
-      <c r="N127" s="10"/>
-      <c r="O127" s="10"/>
+      <c r="J127" s="7"/>
+      <c r="K127" s="7"/>
+      <c r="L127" s="7"/>
+      <c r="M127" s="8"/>
+      <c r="N127" s="8"/>
+      <c r="O127" s="8"/>
     </row>
     <row r="128" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A128" s="1"/>
-      <c r="J128" s="9"/>
-      <c r="K128" s="9"/>
-      <c r="L128" s="9"/>
-      <c r="M128" s="10"/>
-      <c r="N128" s="10"/>
-      <c r="O128" s="10"/>
+      <c r="J128" s="7"/>
+      <c r="K128" s="7"/>
+      <c r="L128" s="7"/>
+      <c r="M128" s="8"/>
+      <c r="N128" s="8"/>
+      <c r="O128" s="8"/>
     </row>
     <row r="129" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A129" s="1"/>
-      <c r="J129" s="9"/>
-      <c r="K129" s="9"/>
-      <c r="L129" s="9"/>
-      <c r="M129" s="10"/>
-      <c r="N129" s="10"/>
-      <c r="O129" s="10"/>
+      <c r="J129" s="7"/>
+      <c r="K129" s="7"/>
+      <c r="L129" s="7"/>
+      <c r="M129" s="8"/>
+      <c r="N129" s="8"/>
+      <c r="O129" s="8"/>
     </row>
     <row r="130" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A130" s="1"/>
-      <c r="J130" s="9"/>
-      <c r="K130" s="9"/>
-      <c r="L130" s="9"/>
-      <c r="M130" s="10"/>
-      <c r="N130" s="10"/>
-      <c r="O130" s="10"/>
+      <c r="J130" s="7"/>
+      <c r="K130" s="7"/>
+      <c r="L130" s="7"/>
+      <c r="M130" s="8"/>
+      <c r="N130" s="8"/>
+      <c r="O130" s="8"/>
     </row>
     <row r="131" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A131" s="1"/>
-      <c r="J131" s="9"/>
-      <c r="K131" s="9"/>
-      <c r="L131" s="9"/>
-      <c r="M131" s="10"/>
-      <c r="N131" s="10"/>
-      <c r="O131" s="10"/>
+      <c r="J131" s="7"/>
+      <c r="K131" s="7"/>
+      <c r="L131" s="7"/>
+      <c r="M131" s="8"/>
+      <c r="N131" s="8"/>
+      <c r="O131" s="8"/>
     </row>
     <row r="132" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A132" s="1"/>
-      <c r="J132" s="9"/>
-      <c r="K132" s="9"/>
-      <c r="L132" s="9"/>
-      <c r="M132" s="10"/>
-      <c r="N132" s="10"/>
-      <c r="O132" s="10"/>
+      <c r="J132" s="7"/>
+      <c r="K132" s="7"/>
+      <c r="L132" s="7"/>
+      <c r="M132" s="8"/>
+      <c r="N132" s="8"/>
+      <c r="O132" s="8"/>
     </row>
     <row r="133" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A133" s="1"/>
-      <c r="J133" s="9"/>
-      <c r="K133" s="9"/>
-      <c r="L133" s="9"/>
-      <c r="M133" s="10"/>
-      <c r="N133" s="10"/>
-      <c r="O133" s="10"/>
+      <c r="J133" s="7"/>
+      <c r="K133" s="7"/>
+      <c r="L133" s="7"/>
+      <c r="M133" s="8"/>
+      <c r="N133" s="8"/>
+      <c r="O133" s="8"/>
     </row>
     <row r="134" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A134" s="1"/>
-      <c r="J134" s="9"/>
-      <c r="K134" s="9"/>
-      <c r="L134" s="9"/>
-      <c r="M134" s="10"/>
-      <c r="N134" s="10"/>
-      <c r="O134" s="10"/>
+      <c r="J134" s="7"/>
+      <c r="K134" s="7"/>
+      <c r="L134" s="7"/>
+      <c r="M134" s="8"/>
+      <c r="N134" s="8"/>
+      <c r="O134" s="8"/>
     </row>
     <row r="135" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A135" s="1"/>
-      <c r="J135" s="9"/>
-      <c r="K135" s="9"/>
-      <c r="L135" s="9"/>
-      <c r="M135" s="10"/>
-      <c r="N135" s="10"/>
-      <c r="O135" s="10"/>
+      <c r="J135" s="7"/>
+      <c r="K135" s="7"/>
+      <c r="L135" s="7"/>
+      <c r="M135" s="8"/>
+      <c r="N135" s="8"/>
+      <c r="O135" s="8"/>
     </row>
     <row r="136" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A136" s="1"/>
-      <c r="J136" s="9"/>
-      <c r="K136" s="9"/>
-      <c r="L136" s="9"/>
-      <c r="M136" s="10"/>
-      <c r="N136" s="10"/>
-      <c r="O136" s="10"/>
+      <c r="J136" s="7"/>
+      <c r="K136" s="7"/>
+      <c r="L136" s="7"/>
+      <c r="M136" s="8"/>
+      <c r="N136" s="8"/>
+      <c r="O136" s="8"/>
     </row>
     <row r="137" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A137" s="1"/>
-      <c r="J137" s="9"/>
-      <c r="K137" s="9"/>
-      <c r="L137" s="9"/>
-      <c r="M137" s="10"/>
-      <c r="N137" s="10"/>
-      <c r="O137" s="10"/>
+      <c r="J137" s="7"/>
+      <c r="K137" s="7"/>
+      <c r="L137" s="7"/>
+      <c r="M137" s="8"/>
+      <c r="N137" s="8"/>
+      <c r="O137" s="8"/>
     </row>
     <row r="138" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A138" s="1"/>
-      <c r="J138" s="9"/>
-      <c r="K138" s="9"/>
-      <c r="L138" s="9"/>
-      <c r="M138" s="10"/>
-      <c r="N138" s="10"/>
-      <c r="O138" s="10"/>
+      <c r="J138" s="7"/>
+      <c r="K138" s="7"/>
+      <c r="L138" s="7"/>
+      <c r="M138" s="8"/>
+      <c r="N138" s="8"/>
+      <c r="O138" s="8"/>
     </row>
     <row r="139" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A139" s="1"/>
-      <c r="J139" s="9"/>
-      <c r="K139" s="9"/>
-      <c r="L139" s="9"/>
-      <c r="M139" s="10"/>
-      <c r="N139" s="10"/>
-      <c r="O139" s="10"/>
+      <c r="J139" s="7"/>
+      <c r="K139" s="7"/>
+      <c r="L139" s="7"/>
+      <c r="M139" s="8"/>
+      <c r="N139" s="8"/>
+      <c r="O139" s="8"/>
     </row>
     <row r="140" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A140" s="1"/>
-      <c r="J140" s="9"/>
-      <c r="K140" s="9"/>
-      <c r="L140" s="9"/>
-      <c r="M140" s="10"/>
-      <c r="N140" s="10"/>
-      <c r="O140" s="10"/>
+      <c r="J140" s="7"/>
+      <c r="K140" s="7"/>
+      <c r="L140" s="7"/>
+      <c r="M140" s="8"/>
+      <c r="N140" s="8"/>
+      <c r="O140" s="8"/>
     </row>
     <row r="141" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A141" s="1"/>
-      <c r="J141" s="9"/>
-      <c r="K141" s="9"/>
-      <c r="L141" s="9"/>
-      <c r="M141" s="10"/>
-      <c r="N141" s="10"/>
-      <c r="O141" s="10"/>
+      <c r="J141" s="7"/>
+      <c r="K141" s="7"/>
+      <c r="L141" s="7"/>
+      <c r="M141" s="8"/>
+      <c r="N141" s="8"/>
+      <c r="O141" s="8"/>
     </row>
     <row r="142" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A142" s="1"/>
-      <c r="J142" s="9"/>
-      <c r="K142" s="9"/>
-      <c r="L142" s="9"/>
-      <c r="M142" s="10"/>
-      <c r="N142" s="10"/>
-      <c r="O142" s="10"/>
+      <c r="J142" s="7"/>
+      <c r="K142" s="7"/>
+      <c r="L142" s="7"/>
+      <c r="M142" s="8"/>
+      <c r="N142" s="8"/>
+      <c r="O142" s="8"/>
     </row>
     <row r="143" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A143" s="1"/>
-      <c r="J143" s="9"/>
-      <c r="K143" s="9"/>
-      <c r="L143" s="9"/>
-      <c r="M143" s="10"/>
-      <c r="N143" s="10"/>
-      <c r="O143" s="10"/>
+      <c r="J143" s="7"/>
+      <c r="K143" s="7"/>
+      <c r="L143" s="7"/>
+      <c r="M143" s="8"/>
+      <c r="N143" s="8"/>
+      <c r="O143" s="8"/>
     </row>
     <row r="144" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A144" s="1"/>
-      <c r="J144" s="9"/>
-      <c r="K144" s="9"/>
-      <c r="L144" s="9"/>
-      <c r="M144" s="10"/>
-      <c r="N144" s="10"/>
-      <c r="O144" s="10"/>
+      <c r="J144" s="7"/>
+      <c r="K144" s="7"/>
+      <c r="L144" s="7"/>
+      <c r="M144" s="8"/>
+      <c r="N144" s="8"/>
+      <c r="O144" s="8"/>
     </row>
     <row r="145" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A145" s="1"/>
-      <c r="J145" s="9"/>
-      <c r="K145" s="9"/>
-      <c r="L145" s="9"/>
-      <c r="M145" s="10"/>
-      <c r="N145" s="10"/>
-      <c r="O145" s="10"/>
+      <c r="J145" s="7"/>
+      <c r="K145" s="7"/>
+      <c r="L145" s="7"/>
+      <c r="M145" s="8"/>
+      <c r="N145" s="8"/>
+      <c r="O145" s="8"/>
     </row>
     <row r="146" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A146" s="1"/>
-      <c r="J146" s="9"/>
-      <c r="K146" s="9"/>
-      <c r="L146" s="9"/>
-      <c r="M146" s="10"/>
-      <c r="N146" s="10"/>
-      <c r="O146" s="10"/>
+      <c r="J146" s="7"/>
+      <c r="K146" s="7"/>
+      <c r="L146" s="7"/>
+      <c r="M146" s="8"/>
+      <c r="N146" s="8"/>
+      <c r="O146" s="8"/>
     </row>
     <row r="147" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A147" s="1"/>
-      <c r="J147" s="9"/>
-      <c r="K147" s="9"/>
-      <c r="L147" s="9"/>
-      <c r="M147" s="10"/>
-      <c r="N147" s="10"/>
-      <c r="O147" s="10"/>
+      <c r="J147" s="7"/>
+      <c r="K147" s="7"/>
+      <c r="L147" s="7"/>
+      <c r="M147" s="8"/>
+      <c r="N147" s="8"/>
+      <c r="O147" s="8"/>
     </row>
     <row r="148" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A148" s="1"/>
-      <c r="J148" s="9"/>
-      <c r="K148" s="9"/>
-      <c r="L148" s="9"/>
-      <c r="M148" s="10"/>
-      <c r="N148" s="10"/>
-      <c r="O148" s="10"/>
+      <c r="J148" s="7"/>
+      <c r="K148" s="7"/>
+      <c r="L148" s="7"/>
+      <c r="M148" s="8"/>
+      <c r="N148" s="8"/>
+      <c r="O148" s="8"/>
     </row>
     <row r="149" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A149" s="1"/>
-      <c r="J149" s="9"/>
-      <c r="K149" s="9"/>
-      <c r="L149" s="9"/>
-      <c r="M149" s="10"/>
-      <c r="N149" s="10"/>
-      <c r="O149" s="10"/>
+      <c r="J149" s="7"/>
+      <c r="K149" s="7"/>
+      <c r="L149" s="7"/>
+      <c r="M149" s="8"/>
+      <c r="N149" s="8"/>
+      <c r="O149" s="8"/>
     </row>
     <row r="150" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A150" s="1"/>
-      <c r="J150" s="9"/>
-      <c r="K150" s="9"/>
-      <c r="L150" s="9"/>
-      <c r="M150" s="10"/>
-      <c r="N150" s="10"/>
-      <c r="O150" s="10"/>
+      <c r="J150" s="7"/>
+      <c r="K150" s="7"/>
+      <c r="L150" s="7"/>
+      <c r="M150" s="8"/>
+      <c r="N150" s="8"/>
+      <c r="O150" s="8"/>
     </row>
     <row r="151" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A151" s="1"/>
-      <c r="J151" s="9"/>
-      <c r="K151" s="9"/>
-      <c r="L151" s="9"/>
-      <c r="M151" s="10"/>
-      <c r="N151" s="10"/>
-      <c r="O151" s="10"/>
+      <c r="J151" s="7"/>
+      <c r="K151" s="7"/>
+      <c r="L151" s="7"/>
+      <c r="M151" s="8"/>
+      <c r="N151" s="8"/>
+      <c r="O151" s="8"/>
     </row>
     <row r="152" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A152" s="1"/>
-      <c r="J152" s="9"/>
-      <c r="K152" s="9"/>
-      <c r="L152" s="9"/>
-      <c r="M152" s="10"/>
-      <c r="N152" s="10"/>
-      <c r="O152" s="10"/>
+      <c r="J152" s="7"/>
+      <c r="K152" s="7"/>
+      <c r="L152" s="7"/>
+      <c r="M152" s="8"/>
+      <c r="N152" s="8"/>
+      <c r="O152" s="8"/>
     </row>
     <row r="153" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A153" s="1"/>
-      <c r="J153" s="9"/>
-      <c r="K153" s="9"/>
-      <c r="L153" s="9"/>
-      <c r="M153" s="10"/>
-      <c r="N153" s="10"/>
-      <c r="O153" s="10"/>
+      <c r="J153" s="7"/>
+      <c r="K153" s="7"/>
+      <c r="L153" s="7"/>
+      <c r="M153" s="8"/>
+      <c r="N153" s="8"/>
+      <c r="O153" s="8"/>
     </row>
     <row r="154" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A154" s="1"/>
-      <c r="J154" s="9"/>
-      <c r="K154" s="9"/>
-      <c r="L154" s="9"/>
-      <c r="M154" s="10"/>
-      <c r="N154" s="10"/>
-      <c r="O154" s="10"/>
+      <c r="J154" s="7"/>
+      <c r="K154" s="7"/>
+      <c r="L154" s="7"/>
+      <c r="M154" s="8"/>
+      <c r="N154" s="8"/>
+      <c r="O154" s="8"/>
     </row>
     <row r="155" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A155" s="1"/>
-      <c r="J155" s="9"/>
-      <c r="K155" s="9"/>
-      <c r="L155" s="9"/>
-      <c r="M155" s="10"/>
-      <c r="N155" s="10"/>
-      <c r="O155" s="10"/>
+      <c r="J155" s="7"/>
+      <c r="K155" s="7"/>
+      <c r="L155" s="7"/>
+      <c r="M155" s="8"/>
+      <c r="N155" s="8"/>
+      <c r="O155" s="8"/>
     </row>
     <row r="156" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A156" s="1"/>
-      <c r="J156" s="9"/>
-      <c r="K156" s="9"/>
-      <c r="L156" s="9"/>
-      <c r="M156" s="10"/>
-      <c r="N156" s="10"/>
-      <c r="O156" s="10"/>
+      <c r="J156" s="7"/>
+      <c r="K156" s="7"/>
+      <c r="L156" s="7"/>
+      <c r="M156" s="8"/>
+      <c r="N156" s="8"/>
+      <c r="O156" s="8"/>
     </row>
     <row r="157" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A157" s="1"/>
-      <c r="J157" s="9"/>
-      <c r="K157" s="9"/>
-      <c r="L157" s="9"/>
-      <c r="M157" s="10"/>
-      <c r="N157" s="10"/>
-      <c r="O157" s="10"/>
+      <c r="J157" s="7"/>
+      <c r="K157" s="7"/>
+      <c r="L157" s="7"/>
+      <c r="M157" s="8"/>
+      <c r="N157" s="8"/>
+      <c r="O157" s="8"/>
     </row>
     <row r="158" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A158" s="1"/>
-      <c r="J158" s="9"/>
-      <c r="K158" s="9"/>
-      <c r="L158" s="9"/>
-      <c r="M158" s="10"/>
-      <c r="N158" s="10"/>
-      <c r="O158" s="10"/>
+      <c r="J158" s="7"/>
+      <c r="K158" s="7"/>
+      <c r="L158" s="7"/>
+      <c r="M158" s="8"/>
+      <c r="N158" s="8"/>
+      <c r="O158" s="8"/>
     </row>
     <row r="159" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A159" s="1"/>
-      <c r="J159" s="9"/>
-      <c r="K159" s="9"/>
-      <c r="L159" s="9"/>
-      <c r="M159" s="10"/>
-      <c r="N159" s="10"/>
-      <c r="O159" s="10"/>
+      <c r="J159" s="7"/>
+      <c r="K159" s="7"/>
+      <c r="L159" s="7"/>
+      <c r="M159" s="8"/>
+      <c r="N159" s="8"/>
+      <c r="O159" s="8"/>
     </row>
     <row r="160" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A160" s="1"/>
-      <c r="J160" s="9"/>
-      <c r="K160" s="9"/>
-      <c r="L160" s="9"/>
-      <c r="M160" s="10"/>
-      <c r="N160" s="10"/>
-      <c r="O160" s="10"/>
+      <c r="J160" s="7"/>
+      <c r="K160" s="7"/>
+      <c r="L160" s="7"/>
+      <c r="M160" s="8"/>
+      <c r="N160" s="8"/>
+      <c r="O160" s="8"/>
     </row>
     <row r="161" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A161" s="1"/>
-      <c r="J161" s="9"/>
-      <c r="K161" s="9"/>
-      <c r="L161" s="9"/>
-      <c r="M161" s="10"/>
-      <c r="N161" s="10"/>
-      <c r="O161" s="10"/>
+      <c r="J161" s="7"/>
+      <c r="K161" s="7"/>
+      <c r="L161" s="7"/>
+      <c r="M161" s="8"/>
+      <c r="N161" s="8"/>
+      <c r="O161" s="8"/>
     </row>
     <row r="162" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A162" s="1"/>
-      <c r="J162" s="9"/>
-      <c r="K162" s="9"/>
-      <c r="L162" s="9"/>
-      <c r="M162" s="10"/>
-      <c r="N162" s="10"/>
-      <c r="O162" s="10"/>
+      <c r="J162" s="7"/>
+      <c r="K162" s="7"/>
+      <c r="L162" s="7"/>
+      <c r="M162" s="8"/>
+      <c r="N162" s="8"/>
+      <c r="O162" s="8"/>
     </row>
     <row r="163" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A163" s="1"/>
-      <c r="J163" s="9"/>
-      <c r="K163" s="9"/>
-      <c r="L163" s="9"/>
-      <c r="M163" s="10"/>
-      <c r="N163" s="10"/>
-      <c r="O163" s="10"/>
+      <c r="J163" s="7"/>
+      <c r="K163" s="7"/>
+      <c r="L163" s="7"/>
+      <c r="M163" s="8"/>
+      <c r="N163" s="8"/>
+      <c r="O163" s="8"/>
     </row>
     <row r="164" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A164" s="1"/>
-      <c r="J164" s="9"/>
-      <c r="K164" s="9"/>
-      <c r="L164" s="9"/>
-      <c r="M164" s="10"/>
-      <c r="N164" s="10"/>
-      <c r="O164" s="10"/>
+      <c r="J164" s="7"/>
+      <c r="K164" s="7"/>
+      <c r="L164" s="7"/>
+      <c r="M164" s="8"/>
+      <c r="N164" s="8"/>
+      <c r="O164" s="8"/>
     </row>
     <row r="165" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A165" s="1"/>
-      <c r="J165" s="9"/>
-      <c r="K165" s="9"/>
-      <c r="L165" s="9"/>
-      <c r="M165" s="10"/>
-      <c r="N165" s="10"/>
-      <c r="O165" s="10"/>
+      <c r="J165" s="7"/>
+      <c r="K165" s="7"/>
+      <c r="L165" s="7"/>
+      <c r="M165" s="8"/>
+      <c r="N165" s="8"/>
+      <c r="O165" s="8"/>
     </row>
     <row r="166" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A166" s="1"/>
-      <c r="J166" s="9"/>
-      <c r="K166" s="9"/>
-      <c r="L166" s="9"/>
-      <c r="M166" s="10"/>
-      <c r="N166" s="10"/>
-      <c r="O166" s="10"/>
+      <c r="J166" s="7"/>
+      <c r="K166" s="7"/>
+      <c r="L166" s="7"/>
+      <c r="M166" s="8"/>
+      <c r="N166" s="8"/>
+      <c r="O166" s="8"/>
     </row>
     <row r="167" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A167" s="1"/>
-      <c r="J167" s="9"/>
-      <c r="K167" s="9"/>
-      <c r="L167" s="9"/>
-      <c r="M167" s="10"/>
-      <c r="N167" s="10"/>
-      <c r="O167" s="10"/>
+      <c r="J167" s="7"/>
+      <c r="K167" s="7"/>
+      <c r="L167" s="7"/>
+      <c r="M167" s="8"/>
+      <c r="N167" s="8"/>
+      <c r="O167" s="8"/>
     </row>
     <row r="168" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A168" s="1"/>
-      <c r="J168" s="9"/>
-      <c r="K168" s="9"/>
-      <c r="L168" s="9"/>
-      <c r="M168" s="10"/>
-      <c r="N168" s="10"/>
-      <c r="O168" s="10"/>
+      <c r="J168" s="7"/>
+      <c r="K168" s="7"/>
+      <c r="L168" s="7"/>
+      <c r="M168" s="8"/>
+      <c r="N168" s="8"/>
+      <c r="O168" s="8"/>
     </row>
     <row r="169" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A169" s="1"/>
-      <c r="J169" s="9"/>
-      <c r="K169" s="9"/>
-      <c r="L169" s="9"/>
-      <c r="M169" s="10"/>
-      <c r="N169" s="10"/>
-      <c r="O169" s="10"/>
+      <c r="J169" s="7"/>
+      <c r="K169" s="7"/>
+      <c r="L169" s="7"/>
+      <c r="M169" s="8"/>
+      <c r="N169" s="8"/>
+      <c r="O169" s="8"/>
     </row>
     <row r="170" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A170" s="1"/>
-      <c r="J170" s="9"/>
-      <c r="K170" s="9"/>
-      <c r="L170" s="9"/>
-      <c r="M170" s="10"/>
-      <c r="N170" s="10"/>
-      <c r="O170" s="10"/>
+      <c r="J170" s="7"/>
+      <c r="K170" s="7"/>
+      <c r="L170" s="7"/>
+      <c r="M170" s="8"/>
+      <c r="N170" s="8"/>
+      <c r="O170" s="8"/>
     </row>
     <row r="171" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A171" s="1"/>
-      <c r="J171" s="9"/>
-      <c r="K171" s="9"/>
-      <c r="L171" s="9"/>
-      <c r="M171" s="10"/>
-      <c r="N171" s="10"/>
-      <c r="O171" s="10"/>
+      <c r="J171" s="7"/>
+      <c r="K171" s="7"/>
+      <c r="L171" s="7"/>
+      <c r="M171" s="8"/>
+      <c r="N171" s="8"/>
+      <c r="O171" s="8"/>
     </row>
     <row r="172" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A172" s="1"/>
-      <c r="J172" s="9"/>
-      <c r="K172" s="9"/>
-      <c r="L172" s="9"/>
-      <c r="M172" s="10"/>
-      <c r="N172" s="10"/>
-      <c r="O172" s="10"/>
+      <c r="J172" s="7"/>
+      <c r="K172" s="7"/>
+      <c r="L172" s="7"/>
+      <c r="M172" s="8"/>
+      <c r="N172" s="8"/>
+      <c r="O172" s="8"/>
     </row>
     <row r="173" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A173" s="1"/>
-      <c r="J173" s="9"/>
-      <c r="K173" s="9"/>
-      <c r="L173" s="9"/>
-      <c r="M173" s="10"/>
-      <c r="N173" s="10"/>
-      <c r="O173" s="10"/>
+      <c r="J173" s="7"/>
+      <c r="K173" s="7"/>
+      <c r="L173" s="7"/>
+      <c r="M173" s="8"/>
+      <c r="N173" s="8"/>
+      <c r="O173" s="8"/>
     </row>
     <row r="174" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A174" s="1"/>
-      <c r="J174" s="9"/>
-      <c r="K174" s="9"/>
-      <c r="L174" s="9"/>
-      <c r="M174" s="10"/>
-      <c r="N174" s="10"/>
-      <c r="O174" s="10"/>
+      <c r="J174" s="7"/>
+      <c r="K174" s="7"/>
+      <c r="L174" s="7"/>
+      <c r="M174" s="8"/>
+      <c r="N174" s="8"/>
+      <c r="O174" s="8"/>
     </row>
     <row r="175" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A175" s="1"/>
-      <c r="J175" s="9"/>
-      <c r="K175" s="9"/>
-      <c r="L175" s="9"/>
-      <c r="M175" s="10"/>
-      <c r="N175" s="10"/>
-      <c r="O175" s="10"/>
+      <c r="J175" s="7"/>
+      <c r="K175" s="7"/>
+      <c r="L175" s="7"/>
+      <c r="M175" s="8"/>
+      <c r="N175" s="8"/>
+      <c r="O175" s="8"/>
     </row>
     <row r="176" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A176" s="1"/>
-      <c r="J176" s="9"/>
-      <c r="K176" s="9"/>
-      <c r="L176" s="9"/>
-      <c r="M176" s="10"/>
-      <c r="N176" s="10"/>
-      <c r="O176" s="10"/>
+      <c r="J176" s="7"/>
+      <c r="K176" s="7"/>
+      <c r="L176" s="7"/>
+      <c r="M176" s="8"/>
+      <c r="N176" s="8"/>
+      <c r="O176" s="8"/>
     </row>
     <row r="177" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A177" s="1"/>
-      <c r="J177" s="9"/>
-      <c r="K177" s="9"/>
-      <c r="L177" s="9"/>
-      <c r="M177" s="10"/>
-      <c r="N177" s="10"/>
-      <c r="O177" s="10"/>
+      <c r="J177" s="7"/>
+      <c r="K177" s="7"/>
+      <c r="L177" s="7"/>
+      <c r="M177" s="8"/>
+      <c r="N177" s="8"/>
+      <c r="O177" s="8"/>
     </row>
     <row r="178" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A178" s="1"/>
-      <c r="J178" s="9"/>
-      <c r="K178" s="9"/>
-      <c r="L178" s="9"/>
-      <c r="M178" s="10"/>
-      <c r="N178" s="10"/>
-      <c r="O178" s="10"/>
+      <c r="J178" s="7"/>
+      <c r="K178" s="7"/>
+      <c r="L178" s="7"/>
+      <c r="M178" s="8"/>
+      <c r="N178" s="8"/>
+      <c r="O178" s="8"/>
     </row>
     <row r="179" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A179" s="1"/>
-      <c r="J179" s="9"/>
-      <c r="K179" s="9"/>
-      <c r="L179" s="9"/>
-      <c r="M179" s="10"/>
-      <c r="N179" s="10"/>
-      <c r="O179" s="10"/>
+      <c r="J179" s="7"/>
+      <c r="K179" s="7"/>
+      <c r="L179" s="7"/>
+      <c r="M179" s="8"/>
+      <c r="N179" s="8"/>
+      <c r="O179" s="8"/>
     </row>
     <row r="180" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A180" s="1"/>
-      <c r="J180" s="9"/>
-      <c r="K180" s="9"/>
-      <c r="L180" s="9"/>
-      <c r="M180" s="10"/>
-      <c r="N180" s="10"/>
-      <c r="O180" s="10"/>
+      <c r="J180" s="7"/>
+      <c r="K180" s="7"/>
+      <c r="L180" s="7"/>
+      <c r="M180" s="8"/>
+      <c r="N180" s="8"/>
+      <c r="O180" s="8"/>
     </row>
     <row r="181" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A181" s="1"/>
-      <c r="J181" s="9"/>
-      <c r="K181" s="9"/>
-      <c r="L181" s="9"/>
-      <c r="M181" s="10"/>
-      <c r="N181" s="10"/>
-      <c r="O181" s="10"/>
+      <c r="J181" s="7"/>
+      <c r="K181" s="7"/>
+      <c r="L181" s="7"/>
+      <c r="M181" s="8"/>
+      <c r="N181" s="8"/>
+      <c r="O181" s="8"/>
     </row>
     <row r="182" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A182" s="1"/>
-      <c r="J182" s="9"/>
-      <c r="K182" s="9"/>
-      <c r="L182" s="9"/>
-      <c r="M182" s="10"/>
-      <c r="N182" s="10"/>
-      <c r="O182" s="10"/>
+      <c r="J182" s="7"/>
+      <c r="K182" s="7"/>
+      <c r="L182" s="7"/>
+      <c r="M182" s="8"/>
+      <c r="N182" s="8"/>
+      <c r="O182" s="8"/>
     </row>
     <row r="183" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A183" s="1"/>
-      <c r="J183" s="9"/>
-      <c r="K183" s="9"/>
-      <c r="L183" s="9"/>
-      <c r="M183" s="10"/>
-      <c r="N183" s="10"/>
-      <c r="O183" s="10"/>
+      <c r="J183" s="7"/>
+      <c r="K183" s="7"/>
+      <c r="L183" s="7"/>
+      <c r="M183" s="8"/>
+      <c r="N183" s="8"/>
+      <c r="O183" s="8"/>
     </row>
     <row r="184" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A184" s="1"/>
-      <c r="J184" s="9"/>
-      <c r="K184" s="9"/>
-      <c r="L184" s="9"/>
-      <c r="M184" s="10"/>
-      <c r="N184" s="10"/>
-      <c r="O184" s="10"/>
+      <c r="J184" s="7"/>
+      <c r="K184" s="7"/>
+      <c r="L184" s="7"/>
+      <c r="M184" s="8"/>
+      <c r="N184" s="8"/>
+      <c r="O184" s="8"/>
     </row>
     <row r="185" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A185" s="1"/>
-      <c r="J185" s="9"/>
-      <c r="K185" s="9"/>
-      <c r="L185" s="9"/>
-      <c r="M185" s="10"/>
-      <c r="N185" s="10"/>
-      <c r="O185" s="10"/>
+      <c r="J185" s="7"/>
+      <c r="K185" s="7"/>
+      <c r="L185" s="7"/>
+      <c r="M185" s="8"/>
+      <c r="N185" s="8"/>
+      <c r="O185" s="8"/>
     </row>
     <row r="186" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A186" s="1"/>
-      <c r="J186" s="9"/>
-      <c r="K186" s="9"/>
-      <c r="L186" s="9"/>
-      <c r="M186" s="10"/>
-      <c r="N186" s="10"/>
-      <c r="O186" s="10"/>
+      <c r="J186" s="7"/>
+      <c r="K186" s="7"/>
+      <c r="L186" s="7"/>
+      <c r="M186" s="8"/>
+      <c r="N186" s="8"/>
+      <c r="O186" s="8"/>
     </row>
     <row r="187" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A187" s="1"/>
-      <c r="J187" s="9"/>
-      <c r="K187" s="9"/>
-      <c r="L187" s="9"/>
-      <c r="M187" s="10"/>
-      <c r="N187" s="10"/>
-      <c r="O187" s="10"/>
+      <c r="J187" s="7"/>
+      <c r="K187" s="7"/>
+      <c r="L187" s="7"/>
+      <c r="M187" s="8"/>
+      <c r="N187" s="8"/>
+      <c r="O187" s="8"/>
     </row>
     <row r="188" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A188" s="1"/>
-      <c r="J188" s="9"/>
-      <c r="K188" s="9"/>
-      <c r="L188" s="9"/>
-      <c r="M188" s="10"/>
-      <c r="N188" s="10"/>
-      <c r="O188" s="10"/>
+      <c r="J188" s="7"/>
+      <c r="K188" s="7"/>
+      <c r="L188" s="7"/>
+      <c r="M188" s="8"/>
+      <c r="N188" s="8"/>
+      <c r="O188" s="8"/>
     </row>
     <row r="189" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A189" s="1"/>
-      <c r="J189" s="9"/>
-      <c r="K189" s="9"/>
-      <c r="L189" s="9"/>
-      <c r="M189" s="10"/>
-      <c r="N189" s="10"/>
-      <c r="O189" s="10"/>
+      <c r="J189" s="7"/>
+      <c r="K189" s="7"/>
+      <c r="L189" s="7"/>
+      <c r="M189" s="8"/>
+      <c r="N189" s="8"/>
+      <c r="O189" s="8"/>
     </row>
     <row r="190" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A190" s="1"/>
-      <c r="J190" s="9"/>
-      <c r="K190" s="9"/>
-      <c r="L190" s="9"/>
-      <c r="M190" s="10"/>
-      <c r="N190" s="10"/>
-      <c r="O190" s="10"/>
+      <c r="J190" s="7"/>
+      <c r="K190" s="7"/>
+      <c r="L190" s="7"/>
+      <c r="M190" s="8"/>
+      <c r="N190" s="8"/>
+      <c r="O190" s="8"/>
     </row>
     <row r="191" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A191" s="1"/>
-      <c r="J191" s="9"/>
-      <c r="K191" s="9"/>
-      <c r="L191" s="9"/>
-      <c r="M191" s="10"/>
-      <c r="N191" s="10"/>
-      <c r="O191" s="10"/>
+      <c r="J191" s="7"/>
+      <c r="K191" s="7"/>
+      <c r="L191" s="7"/>
+      <c r="M191" s="8"/>
+      <c r="N191" s="8"/>
+      <c r="O191" s="8"/>
     </row>
     <row r="192" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A192" s="1"/>
-      <c r="J192" s="9"/>
-      <c r="K192" s="9"/>
-      <c r="L192" s="9"/>
-      <c r="M192" s="10"/>
-      <c r="N192" s="10"/>
-      <c r="O192" s="10"/>
+      <c r="J192" s="7"/>
+      <c r="K192" s="7"/>
+      <c r="L192" s="7"/>
+      <c r="M192" s="8"/>
+      <c r="N192" s="8"/>
+      <c r="O192" s="8"/>
     </row>
     <row r="193" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A193" s="1"/>
-      <c r="J193" s="9"/>
-      <c r="K193" s="9"/>
-      <c r="L193" s="9"/>
-      <c r="M193" s="10"/>
-      <c r="N193" s="10"/>
-      <c r="O193" s="10"/>
+      <c r="J193" s="7"/>
+      <c r="K193" s="7"/>
+      <c r="L193" s="7"/>
+      <c r="M193" s="8"/>
+      <c r="N193" s="8"/>
+      <c r="O193" s="8"/>
     </row>
     <row r="194" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A194" s="1"/>
-      <c r="J194" s="9"/>
-      <c r="K194" s="9"/>
-      <c r="L194" s="9"/>
-      <c r="M194" s="10"/>
-      <c r="N194" s="10"/>
-      <c r="O194" s="10"/>
+      <c r="J194" s="7"/>
+      <c r="K194" s="7"/>
+      <c r="L194" s="7"/>
+      <c r="M194" s="8"/>
+      <c r="N194" s="8"/>
+      <c r="O194" s="8"/>
     </row>
     <row r="195" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A195" s="1"/>
-      <c r="J195" s="9"/>
-      <c r="K195" s="9"/>
-      <c r="L195" s="9"/>
-      <c r="M195" s="10"/>
-      <c r="N195" s="10"/>
-      <c r="O195" s="10"/>
+      <c r="J195" s="7"/>
+      <c r="K195" s="7"/>
+      <c r="L195" s="7"/>
+      <c r="M195" s="8"/>
+      <c r="N195" s="8"/>
+      <c r="O195" s="8"/>
     </row>
     <row r="196" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A196" s="1"/>
-      <c r="J196" s="9"/>
-      <c r="K196" s="9"/>
-      <c r="L196" s="9"/>
-      <c r="M196" s="10"/>
-      <c r="N196" s="10"/>
-      <c r="O196" s="10"/>
+      <c r="J196" s="7"/>
+      <c r="K196" s="7"/>
+      <c r="L196" s="7"/>
+      <c r="M196" s="8"/>
+      <c r="N196" s="8"/>
+      <c r="O196" s="8"/>
     </row>
     <row r="197" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A197" s="1"/>
-      <c r="J197" s="9"/>
-      <c r="K197" s="9"/>
-      <c r="L197" s="9"/>
-      <c r="M197" s="10"/>
-      <c r="N197" s="10"/>
-      <c r="O197" s="10"/>
+      <c r="J197" s="7"/>
+      <c r="K197" s="7"/>
+      <c r="L197" s="7"/>
+      <c r="M197" s="8"/>
+      <c r="N197" s="8"/>
+      <c r="O197" s="8"/>
     </row>
     <row r="198" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A198" s="1"/>
-      <c r="J198" s="9"/>
-      <c r="K198" s="9"/>
-      <c r="L198" s="9"/>
-      <c r="M198" s="10"/>
-      <c r="N198" s="10"/>
-      <c r="O198" s="10"/>
+      <c r="J198" s="7"/>
+      <c r="K198" s="7"/>
+      <c r="L198" s="7"/>
+      <c r="M198" s="8"/>
+      <c r="N198" s="8"/>
+      <c r="O198" s="8"/>
     </row>
     <row r="199" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A199" s="1"/>
-      <c r="J199" s="9"/>
-      <c r="K199" s="9"/>
-      <c r="L199" s="9"/>
-      <c r="M199" s="10"/>
-      <c r="N199" s="10"/>
-      <c r="O199" s="10"/>
+      <c r="J199" s="7"/>
+      <c r="K199" s="7"/>
+      <c r="L199" s="7"/>
+      <c r="M199" s="8"/>
+      <c r="N199" s="8"/>
+      <c r="O199" s="8"/>
     </row>
     <row r="200" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A200" s="1"/>
-      <c r="J200" s="9"/>
-      <c r="K200" s="9"/>
-      <c r="L200" s="9"/>
-      <c r="M200" s="10"/>
-      <c r="N200" s="10"/>
-      <c r="O200" s="10"/>
+      <c r="J200" s="7"/>
+      <c r="K200" s="7"/>
+      <c r="L200" s="7"/>
+      <c r="M200" s="8"/>
+      <c r="N200" s="8"/>
+      <c r="O200" s="8"/>
     </row>
     <row r="201" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A201" s="1"/>
-      <c r="J201" s="9"/>
-      <c r="K201" s="9"/>
-      <c r="L201" s="9"/>
-      <c r="M201" s="10"/>
-      <c r="N201" s="10"/>
-      <c r="O201" s="10"/>
+      <c r="J201" s="7"/>
+      <c r="K201" s="7"/>
+      <c r="L201" s="7"/>
+      <c r="M201" s="8"/>
+      <c r="N201" s="8"/>
+      <c r="O201" s="8"/>
     </row>
     <row r="202" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A202" s="1"/>
-      <c r="J202" s="9"/>
-      <c r="K202" s="9"/>
-      <c r="L202" s="9"/>
-      <c r="M202" s="10"/>
-      <c r="N202" s="10"/>
-      <c r="O202" s="10"/>
+      <c r="J202" s="7"/>
+      <c r="K202" s="7"/>
+      <c r="L202" s="7"/>
+      <c r="M202" s="8"/>
+      <c r="N202" s="8"/>
+      <c r="O202" s="8"/>
     </row>
     <row r="203" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A203" s="1"/>
-      <c r="J203" s="9"/>
-      <c r="K203" s="9"/>
-      <c r="L203" s="9"/>
-      <c r="M203" s="10"/>
-      <c r="N203" s="10"/>
-      <c r="O203" s="10"/>
+      <c r="J203" s="7"/>
+      <c r="K203" s="7"/>
+      <c r="L203" s="7"/>
+      <c r="M203" s="8"/>
+      <c r="N203" s="8"/>
+      <c r="O203" s="8"/>
     </row>
     <row r="204" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A204" s="1"/>
-      <c r="J204" s="9"/>
-      <c r="K204" s="9"/>
-      <c r="L204" s="9"/>
-      <c r="M204" s="10"/>
-      <c r="N204" s="10"/>
-      <c r="O204" s="10"/>
+      <c r="J204" s="7"/>
+      <c r="K204" s="7"/>
+      <c r="L204" s="7"/>
+      <c r="M204" s="8"/>
+      <c r="N204" s="8"/>
+      <c r="O204" s="8"/>
     </row>
     <row r="205" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A205" s="1"/>
-      <c r="J205" s="9"/>
-      <c r="K205" s="9"/>
-      <c r="L205" s="9"/>
-      <c r="M205" s="10"/>
-      <c r="N205" s="10"/>
-      <c r="O205" s="10"/>
+      <c r="J205" s="7"/>
+      <c r="K205" s="7"/>
+      <c r="L205" s="7"/>
+      <c r="M205" s="8"/>
+      <c r="N205" s="8"/>
+      <c r="O205" s="8"/>
     </row>
     <row r="206" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A206" s="1"/>
-      <c r="J206" s="9"/>
-      <c r="K206" s="9"/>
-      <c r="L206" s="9"/>
-      <c r="M206" s="10"/>
-      <c r="N206" s="10"/>
-      <c r="O206" s="10"/>
+      <c r="J206" s="7"/>
+      <c r="K206" s="7"/>
+      <c r="L206" s="7"/>
+      <c r="M206" s="8"/>
+      <c r="N206" s="8"/>
+      <c r="O206" s="8"/>
     </row>
     <row r="207" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A207" s="1"/>
-      <c r="J207" s="9"/>
-      <c r="K207" s="9"/>
-      <c r="L207" s="9"/>
-      <c r="M207" s="10"/>
-      <c r="N207" s="10"/>
-      <c r="O207" s="10"/>
+      <c r="J207" s="7"/>
+      <c r="K207" s="7"/>
+      <c r="L207" s="7"/>
+      <c r="M207" s="8"/>
+      <c r="N207" s="8"/>
+      <c r="O207" s="8"/>
     </row>
     <row r="208" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A208" s="1"/>
@@ -7382,10 +7396,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
       <formula>"blocker"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"critical"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7442,7 +7456,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="10" t="s">
         <v>17</v>
       </c>
       <c r="C2" t="s">
@@ -7450,15 +7464,15 @@
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="10" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="10" t="s">
         <v>22</v>
       </c>
       <c r="C5" t="s">
@@ -7469,18 +7483,18 @@
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add 'auto filter' in the Excel template for all columns (in our default transformation)
Fixes #3467

git-svn-id: file:///mnt/ramdisk/d4-svn/trunk@12238 484df14f-75d2-4b3f-8ba0-490e05069a01
</commit_message>
<xml_diff>
--- a/businessintelligenceplugin/default-transformation-templates/ticket-list/report-template.xlsx
+++ b/businessintelligenceplugin/default-transformation-templates/ticket-list/report-template.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Analysis" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tickets!$A$7:$Q$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tickets!$A$7:$AD$7</definedName>
     <definedName name="_FilterDatabase_1" localSheetId="0">Tickets!$B$7:$K$7</definedName>
     <definedName name="_FilterDatabase_1_1" localSheetId="0">Tickets!$B$7:$K$7</definedName>
     <definedName name="_FilterDatabase_1_1_1" localSheetId="0">Tickets!#REF!</definedName>
@@ -19,9 +19,9 @@
     <definedName name="Slicer_Priority">#N/A</definedName>
     <definedName name="Slicer_Status">#N/A</definedName>
   </definedNames>
-  <calcPr calcId="145621" iterateDelta="1E-4"/>
+  <calcPr calcId="145621"/>
   <pivotCaches>
-    <pivotCache cacheId="14" r:id="rId3"/>
+    <pivotCache cacheId="9" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
   <si>
     <t>PROJECT:</t>
   </si>
@@ -114,6 +114,45 @@
   <si>
     <t>Days in Status</t>
   </si>
+  <si>
+    <t>assigned</t>
+  </si>
+  <si>
+    <t>accepted</t>
+  </si>
+  <si>
+    <t>review</t>
+  </si>
+  <si>
+    <t>testing</t>
+  </si>
+  <si>
+    <t>integration</t>
+  </si>
+  <si>
+    <t>closed</t>
+  </si>
+  <si>
+    <t>duration_new</t>
+  </si>
+  <si>
+    <t>hours_assigned</t>
+  </si>
+  <si>
+    <t>hours_accepted</t>
+  </si>
+  <si>
+    <t>hours_review</t>
+  </si>
+  <si>
+    <t>hours_testing</t>
+  </si>
+  <si>
+    <t>hours_integration</t>
+  </si>
+  <si>
+    <t>hours_closed</t>
+  </si>
 </sst>
 </file>
 
@@ -123,7 +162,7 @@
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -171,6 +210,13 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -220,8 +266,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2"/>
   </cellStyleXfs>
   <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -241,6 +288,10 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -253,13 +304,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -301,7 +349,6 @@
   </c:pivotSource>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -367,11 +414,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="110800896"/>
-        <c:axId val="110802432"/>
+        <c:axId val="212641664"/>
+        <c:axId val="212643200"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="110800896"/>
+        <c:axId val="212641664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -380,7 +427,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110802432"/>
+        <c:crossAx val="212643200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -388,7 +435,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="110802432"/>
+        <c:axId val="212643200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -399,14 +446,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110800896"/>
+        <c:crossAx val="212641664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -695,7 +741,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="Piper, Nick" refreshedDate="41418.62409085648" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="243">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="Piper, Nick" refreshedDate="41450.44012777778" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="243">
   <cacheSource type="worksheet">
     <worksheetSource ref="A7:P10000" sheet="Tickets"/>
   </cacheSource>
@@ -746,7 +792,7 @@
     <cacheField name="Changed" numFmtId="0">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
-    <cacheField name="Hours in Status" numFmtId="0">
+    <cacheField name="Days in Status" numFmtId="1">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
     <cacheField name="Resolved" numFmtId="0">
@@ -5150,7 +5196,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="B4:D7" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="16">
     <pivotField showAll="0"/>
@@ -5587,7 +5633,7 @@
   <dimension ref="A1:AMM249"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5602,7 +5648,7 @@
     <col min="8" max="8" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="11" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="11.5703125" style="18" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" style="14" customWidth="1"/>
     <col min="13" max="13" width="9.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="14" max="14" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="15" max="15" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
@@ -5611,69 +5657,69 @@
     <col min="18" max="1027" width="8.7109375" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="16"/>
-      <c r="B1" s="16"/>
+    <row r="1" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="20"/>
+      <c r="B1" s="20"/>
       <c r="G1" s="8"/>
-      <c r="L1" s="17"/>
-    </row>
-    <row r="2" spans="1:17" s="2" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
+      <c r="L1" s="13"/>
+    </row>
+    <row r="2" spans="1:30" s="2" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="20"/>
+      <c r="B2" s="20"/>
       <c r="C2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="L2" s="17"/>
-    </row>
-    <row r="3" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="16"/>
-      <c r="B3" s="16"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="L2" s="13"/>
+    </row>
+    <row r="3" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="20"/>
+      <c r="B3" s="20"/>
       <c r="C3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="L3" s="17"/>
-    </row>
-    <row r="4" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="16"/>
-      <c r="B4" s="16"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="L3" s="13"/>
+    </row>
+    <row r="4" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="20"/>
+      <c r="B4" s="20"/>
       <c r="C4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="15"/>
-      <c r="L4" s="17"/>
-    </row>
-    <row r="5" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="16"/>
-      <c r="B5" s="16"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="19"/>
+      <c r="L4" s="13"/>
+    </row>
+    <row r="5" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="20"/>
+      <c r="B5" s="20"/>
       <c r="G5" s="8"/>
-      <c r="L5" s="17"/>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="L5" s="13"/>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="N6" s="6"/>
       <c r="O6" s="6"/>
       <c r="P6" s="6"/>
     </row>
-    <row r="7" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>3</v>
       </c>
@@ -5707,7 +5753,7 @@
       <c r="K7" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="L7" s="19" t="s">
+      <c r="L7" s="15" t="s">
         <v>24</v>
       </c>
       <c r="M7" s="11" t="s">
@@ -5725,92 +5771,131 @@
       <c r="Q7" s="11" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R7" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="S7" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="T7" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="U7" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="V7" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="W7" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="X7" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y7" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z7" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA7" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB7" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC7" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD7" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
-      <c r="L8" s="20"/>
+      <c r="L8" s="16"/>
       <c r="M8" s="4"/>
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
       <c r="P8" s="5"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
-      <c r="L9" s="20"/>
+      <c r="L9" s="16"/>
       <c r="M9" s="4"/>
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
       <c r="P9" s="5"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
-      <c r="L10" s="20"/>
+      <c r="L10" s="16"/>
       <c r="M10" s="4"/>
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
       <c r="P10" s="5"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
-      <c r="L11" s="20"/>
+      <c r="L11" s="16"/>
       <c r="M11" s="4"/>
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
       <c r="P11" s="5"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
-      <c r="L12" s="20"/>
+      <c r="L12" s="16"/>
       <c r="M12" s="4"/>
       <c r="N12" s="5"/>
       <c r="O12" s="5"/>
       <c r="P12" s="5"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
-      <c r="L13" s="20"/>
+      <c r="L13" s="16"/>
       <c r="M13" s="4"/>
       <c r="N13" s="5"/>
       <c r="O13" s="5"/>
       <c r="P13" s="5"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
-      <c r="L14" s="20"/>
+      <c r="L14" s="16"/>
       <c r="M14" s="4"/>
       <c r="N14" s="5"/>
       <c r="O14" s="5"/>
       <c r="P14" s="5"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
-      <c r="L15" s="20"/>
+      <c r="L15" s="16"/>
       <c r="M15" s="4"/>
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
       <c r="P15" s="5"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
-      <c r="L16" s="20"/>
+      <c r="L16" s="16"/>
       <c r="M16" s="4"/>
       <c r="N16" s="5"/>
       <c r="O16" s="5"/>
@@ -5820,7 +5905,7 @@
       <c r="A17" s="1"/>
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
-      <c r="L17" s="20"/>
+      <c r="L17" s="16"/>
       <c r="M17" s="4"/>
       <c r="N17" s="5"/>
       <c r="O17" s="5"/>
@@ -5830,7 +5915,7 @@
       <c r="A18" s="1"/>
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
-      <c r="L18" s="20"/>
+      <c r="L18" s="16"/>
       <c r="M18" s="4"/>
       <c r="N18" s="5"/>
       <c r="O18" s="5"/>
@@ -5840,7 +5925,7 @@
       <c r="A19" s="1"/>
       <c r="J19" s="4"/>
       <c r="K19" s="4"/>
-      <c r="L19" s="20"/>
+      <c r="L19" s="16"/>
       <c r="M19" s="4"/>
       <c r="N19" s="5"/>
       <c r="O19" s="5"/>
@@ -5850,7 +5935,7 @@
       <c r="A20" s="1"/>
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
-      <c r="L20" s="20"/>
+      <c r="L20" s="16"/>
       <c r="M20" s="4"/>
       <c r="N20" s="5"/>
       <c r="O20" s="5"/>
@@ -5860,7 +5945,7 @@
       <c r="A21" s="1"/>
       <c r="J21" s="4"/>
       <c r="K21" s="4"/>
-      <c r="L21" s="20"/>
+      <c r="L21" s="16"/>
       <c r="M21" s="4"/>
       <c r="N21" s="5"/>
       <c r="O21" s="5"/>
@@ -5870,7 +5955,7 @@
       <c r="A22" s="1"/>
       <c r="J22" s="4"/>
       <c r="K22" s="4"/>
-      <c r="L22" s="20"/>
+      <c r="L22" s="16"/>
       <c r="M22" s="4"/>
       <c r="N22" s="5"/>
       <c r="O22" s="5"/>
@@ -5880,7 +5965,7 @@
       <c r="A23" s="1"/>
       <c r="J23" s="4"/>
       <c r="K23" s="4"/>
-      <c r="L23" s="20"/>
+      <c r="L23" s="16"/>
       <c r="M23" s="4"/>
       <c r="N23" s="5"/>
       <c r="O23" s="5"/>
@@ -5890,7 +5975,7 @@
       <c r="A24" s="1"/>
       <c r="J24" s="4"/>
       <c r="K24" s="4"/>
-      <c r="L24" s="20"/>
+      <c r="L24" s="16"/>
       <c r="M24" s="4"/>
       <c r="N24" s="5"/>
       <c r="O24" s="5"/>
@@ -5900,7 +5985,7 @@
       <c r="A25" s="1"/>
       <c r="J25" s="4"/>
       <c r="K25" s="4"/>
-      <c r="L25" s="20"/>
+      <c r="L25" s="16"/>
       <c r="M25" s="4"/>
       <c r="N25" s="5"/>
       <c r="O25" s="5"/>
@@ -5910,7 +5995,7 @@
       <c r="A26" s="1"/>
       <c r="J26" s="4"/>
       <c r="K26" s="4"/>
-      <c r="L26" s="20"/>
+      <c r="L26" s="16"/>
       <c r="M26" s="4"/>
       <c r="N26" s="5"/>
       <c r="O26" s="5"/>
@@ -5920,7 +6005,7 @@
       <c r="A27" s="1"/>
       <c r="J27" s="4"/>
       <c r="K27" s="4"/>
-      <c r="L27" s="20"/>
+      <c r="L27" s="16"/>
       <c r="M27" s="4"/>
       <c r="N27" s="5"/>
       <c r="O27" s="5"/>
@@ -5930,7 +6015,7 @@
       <c r="A28" s="1"/>
       <c r="J28" s="4"/>
       <c r="K28" s="4"/>
-      <c r="L28" s="20"/>
+      <c r="L28" s="16"/>
       <c r="M28" s="4"/>
       <c r="N28" s="5"/>
       <c r="O28" s="5"/>
@@ -5940,7 +6025,7 @@
       <c r="A29" s="1"/>
       <c r="J29" s="4"/>
       <c r="K29" s="4"/>
-      <c r="L29" s="20"/>
+      <c r="L29" s="16"/>
       <c r="M29" s="4"/>
       <c r="N29" s="5"/>
       <c r="O29" s="5"/>
@@ -5950,7 +6035,7 @@
       <c r="A30" s="1"/>
       <c r="J30" s="4"/>
       <c r="K30" s="4"/>
-      <c r="L30" s="20"/>
+      <c r="L30" s="16"/>
       <c r="M30" s="4"/>
       <c r="N30" s="5"/>
       <c r="O30" s="5"/>
@@ -5960,7 +6045,7 @@
       <c r="A31" s="1"/>
       <c r="J31" s="4"/>
       <c r="K31" s="4"/>
-      <c r="L31" s="20"/>
+      <c r="L31" s="16"/>
       <c r="M31" s="4"/>
       <c r="N31" s="5"/>
       <c r="O31" s="5"/>
@@ -5970,7 +6055,7 @@
       <c r="A32" s="1"/>
       <c r="J32" s="4"/>
       <c r="K32" s="4"/>
-      <c r="L32" s="20"/>
+      <c r="L32" s="16"/>
       <c r="M32" s="4"/>
       <c r="N32" s="5"/>
       <c r="O32" s="5"/>
@@ -5980,7 +6065,7 @@
       <c r="A33" s="1"/>
       <c r="J33" s="4"/>
       <c r="K33" s="4"/>
-      <c r="L33" s="20"/>
+      <c r="L33" s="16"/>
       <c r="M33" s="4"/>
       <c r="N33" s="5"/>
       <c r="O33" s="5"/>
@@ -5990,7 +6075,7 @@
       <c r="A34" s="1"/>
       <c r="J34" s="4"/>
       <c r="K34" s="4"/>
-      <c r="L34" s="20"/>
+      <c r="L34" s="16"/>
       <c r="M34" s="4"/>
       <c r="N34" s="5"/>
       <c r="O34" s="5"/>
@@ -6000,7 +6085,7 @@
       <c r="A35" s="1"/>
       <c r="J35" s="4"/>
       <c r="K35" s="4"/>
-      <c r="L35" s="20"/>
+      <c r="L35" s="16"/>
       <c r="M35" s="4"/>
       <c r="N35" s="5"/>
       <c r="O35" s="5"/>
@@ -6010,7 +6095,7 @@
       <c r="A36" s="1"/>
       <c r="J36" s="4"/>
       <c r="K36" s="4"/>
-      <c r="L36" s="20"/>
+      <c r="L36" s="16"/>
       <c r="M36" s="4"/>
       <c r="N36" s="5"/>
       <c r="O36" s="5"/>
@@ -6020,7 +6105,7 @@
       <c r="A37" s="1"/>
       <c r="J37" s="4"/>
       <c r="K37" s="4"/>
-      <c r="L37" s="20"/>
+      <c r="L37" s="16"/>
       <c r="M37" s="4"/>
       <c r="N37" s="5"/>
       <c r="O37" s="5"/>
@@ -6030,7 +6115,7 @@
       <c r="A38" s="1"/>
       <c r="J38" s="4"/>
       <c r="K38" s="4"/>
-      <c r="L38" s="20"/>
+      <c r="L38" s="16"/>
       <c r="M38" s="4"/>
       <c r="N38" s="5"/>
       <c r="O38" s="5"/>
@@ -6040,7 +6125,7 @@
       <c r="A39" s="1"/>
       <c r="J39" s="4"/>
       <c r="K39" s="4"/>
-      <c r="L39" s="20"/>
+      <c r="L39" s="16"/>
       <c r="M39" s="4"/>
       <c r="N39" s="5"/>
       <c r="O39" s="5"/>
@@ -6050,7 +6135,7 @@
       <c r="A40" s="1"/>
       <c r="J40" s="4"/>
       <c r="K40" s="4"/>
-      <c r="L40" s="20"/>
+      <c r="L40" s="16"/>
       <c r="M40" s="4"/>
       <c r="N40" s="5"/>
       <c r="O40" s="5"/>
@@ -6060,7 +6145,7 @@
       <c r="A41" s="1"/>
       <c r="J41" s="4"/>
       <c r="K41" s="4"/>
-      <c r="L41" s="20"/>
+      <c r="L41" s="16"/>
       <c r="M41" s="4"/>
       <c r="N41" s="5"/>
       <c r="O41" s="5"/>
@@ -6070,7 +6155,7 @@
       <c r="A42" s="1"/>
       <c r="J42" s="4"/>
       <c r="K42" s="4"/>
-      <c r="L42" s="20"/>
+      <c r="L42" s="16"/>
       <c r="M42" s="4"/>
       <c r="N42" s="5"/>
       <c r="O42" s="5"/>
@@ -6080,7 +6165,7 @@
       <c r="A43" s="1"/>
       <c r="J43" s="4"/>
       <c r="K43" s="4"/>
-      <c r="L43" s="20"/>
+      <c r="L43" s="16"/>
       <c r="M43" s="4"/>
       <c r="N43" s="5"/>
       <c r="O43" s="5"/>
@@ -6090,7 +6175,7 @@
       <c r="A44" s="1"/>
       <c r="J44" s="4"/>
       <c r="K44" s="4"/>
-      <c r="L44" s="20"/>
+      <c r="L44" s="16"/>
       <c r="M44" s="4"/>
       <c r="N44" s="5"/>
       <c r="O44" s="5"/>
@@ -6100,7 +6185,7 @@
       <c r="A45" s="1"/>
       <c r="J45" s="4"/>
       <c r="K45" s="4"/>
-      <c r="L45" s="20"/>
+      <c r="L45" s="16"/>
       <c r="M45" s="4"/>
       <c r="N45" s="5"/>
       <c r="O45" s="5"/>
@@ -6110,7 +6195,7 @@
       <c r="A46" s="1"/>
       <c r="J46" s="4"/>
       <c r="K46" s="4"/>
-      <c r="L46" s="20"/>
+      <c r="L46" s="16"/>
       <c r="M46" s="4"/>
       <c r="N46" s="5"/>
       <c r="O46" s="5"/>
@@ -6120,7 +6205,7 @@
       <c r="A47" s="1"/>
       <c r="J47" s="4"/>
       <c r="K47" s="4"/>
-      <c r="L47" s="20"/>
+      <c r="L47" s="16"/>
       <c r="M47" s="4"/>
       <c r="N47" s="5"/>
       <c r="O47" s="5"/>
@@ -6130,7 +6215,7 @@
       <c r="A48" s="1"/>
       <c r="J48" s="4"/>
       <c r="K48" s="4"/>
-      <c r="L48" s="20"/>
+      <c r="L48" s="16"/>
       <c r="M48" s="4"/>
       <c r="N48" s="5"/>
       <c r="O48" s="5"/>
@@ -6140,7 +6225,7 @@
       <c r="A49" s="1"/>
       <c r="J49" s="4"/>
       <c r="K49" s="4"/>
-      <c r="L49" s="20"/>
+      <c r="L49" s="16"/>
       <c r="M49" s="4"/>
       <c r="N49" s="5"/>
       <c r="O49" s="5"/>
@@ -6150,7 +6235,7 @@
       <c r="A50" s="1"/>
       <c r="J50" s="4"/>
       <c r="K50" s="4"/>
-      <c r="L50" s="20"/>
+      <c r="L50" s="16"/>
       <c r="M50" s="4"/>
       <c r="N50" s="5"/>
       <c r="O50" s="5"/>
@@ -6160,7 +6245,7 @@
       <c r="A51" s="1"/>
       <c r="J51" s="4"/>
       <c r="K51" s="4"/>
-      <c r="L51" s="20"/>
+      <c r="L51" s="16"/>
       <c r="M51" s="4"/>
       <c r="N51" s="5"/>
       <c r="O51" s="5"/>
@@ -6170,7 +6255,7 @@
       <c r="A52" s="1"/>
       <c r="J52" s="4"/>
       <c r="K52" s="4"/>
-      <c r="L52" s="20"/>
+      <c r="L52" s="16"/>
       <c r="M52" s="4"/>
       <c r="N52" s="5"/>
       <c r="O52" s="5"/>
@@ -6180,7 +6265,7 @@
       <c r="A53" s="1"/>
       <c r="J53" s="4"/>
       <c r="K53" s="4"/>
-      <c r="L53" s="20"/>
+      <c r="L53" s="16"/>
       <c r="M53" s="4"/>
       <c r="N53" s="5"/>
       <c r="O53" s="5"/>
@@ -6190,7 +6275,7 @@
       <c r="A54" s="1"/>
       <c r="J54" s="4"/>
       <c r="K54" s="4"/>
-      <c r="L54" s="20"/>
+      <c r="L54" s="16"/>
       <c r="M54" s="4"/>
       <c r="N54" s="5"/>
       <c r="O54" s="5"/>
@@ -6200,7 +6285,7 @@
       <c r="A55" s="1"/>
       <c r="J55" s="4"/>
       <c r="K55" s="4"/>
-      <c r="L55" s="20"/>
+      <c r="L55" s="16"/>
       <c r="M55" s="4"/>
       <c r="N55" s="5"/>
       <c r="O55" s="5"/>
@@ -6210,7 +6295,7 @@
       <c r="A56" s="1"/>
       <c r="J56" s="4"/>
       <c r="K56" s="4"/>
-      <c r="L56" s="20"/>
+      <c r="L56" s="16"/>
       <c r="M56" s="4"/>
       <c r="N56" s="5"/>
       <c r="O56" s="5"/>
@@ -6220,7 +6305,7 @@
       <c r="A57" s="1"/>
       <c r="J57" s="4"/>
       <c r="K57" s="4"/>
-      <c r="L57" s="20"/>
+      <c r="L57" s="16"/>
       <c r="M57" s="4"/>
       <c r="N57" s="5"/>
       <c r="O57" s="5"/>
@@ -6230,7 +6315,7 @@
       <c r="A58" s="1"/>
       <c r="J58" s="4"/>
       <c r="K58" s="4"/>
-      <c r="L58" s="20"/>
+      <c r="L58" s="16"/>
       <c r="M58" s="4"/>
       <c r="N58" s="5"/>
       <c r="O58" s="5"/>
@@ -6240,7 +6325,7 @@
       <c r="A59" s="1"/>
       <c r="J59" s="4"/>
       <c r="K59" s="4"/>
-      <c r="L59" s="20"/>
+      <c r="L59" s="16"/>
       <c r="M59" s="4"/>
       <c r="N59" s="5"/>
       <c r="O59" s="5"/>
@@ -6250,7 +6335,7 @@
       <c r="A60" s="1"/>
       <c r="J60" s="4"/>
       <c r="K60" s="4"/>
-      <c r="L60" s="20"/>
+      <c r="L60" s="16"/>
       <c r="M60" s="4"/>
       <c r="N60" s="5"/>
       <c r="O60" s="5"/>
@@ -6260,7 +6345,7 @@
       <c r="A61" s="1"/>
       <c r="J61" s="4"/>
       <c r="K61" s="4"/>
-      <c r="L61" s="20"/>
+      <c r="L61" s="16"/>
       <c r="M61" s="4"/>
       <c r="N61" s="5"/>
       <c r="O61" s="5"/>
@@ -6270,7 +6355,7 @@
       <c r="A62" s="1"/>
       <c r="J62" s="4"/>
       <c r="K62" s="4"/>
-      <c r="L62" s="20"/>
+      <c r="L62" s="16"/>
       <c r="M62" s="4"/>
       <c r="N62" s="5"/>
       <c r="O62" s="5"/>
@@ -6280,7 +6365,7 @@
       <c r="A63" s="1"/>
       <c r="J63" s="4"/>
       <c r="K63" s="4"/>
-      <c r="L63" s="20"/>
+      <c r="L63" s="16"/>
       <c r="M63" s="4"/>
       <c r="N63" s="5"/>
       <c r="O63" s="5"/>
@@ -6290,7 +6375,7 @@
       <c r="A64" s="1"/>
       <c r="J64" s="4"/>
       <c r="K64" s="4"/>
-      <c r="L64" s="20"/>
+      <c r="L64" s="16"/>
       <c r="M64" s="4"/>
       <c r="N64" s="5"/>
       <c r="O64" s="5"/>
@@ -6300,7 +6385,7 @@
       <c r="A65" s="1"/>
       <c r="J65" s="4"/>
       <c r="K65" s="4"/>
-      <c r="L65" s="20"/>
+      <c r="L65" s="16"/>
       <c r="M65" s="4"/>
       <c r="N65" s="5"/>
       <c r="O65" s="5"/>
@@ -6310,7 +6395,7 @@
       <c r="A66" s="1"/>
       <c r="J66" s="4"/>
       <c r="K66" s="4"/>
-      <c r="L66" s="20"/>
+      <c r="L66" s="16"/>
       <c r="M66" s="4"/>
       <c r="N66" s="5"/>
       <c r="O66" s="5"/>
@@ -6320,7 +6405,7 @@
       <c r="A67" s="1"/>
       <c r="J67" s="4"/>
       <c r="K67" s="4"/>
-      <c r="L67" s="20"/>
+      <c r="L67" s="16"/>
       <c r="M67" s="4"/>
       <c r="N67" s="5"/>
       <c r="O67" s="5"/>
@@ -6330,7 +6415,7 @@
       <c r="A68" s="1"/>
       <c r="J68" s="4"/>
       <c r="K68" s="4"/>
-      <c r="L68" s="20"/>
+      <c r="L68" s="16"/>
       <c r="M68" s="4"/>
       <c r="N68" s="5"/>
       <c r="O68" s="5"/>
@@ -6340,7 +6425,7 @@
       <c r="A69" s="1"/>
       <c r="J69" s="4"/>
       <c r="K69" s="4"/>
-      <c r="L69" s="20"/>
+      <c r="L69" s="16"/>
       <c r="M69" s="4"/>
       <c r="N69" s="5"/>
       <c r="O69" s="5"/>
@@ -6350,7 +6435,7 @@
       <c r="A70" s="1"/>
       <c r="J70" s="4"/>
       <c r="K70" s="4"/>
-      <c r="L70" s="20"/>
+      <c r="L70" s="16"/>
       <c r="M70" s="4"/>
       <c r="N70" s="5"/>
       <c r="O70" s="5"/>
@@ -6360,7 +6445,7 @@
       <c r="A71" s="1"/>
       <c r="J71" s="4"/>
       <c r="K71" s="4"/>
-      <c r="L71" s="20"/>
+      <c r="L71" s="16"/>
       <c r="M71" s="4"/>
       <c r="N71" s="5"/>
       <c r="O71" s="5"/>
@@ -6370,7 +6455,7 @@
       <c r="A72" s="1"/>
       <c r="J72" s="4"/>
       <c r="K72" s="4"/>
-      <c r="L72" s="20"/>
+      <c r="L72" s="16"/>
       <c r="M72" s="4"/>
       <c r="N72" s="5"/>
       <c r="O72" s="5"/>
@@ -6380,7 +6465,7 @@
       <c r="A73" s="1"/>
       <c r="J73" s="4"/>
       <c r="K73" s="4"/>
-      <c r="L73" s="20"/>
+      <c r="L73" s="16"/>
       <c r="M73" s="4"/>
       <c r="N73" s="5"/>
       <c r="O73" s="5"/>
@@ -6390,7 +6475,7 @@
       <c r="A74" s="1"/>
       <c r="J74" s="4"/>
       <c r="K74" s="4"/>
-      <c r="L74" s="20"/>
+      <c r="L74" s="16"/>
       <c r="M74" s="4"/>
       <c r="N74" s="5"/>
       <c r="O74" s="5"/>
@@ -6400,7 +6485,7 @@
       <c r="A75" s="1"/>
       <c r="J75" s="4"/>
       <c r="K75" s="4"/>
-      <c r="L75" s="20"/>
+      <c r="L75" s="16"/>
       <c r="M75" s="4"/>
       <c r="N75" s="5"/>
       <c r="O75" s="5"/>
@@ -6410,7 +6495,7 @@
       <c r="A76" s="1"/>
       <c r="J76" s="4"/>
       <c r="K76" s="4"/>
-      <c r="L76" s="20"/>
+      <c r="L76" s="16"/>
       <c r="M76" s="4"/>
       <c r="N76" s="5"/>
       <c r="O76" s="5"/>
@@ -6420,7 +6505,7 @@
       <c r="A77" s="1"/>
       <c r="J77" s="4"/>
       <c r="K77" s="4"/>
-      <c r="L77" s="20"/>
+      <c r="L77" s="16"/>
       <c r="M77" s="4"/>
       <c r="N77" s="5"/>
       <c r="O77" s="5"/>
@@ -6430,7 +6515,7 @@
       <c r="A78" s="1"/>
       <c r="J78" s="4"/>
       <c r="K78" s="4"/>
-      <c r="L78" s="20"/>
+      <c r="L78" s="16"/>
       <c r="M78" s="4"/>
       <c r="N78" s="5"/>
       <c r="O78" s="5"/>
@@ -6440,7 +6525,7 @@
       <c r="A79" s="1"/>
       <c r="J79" s="4"/>
       <c r="K79" s="4"/>
-      <c r="L79" s="20"/>
+      <c r="L79" s="16"/>
       <c r="M79" s="4"/>
       <c r="N79" s="5"/>
       <c r="O79" s="5"/>
@@ -6450,7 +6535,7 @@
       <c r="A80" s="1"/>
       <c r="J80" s="4"/>
       <c r="K80" s="4"/>
-      <c r="L80" s="20"/>
+      <c r="L80" s="16"/>
       <c r="M80" s="4"/>
       <c r="N80" s="5"/>
       <c r="O80" s="5"/>
@@ -6460,7 +6545,7 @@
       <c r="A81" s="1"/>
       <c r="J81" s="4"/>
       <c r="K81" s="4"/>
-      <c r="L81" s="20"/>
+      <c r="L81" s="16"/>
       <c r="M81" s="4"/>
       <c r="N81" s="5"/>
       <c r="O81" s="5"/>
@@ -6470,7 +6555,7 @@
       <c r="A82" s="1"/>
       <c r="J82" s="4"/>
       <c r="K82" s="4"/>
-      <c r="L82" s="20"/>
+      <c r="L82" s="16"/>
       <c r="M82" s="4"/>
       <c r="N82" s="5"/>
       <c r="O82" s="5"/>
@@ -6480,7 +6565,7 @@
       <c r="A83" s="1"/>
       <c r="J83" s="4"/>
       <c r="K83" s="4"/>
-      <c r="L83" s="20"/>
+      <c r="L83" s="16"/>
       <c r="M83" s="4"/>
       <c r="N83" s="5"/>
       <c r="O83" s="5"/>
@@ -6490,7 +6575,7 @@
       <c r="A84" s="1"/>
       <c r="J84" s="4"/>
       <c r="K84" s="4"/>
-      <c r="L84" s="20"/>
+      <c r="L84" s="16"/>
       <c r="M84" s="4"/>
       <c r="N84" s="5"/>
       <c r="O84" s="5"/>
@@ -6500,7 +6585,7 @@
       <c r="A85" s="1"/>
       <c r="J85" s="4"/>
       <c r="K85" s="4"/>
-      <c r="L85" s="20"/>
+      <c r="L85" s="16"/>
       <c r="M85" s="4"/>
       <c r="N85" s="5"/>
       <c r="O85" s="5"/>
@@ -6510,7 +6595,7 @@
       <c r="A86" s="1"/>
       <c r="J86" s="4"/>
       <c r="K86" s="4"/>
-      <c r="L86" s="20"/>
+      <c r="L86" s="16"/>
       <c r="M86" s="4"/>
       <c r="N86" s="5"/>
       <c r="O86" s="5"/>
@@ -6520,7 +6605,7 @@
       <c r="A87" s="1"/>
       <c r="J87" s="4"/>
       <c r="K87" s="4"/>
-      <c r="L87" s="20"/>
+      <c r="L87" s="16"/>
       <c r="M87" s="4"/>
       <c r="N87" s="5"/>
       <c r="O87" s="5"/>
@@ -6530,7 +6615,7 @@
       <c r="A88" s="1"/>
       <c r="J88" s="4"/>
       <c r="K88" s="4"/>
-      <c r="L88" s="20"/>
+      <c r="L88" s="16"/>
       <c r="M88" s="4"/>
       <c r="N88" s="5"/>
       <c r="O88" s="5"/>
@@ -6540,7 +6625,7 @@
       <c r="A89" s="1"/>
       <c r="J89" s="4"/>
       <c r="K89" s="4"/>
-      <c r="L89" s="20"/>
+      <c r="L89" s="16"/>
       <c r="M89" s="4"/>
       <c r="N89" s="5"/>
       <c r="O89" s="5"/>
@@ -6550,7 +6635,7 @@
       <c r="A90" s="1"/>
       <c r="J90" s="4"/>
       <c r="K90" s="4"/>
-      <c r="L90" s="20"/>
+      <c r="L90" s="16"/>
       <c r="M90" s="4"/>
       <c r="N90" s="5"/>
       <c r="O90" s="5"/>
@@ -6560,7 +6645,7 @@
       <c r="A91" s="1"/>
       <c r="J91" s="4"/>
       <c r="K91" s="4"/>
-      <c r="L91" s="20"/>
+      <c r="L91" s="16"/>
       <c r="M91" s="4"/>
       <c r="N91" s="5"/>
       <c r="O91" s="5"/>
@@ -6570,7 +6655,7 @@
       <c r="A92" s="1"/>
       <c r="J92" s="4"/>
       <c r="K92" s="4"/>
-      <c r="L92" s="20"/>
+      <c r="L92" s="16"/>
       <c r="M92" s="4"/>
       <c r="N92" s="5"/>
       <c r="O92" s="5"/>
@@ -6580,7 +6665,7 @@
       <c r="A93" s="1"/>
       <c r="J93" s="4"/>
       <c r="K93" s="4"/>
-      <c r="L93" s="20"/>
+      <c r="L93" s="16"/>
       <c r="M93" s="4"/>
       <c r="N93" s="5"/>
       <c r="O93" s="5"/>
@@ -6590,7 +6675,7 @@
       <c r="A94" s="1"/>
       <c r="J94" s="4"/>
       <c r="K94" s="4"/>
-      <c r="L94" s="20"/>
+      <c r="L94" s="16"/>
       <c r="M94" s="4"/>
       <c r="N94" s="5"/>
       <c r="O94" s="5"/>
@@ -6600,7 +6685,7 @@
       <c r="A95" s="1"/>
       <c r="J95" s="4"/>
       <c r="K95" s="4"/>
-      <c r="L95" s="20"/>
+      <c r="L95" s="16"/>
       <c r="M95" s="4"/>
       <c r="N95" s="5"/>
       <c r="O95" s="5"/>
@@ -6610,7 +6695,7 @@
       <c r="A96" s="1"/>
       <c r="J96" s="4"/>
       <c r="K96" s="4"/>
-      <c r="L96" s="20"/>
+      <c r="L96" s="16"/>
       <c r="M96" s="4"/>
       <c r="N96" s="5"/>
       <c r="O96" s="5"/>
@@ -6620,7 +6705,7 @@
       <c r="A97" s="1"/>
       <c r="J97" s="4"/>
       <c r="K97" s="4"/>
-      <c r="L97" s="20"/>
+      <c r="L97" s="16"/>
       <c r="M97" s="4"/>
       <c r="N97" s="5"/>
       <c r="O97" s="5"/>
@@ -6630,7 +6715,7 @@
       <c r="A98" s="1"/>
       <c r="J98" s="4"/>
       <c r="K98" s="4"/>
-      <c r="L98" s="20"/>
+      <c r="L98" s="16"/>
       <c r="M98" s="4"/>
       <c r="N98" s="5"/>
       <c r="O98" s="5"/>
@@ -6640,7 +6725,7 @@
       <c r="A99" s="1"/>
       <c r="J99" s="4"/>
       <c r="K99" s="4"/>
-      <c r="L99" s="20"/>
+      <c r="L99" s="16"/>
       <c r="M99" s="4"/>
       <c r="N99" s="5"/>
       <c r="O99" s="5"/>
@@ -6650,7 +6735,7 @@
       <c r="A100" s="1"/>
       <c r="J100" s="4"/>
       <c r="K100" s="4"/>
-      <c r="L100" s="20"/>
+      <c r="L100" s="16"/>
       <c r="M100" s="4"/>
       <c r="N100" s="5"/>
       <c r="O100" s="5"/>
@@ -6660,7 +6745,7 @@
       <c r="A101" s="1"/>
       <c r="J101" s="4"/>
       <c r="K101" s="4"/>
-      <c r="L101" s="20"/>
+      <c r="L101" s="16"/>
       <c r="M101" s="4"/>
       <c r="N101" s="5"/>
       <c r="O101" s="5"/>
@@ -6670,7 +6755,7 @@
       <c r="A102" s="1"/>
       <c r="J102" s="4"/>
       <c r="K102" s="4"/>
-      <c r="L102" s="20"/>
+      <c r="L102" s="16"/>
       <c r="M102" s="4"/>
       <c r="N102" s="5"/>
       <c r="O102" s="5"/>
@@ -6680,7 +6765,7 @@
       <c r="A103" s="1"/>
       <c r="J103" s="4"/>
       <c r="K103" s="4"/>
-      <c r="L103" s="20"/>
+      <c r="L103" s="16"/>
       <c r="M103" s="4"/>
       <c r="N103" s="5"/>
       <c r="O103" s="5"/>
@@ -6690,7 +6775,7 @@
       <c r="A104" s="1"/>
       <c r="J104" s="4"/>
       <c r="K104" s="4"/>
-      <c r="L104" s="20"/>
+      <c r="L104" s="16"/>
       <c r="M104" s="4"/>
       <c r="N104" s="5"/>
       <c r="O104" s="5"/>
@@ -6700,7 +6785,7 @@
       <c r="A105" s="1"/>
       <c r="J105" s="4"/>
       <c r="K105" s="4"/>
-      <c r="L105" s="20"/>
+      <c r="L105" s="16"/>
       <c r="M105" s="4"/>
       <c r="N105" s="5"/>
       <c r="O105" s="5"/>
@@ -6710,7 +6795,7 @@
       <c r="A106" s="1"/>
       <c r="J106" s="4"/>
       <c r="K106" s="4"/>
-      <c r="L106" s="20"/>
+      <c r="L106" s="16"/>
       <c r="M106" s="4"/>
       <c r="N106" s="5"/>
       <c r="O106" s="5"/>
@@ -6720,7 +6805,7 @@
       <c r="A107" s="1"/>
       <c r="J107" s="4"/>
       <c r="K107" s="4"/>
-      <c r="L107" s="20"/>
+      <c r="L107" s="16"/>
       <c r="M107" s="4"/>
       <c r="N107" s="5"/>
       <c r="O107" s="5"/>
@@ -6730,7 +6815,7 @@
       <c r="A108" s="1"/>
       <c r="J108" s="4"/>
       <c r="K108" s="4"/>
-      <c r="L108" s="20"/>
+      <c r="L108" s="16"/>
       <c r="M108" s="4"/>
       <c r="N108" s="5"/>
       <c r="O108" s="5"/>
@@ -6740,7 +6825,7 @@
       <c r="A109" s="1"/>
       <c r="J109" s="4"/>
       <c r="K109" s="4"/>
-      <c r="L109" s="20"/>
+      <c r="L109" s="16"/>
       <c r="M109" s="4"/>
       <c r="N109" s="5"/>
       <c r="O109" s="5"/>
@@ -6750,7 +6835,7 @@
       <c r="A110" s="1"/>
       <c r="J110" s="4"/>
       <c r="K110" s="4"/>
-      <c r="L110" s="20"/>
+      <c r="L110" s="16"/>
       <c r="M110" s="4"/>
       <c r="N110" s="5"/>
       <c r="O110" s="5"/>
@@ -6760,7 +6845,7 @@
       <c r="A111" s="1"/>
       <c r="J111" s="4"/>
       <c r="K111" s="4"/>
-      <c r="L111" s="20"/>
+      <c r="L111" s="16"/>
       <c r="M111" s="4"/>
       <c r="N111" s="5"/>
       <c r="O111" s="5"/>
@@ -6770,7 +6855,7 @@
       <c r="A112" s="1"/>
       <c r="J112" s="4"/>
       <c r="K112" s="4"/>
-      <c r="L112" s="20"/>
+      <c r="L112" s="16"/>
       <c r="M112" s="4"/>
       <c r="N112" s="5"/>
       <c r="O112" s="5"/>
@@ -6780,7 +6865,7 @@
       <c r="A113" s="1"/>
       <c r="J113" s="4"/>
       <c r="K113" s="4"/>
-      <c r="L113" s="20"/>
+      <c r="L113" s="16"/>
       <c r="M113" s="4"/>
       <c r="N113" s="5"/>
       <c r="O113" s="5"/>
@@ -6790,7 +6875,7 @@
       <c r="A114" s="1"/>
       <c r="J114" s="4"/>
       <c r="K114" s="4"/>
-      <c r="L114" s="20"/>
+      <c r="L114" s="16"/>
       <c r="M114" s="4"/>
       <c r="N114" s="5"/>
       <c r="O114" s="5"/>
@@ -6800,7 +6885,7 @@
       <c r="A115" s="1"/>
       <c r="J115" s="4"/>
       <c r="K115" s="4"/>
-      <c r="L115" s="20"/>
+      <c r="L115" s="16"/>
       <c r="M115" s="4"/>
       <c r="N115" s="5"/>
       <c r="O115" s="5"/>
@@ -6810,7 +6895,7 @@
       <c r="A116" s="1"/>
       <c r="J116" s="4"/>
       <c r="K116" s="4"/>
-      <c r="L116" s="20"/>
+      <c r="L116" s="16"/>
       <c r="M116" s="4"/>
       <c r="N116" s="5"/>
       <c r="O116" s="5"/>
@@ -6820,7 +6905,7 @@
       <c r="A117" s="1"/>
       <c r="J117" s="4"/>
       <c r="K117" s="4"/>
-      <c r="L117" s="20"/>
+      <c r="L117" s="16"/>
       <c r="M117" s="4"/>
       <c r="N117" s="5"/>
       <c r="O117" s="5"/>
@@ -6830,7 +6915,7 @@
       <c r="A118" s="1"/>
       <c r="J118" s="4"/>
       <c r="K118" s="4"/>
-      <c r="L118" s="20"/>
+      <c r="L118" s="16"/>
       <c r="M118" s="4"/>
       <c r="N118" s="5"/>
       <c r="O118" s="5"/>
@@ -6840,7 +6925,7 @@
       <c r="A119" s="1"/>
       <c r="J119" s="4"/>
       <c r="K119" s="4"/>
-      <c r="L119" s="20"/>
+      <c r="L119" s="16"/>
       <c r="M119" s="4"/>
       <c r="N119" s="5"/>
       <c r="O119" s="5"/>
@@ -6850,7 +6935,7 @@
       <c r="A120" s="1"/>
       <c r="J120" s="4"/>
       <c r="K120" s="4"/>
-      <c r="L120" s="20"/>
+      <c r="L120" s="16"/>
       <c r="M120" s="4"/>
       <c r="N120" s="5"/>
       <c r="O120" s="5"/>
@@ -6860,7 +6945,7 @@
       <c r="A121" s="1"/>
       <c r="J121" s="4"/>
       <c r="K121" s="4"/>
-      <c r="L121" s="20"/>
+      <c r="L121" s="16"/>
       <c r="M121" s="4"/>
       <c r="N121" s="5"/>
       <c r="O121" s="5"/>
@@ -6870,7 +6955,7 @@
       <c r="A122" s="1"/>
       <c r="J122" s="4"/>
       <c r="K122" s="4"/>
-      <c r="L122" s="20"/>
+      <c r="L122" s="16"/>
       <c r="M122" s="4"/>
       <c r="N122" s="5"/>
       <c r="O122" s="5"/>
@@ -6880,7 +6965,7 @@
       <c r="A123" s="1"/>
       <c r="J123" s="4"/>
       <c r="K123" s="4"/>
-      <c r="L123" s="20"/>
+      <c r="L123" s="16"/>
       <c r="M123" s="4"/>
       <c r="N123" s="5"/>
       <c r="O123" s="5"/>
@@ -6890,7 +6975,7 @@
       <c r="A124" s="1"/>
       <c r="J124" s="4"/>
       <c r="K124" s="4"/>
-      <c r="L124" s="20"/>
+      <c r="L124" s="16"/>
       <c r="M124" s="4"/>
       <c r="N124" s="5"/>
       <c r="O124" s="5"/>
@@ -6900,7 +6985,7 @@
       <c r="A125" s="1"/>
       <c r="J125" s="4"/>
       <c r="K125" s="4"/>
-      <c r="L125" s="20"/>
+      <c r="L125" s="16"/>
       <c r="M125" s="4"/>
       <c r="N125" s="5"/>
       <c r="O125" s="5"/>
@@ -6910,7 +6995,7 @@
       <c r="A126" s="1"/>
       <c r="J126" s="4"/>
       <c r="K126" s="4"/>
-      <c r="L126" s="20"/>
+      <c r="L126" s="16"/>
       <c r="M126" s="4"/>
       <c r="N126" s="5"/>
       <c r="O126" s="5"/>
@@ -6920,7 +7005,7 @@
       <c r="A127" s="1"/>
       <c r="J127" s="4"/>
       <c r="K127" s="4"/>
-      <c r="L127" s="20"/>
+      <c r="L127" s="16"/>
       <c r="M127" s="4"/>
       <c r="N127" s="5"/>
       <c r="O127" s="5"/>
@@ -6930,7 +7015,7 @@
       <c r="A128" s="1"/>
       <c r="J128" s="4"/>
       <c r="K128" s="4"/>
-      <c r="L128" s="20"/>
+      <c r="L128" s="16"/>
       <c r="M128" s="4"/>
       <c r="N128" s="5"/>
       <c r="O128" s="5"/>
@@ -6940,7 +7025,7 @@
       <c r="A129" s="1"/>
       <c r="J129" s="4"/>
       <c r="K129" s="4"/>
-      <c r="L129" s="20"/>
+      <c r="L129" s="16"/>
       <c r="M129" s="4"/>
       <c r="N129" s="5"/>
       <c r="O129" s="5"/>
@@ -6950,7 +7035,7 @@
       <c r="A130" s="1"/>
       <c r="J130" s="4"/>
       <c r="K130" s="4"/>
-      <c r="L130" s="20"/>
+      <c r="L130" s="16"/>
       <c r="M130" s="4"/>
       <c r="N130" s="5"/>
       <c r="O130" s="5"/>
@@ -6960,7 +7045,7 @@
       <c r="A131" s="1"/>
       <c r="J131" s="4"/>
       <c r="K131" s="4"/>
-      <c r="L131" s="20"/>
+      <c r="L131" s="16"/>
       <c r="M131" s="4"/>
       <c r="N131" s="5"/>
       <c r="O131" s="5"/>
@@ -6970,7 +7055,7 @@
       <c r="A132" s="1"/>
       <c r="J132" s="4"/>
       <c r="K132" s="4"/>
-      <c r="L132" s="20"/>
+      <c r="L132" s="16"/>
       <c r="M132" s="4"/>
       <c r="N132" s="5"/>
       <c r="O132" s="5"/>
@@ -6980,7 +7065,7 @@
       <c r="A133" s="1"/>
       <c r="J133" s="4"/>
       <c r="K133" s="4"/>
-      <c r="L133" s="20"/>
+      <c r="L133" s="16"/>
       <c r="M133" s="4"/>
       <c r="N133" s="5"/>
       <c r="O133" s="5"/>
@@ -6990,7 +7075,7 @@
       <c r="A134" s="1"/>
       <c r="J134" s="4"/>
       <c r="K134" s="4"/>
-      <c r="L134" s="20"/>
+      <c r="L134" s="16"/>
       <c r="M134" s="4"/>
       <c r="N134" s="5"/>
       <c r="O134" s="5"/>
@@ -7000,7 +7085,7 @@
       <c r="A135" s="1"/>
       <c r="J135" s="4"/>
       <c r="K135" s="4"/>
-      <c r="L135" s="20"/>
+      <c r="L135" s="16"/>
       <c r="M135" s="4"/>
       <c r="N135" s="5"/>
       <c r="O135" s="5"/>
@@ -7010,7 +7095,7 @@
       <c r="A136" s="1"/>
       <c r="J136" s="4"/>
       <c r="K136" s="4"/>
-      <c r="L136" s="20"/>
+      <c r="L136" s="16"/>
       <c r="M136" s="4"/>
       <c r="N136" s="5"/>
       <c r="O136" s="5"/>
@@ -7020,7 +7105,7 @@
       <c r="A137" s="1"/>
       <c r="J137" s="4"/>
       <c r="K137" s="4"/>
-      <c r="L137" s="20"/>
+      <c r="L137" s="16"/>
       <c r="M137" s="4"/>
       <c r="N137" s="5"/>
       <c r="O137" s="5"/>
@@ -7030,7 +7115,7 @@
       <c r="A138" s="1"/>
       <c r="J138" s="4"/>
       <c r="K138" s="4"/>
-      <c r="L138" s="20"/>
+      <c r="L138" s="16"/>
       <c r="M138" s="4"/>
       <c r="N138" s="5"/>
       <c r="O138" s="5"/>
@@ -7040,7 +7125,7 @@
       <c r="A139" s="1"/>
       <c r="J139" s="4"/>
       <c r="K139" s="4"/>
-      <c r="L139" s="20"/>
+      <c r="L139" s="16"/>
       <c r="M139" s="4"/>
       <c r="N139" s="5"/>
       <c r="O139" s="5"/>
@@ -7050,7 +7135,7 @@
       <c r="A140" s="1"/>
       <c r="J140" s="4"/>
       <c r="K140" s="4"/>
-      <c r="L140" s="20"/>
+      <c r="L140" s="16"/>
       <c r="M140" s="4"/>
       <c r="N140" s="5"/>
       <c r="O140" s="5"/>
@@ -7060,7 +7145,7 @@
       <c r="A141" s="1"/>
       <c r="J141" s="4"/>
       <c r="K141" s="4"/>
-      <c r="L141" s="20"/>
+      <c r="L141" s="16"/>
       <c r="M141" s="4"/>
       <c r="N141" s="5"/>
       <c r="O141" s="5"/>
@@ -7070,7 +7155,7 @@
       <c r="A142" s="1"/>
       <c r="J142" s="4"/>
       <c r="K142" s="4"/>
-      <c r="L142" s="20"/>
+      <c r="L142" s="16"/>
       <c r="M142" s="4"/>
       <c r="N142" s="5"/>
       <c r="O142" s="5"/>
@@ -7080,7 +7165,7 @@
       <c r="A143" s="1"/>
       <c r="J143" s="4"/>
       <c r="K143" s="4"/>
-      <c r="L143" s="20"/>
+      <c r="L143" s="16"/>
       <c r="M143" s="4"/>
       <c r="N143" s="5"/>
       <c r="O143" s="5"/>
@@ -7090,7 +7175,7 @@
       <c r="A144" s="1"/>
       <c r="J144" s="4"/>
       <c r="K144" s="4"/>
-      <c r="L144" s="20"/>
+      <c r="L144" s="16"/>
       <c r="M144" s="4"/>
       <c r="N144" s="5"/>
       <c r="O144" s="5"/>
@@ -7100,7 +7185,7 @@
       <c r="A145" s="1"/>
       <c r="J145" s="4"/>
       <c r="K145" s="4"/>
-      <c r="L145" s="20"/>
+      <c r="L145" s="16"/>
       <c r="M145" s="4"/>
       <c r="N145" s="5"/>
       <c r="O145" s="5"/>
@@ -7110,7 +7195,7 @@
       <c r="A146" s="1"/>
       <c r="J146" s="4"/>
       <c r="K146" s="4"/>
-      <c r="L146" s="20"/>
+      <c r="L146" s="16"/>
       <c r="M146" s="4"/>
       <c r="N146" s="5"/>
       <c r="O146" s="5"/>
@@ -7120,7 +7205,7 @@
       <c r="A147" s="1"/>
       <c r="J147" s="4"/>
       <c r="K147" s="4"/>
-      <c r="L147" s="20"/>
+      <c r="L147" s="16"/>
       <c r="M147" s="4"/>
       <c r="N147" s="5"/>
       <c r="O147" s="5"/>
@@ -7130,7 +7215,7 @@
       <c r="A148" s="1"/>
       <c r="J148" s="4"/>
       <c r="K148" s="4"/>
-      <c r="L148" s="20"/>
+      <c r="L148" s="16"/>
       <c r="M148" s="4"/>
       <c r="N148" s="5"/>
       <c r="O148" s="5"/>
@@ -7140,7 +7225,7 @@
       <c r="A149" s="1"/>
       <c r="J149" s="4"/>
       <c r="K149" s="4"/>
-      <c r="L149" s="20"/>
+      <c r="L149" s="16"/>
       <c r="M149" s="4"/>
       <c r="N149" s="5"/>
       <c r="O149" s="5"/>
@@ -7150,7 +7235,7 @@
       <c r="A150" s="1"/>
       <c r="J150" s="4"/>
       <c r="K150" s="4"/>
-      <c r="L150" s="20"/>
+      <c r="L150" s="16"/>
       <c r="M150" s="4"/>
       <c r="N150" s="5"/>
       <c r="O150" s="5"/>
@@ -7160,7 +7245,7 @@
       <c r="A151" s="1"/>
       <c r="J151" s="4"/>
       <c r="K151" s="4"/>
-      <c r="L151" s="20"/>
+      <c r="L151" s="16"/>
       <c r="M151" s="4"/>
       <c r="N151" s="5"/>
       <c r="O151" s="5"/>
@@ -7170,7 +7255,7 @@
       <c r="A152" s="1"/>
       <c r="J152" s="4"/>
       <c r="K152" s="4"/>
-      <c r="L152" s="20"/>
+      <c r="L152" s="16"/>
       <c r="M152" s="4"/>
       <c r="N152" s="5"/>
       <c r="O152" s="5"/>
@@ -7180,7 +7265,7 @@
       <c r="A153" s="1"/>
       <c r="J153" s="4"/>
       <c r="K153" s="4"/>
-      <c r="L153" s="20"/>
+      <c r="L153" s="16"/>
       <c r="M153" s="4"/>
       <c r="N153" s="5"/>
       <c r="O153" s="5"/>
@@ -7190,7 +7275,7 @@
       <c r="A154" s="1"/>
       <c r="J154" s="4"/>
       <c r="K154" s="4"/>
-      <c r="L154" s="20"/>
+      <c r="L154" s="16"/>
       <c r="M154" s="4"/>
       <c r="N154" s="5"/>
       <c r="O154" s="5"/>
@@ -7200,7 +7285,7 @@
       <c r="A155" s="1"/>
       <c r="J155" s="4"/>
       <c r="K155" s="4"/>
-      <c r="L155" s="20"/>
+      <c r="L155" s="16"/>
       <c r="M155" s="4"/>
       <c r="N155" s="5"/>
       <c r="O155" s="5"/>
@@ -7210,7 +7295,7 @@
       <c r="A156" s="1"/>
       <c r="J156" s="4"/>
       <c r="K156" s="4"/>
-      <c r="L156" s="20"/>
+      <c r="L156" s="16"/>
       <c r="M156" s="4"/>
       <c r="N156" s="5"/>
       <c r="O156" s="5"/>
@@ -7220,7 +7305,7 @@
       <c r="A157" s="1"/>
       <c r="J157" s="4"/>
       <c r="K157" s="4"/>
-      <c r="L157" s="20"/>
+      <c r="L157" s="16"/>
       <c r="M157" s="4"/>
       <c r="N157" s="5"/>
       <c r="O157" s="5"/>
@@ -7230,7 +7315,7 @@
       <c r="A158" s="1"/>
       <c r="J158" s="4"/>
       <c r="K158" s="4"/>
-      <c r="L158" s="20"/>
+      <c r="L158" s="16"/>
       <c r="M158" s="4"/>
       <c r="N158" s="5"/>
       <c r="O158" s="5"/>
@@ -7240,7 +7325,7 @@
       <c r="A159" s="1"/>
       <c r="J159" s="4"/>
       <c r="K159" s="4"/>
-      <c r="L159" s="20"/>
+      <c r="L159" s="16"/>
       <c r="M159" s="4"/>
       <c r="N159" s="5"/>
       <c r="O159" s="5"/>
@@ -7250,7 +7335,7 @@
       <c r="A160" s="1"/>
       <c r="J160" s="4"/>
       <c r="K160" s="4"/>
-      <c r="L160" s="20"/>
+      <c r="L160" s="16"/>
       <c r="M160" s="4"/>
       <c r="N160" s="5"/>
       <c r="O160" s="5"/>
@@ -7260,7 +7345,7 @@
       <c r="A161" s="1"/>
       <c r="J161" s="4"/>
       <c r="K161" s="4"/>
-      <c r="L161" s="20"/>
+      <c r="L161" s="16"/>
       <c r="M161" s="4"/>
       <c r="N161" s="5"/>
       <c r="O161" s="5"/>
@@ -7270,7 +7355,7 @@
       <c r="A162" s="1"/>
       <c r="J162" s="4"/>
       <c r="K162" s="4"/>
-      <c r="L162" s="20"/>
+      <c r="L162" s="16"/>
       <c r="M162" s="4"/>
       <c r="N162" s="5"/>
       <c r="O162" s="5"/>
@@ -7280,7 +7365,7 @@
       <c r="A163" s="1"/>
       <c r="J163" s="4"/>
       <c r="K163" s="4"/>
-      <c r="L163" s="20"/>
+      <c r="L163" s="16"/>
       <c r="M163" s="4"/>
       <c r="N163" s="5"/>
       <c r="O163" s="5"/>
@@ -7290,7 +7375,7 @@
       <c r="A164" s="1"/>
       <c r="J164" s="4"/>
       <c r="K164" s="4"/>
-      <c r="L164" s="20"/>
+      <c r="L164" s="16"/>
       <c r="M164" s="4"/>
       <c r="N164" s="5"/>
       <c r="O164" s="5"/>
@@ -7300,7 +7385,7 @@
       <c r="A165" s="1"/>
       <c r="J165" s="4"/>
       <c r="K165" s="4"/>
-      <c r="L165" s="20"/>
+      <c r="L165" s="16"/>
       <c r="M165" s="4"/>
       <c r="N165" s="5"/>
       <c r="O165" s="5"/>
@@ -7310,7 +7395,7 @@
       <c r="A166" s="1"/>
       <c r="J166" s="4"/>
       <c r="K166" s="4"/>
-      <c r="L166" s="20"/>
+      <c r="L166" s="16"/>
       <c r="M166" s="4"/>
       <c r="N166" s="5"/>
       <c r="O166" s="5"/>
@@ -7320,7 +7405,7 @@
       <c r="A167" s="1"/>
       <c r="J167" s="4"/>
       <c r="K167" s="4"/>
-      <c r="L167" s="20"/>
+      <c r="L167" s="16"/>
       <c r="M167" s="4"/>
       <c r="N167" s="5"/>
       <c r="O167" s="5"/>
@@ -7330,7 +7415,7 @@
       <c r="A168" s="1"/>
       <c r="J168" s="4"/>
       <c r="K168" s="4"/>
-      <c r="L168" s="20"/>
+      <c r="L168" s="16"/>
       <c r="M168" s="4"/>
       <c r="N168" s="5"/>
       <c r="O168" s="5"/>
@@ -7340,7 +7425,7 @@
       <c r="A169" s="1"/>
       <c r="J169" s="4"/>
       <c r="K169" s="4"/>
-      <c r="L169" s="20"/>
+      <c r="L169" s="16"/>
       <c r="M169" s="4"/>
       <c r="N169" s="5"/>
       <c r="O169" s="5"/>
@@ -7350,7 +7435,7 @@
       <c r="A170" s="1"/>
       <c r="J170" s="4"/>
       <c r="K170" s="4"/>
-      <c r="L170" s="20"/>
+      <c r="L170" s="16"/>
       <c r="M170" s="4"/>
       <c r="N170" s="5"/>
       <c r="O170" s="5"/>
@@ -7360,7 +7445,7 @@
       <c r="A171" s="1"/>
       <c r="J171" s="4"/>
       <c r="K171" s="4"/>
-      <c r="L171" s="20"/>
+      <c r="L171" s="16"/>
       <c r="M171" s="4"/>
       <c r="N171" s="5"/>
       <c r="O171" s="5"/>
@@ -7370,7 +7455,7 @@
       <c r="A172" s="1"/>
       <c r="J172" s="4"/>
       <c r="K172" s="4"/>
-      <c r="L172" s="20"/>
+      <c r="L172" s="16"/>
       <c r="M172" s="4"/>
       <c r="N172" s="5"/>
       <c r="O172" s="5"/>
@@ -7380,7 +7465,7 @@
       <c r="A173" s="1"/>
       <c r="J173" s="4"/>
       <c r="K173" s="4"/>
-      <c r="L173" s="20"/>
+      <c r="L173" s="16"/>
       <c r="M173" s="4"/>
       <c r="N173" s="5"/>
       <c r="O173" s="5"/>
@@ -7390,7 +7475,7 @@
       <c r="A174" s="1"/>
       <c r="J174" s="4"/>
       <c r="K174" s="4"/>
-      <c r="L174" s="20"/>
+      <c r="L174" s="16"/>
       <c r="M174" s="4"/>
       <c r="N174" s="5"/>
       <c r="O174" s="5"/>
@@ -7400,7 +7485,7 @@
       <c r="A175" s="1"/>
       <c r="J175" s="4"/>
       <c r="K175" s="4"/>
-      <c r="L175" s="20"/>
+      <c r="L175" s="16"/>
       <c r="M175" s="4"/>
       <c r="N175" s="5"/>
       <c r="O175" s="5"/>
@@ -7410,7 +7495,7 @@
       <c r="A176" s="1"/>
       <c r="J176" s="4"/>
       <c r="K176" s="4"/>
-      <c r="L176" s="20"/>
+      <c r="L176" s="16"/>
       <c r="M176" s="4"/>
       <c r="N176" s="5"/>
       <c r="O176" s="5"/>
@@ -7420,7 +7505,7 @@
       <c r="A177" s="1"/>
       <c r="J177" s="4"/>
       <c r="K177" s="4"/>
-      <c r="L177" s="20"/>
+      <c r="L177" s="16"/>
       <c r="M177" s="4"/>
       <c r="N177" s="5"/>
       <c r="O177" s="5"/>
@@ -7430,7 +7515,7 @@
       <c r="A178" s="1"/>
       <c r="J178" s="4"/>
       <c r="K178" s="4"/>
-      <c r="L178" s="20"/>
+      <c r="L178" s="16"/>
       <c r="M178" s="4"/>
       <c r="N178" s="5"/>
       <c r="O178" s="5"/>
@@ -7440,7 +7525,7 @@
       <c r="A179" s="1"/>
       <c r="J179" s="4"/>
       <c r="K179" s="4"/>
-      <c r="L179" s="20"/>
+      <c r="L179" s="16"/>
       <c r="M179" s="4"/>
       <c r="N179" s="5"/>
       <c r="O179" s="5"/>
@@ -7450,7 +7535,7 @@
       <c r="A180" s="1"/>
       <c r="J180" s="4"/>
       <c r="K180" s="4"/>
-      <c r="L180" s="20"/>
+      <c r="L180" s="16"/>
       <c r="M180" s="4"/>
       <c r="N180" s="5"/>
       <c r="O180" s="5"/>
@@ -7460,7 +7545,7 @@
       <c r="A181" s="1"/>
       <c r="J181" s="4"/>
       <c r="K181" s="4"/>
-      <c r="L181" s="20"/>
+      <c r="L181" s="16"/>
       <c r="M181" s="4"/>
       <c r="N181" s="5"/>
       <c r="O181" s="5"/>
@@ -7470,7 +7555,7 @@
       <c r="A182" s="1"/>
       <c r="J182" s="4"/>
       <c r="K182" s="4"/>
-      <c r="L182" s="20"/>
+      <c r="L182" s="16"/>
       <c r="M182" s="4"/>
       <c r="N182" s="5"/>
       <c r="O182" s="5"/>
@@ -7480,7 +7565,7 @@
       <c r="A183" s="1"/>
       <c r="J183" s="4"/>
       <c r="K183" s="4"/>
-      <c r="L183" s="20"/>
+      <c r="L183" s="16"/>
       <c r="M183" s="4"/>
       <c r="N183" s="5"/>
       <c r="O183" s="5"/>
@@ -7490,7 +7575,7 @@
       <c r="A184" s="1"/>
       <c r="J184" s="4"/>
       <c r="K184" s="4"/>
-      <c r="L184" s="20"/>
+      <c r="L184" s="16"/>
       <c r="M184" s="4"/>
       <c r="N184" s="5"/>
       <c r="O184" s="5"/>
@@ -7500,7 +7585,7 @@
       <c r="A185" s="1"/>
       <c r="J185" s="4"/>
       <c r="K185" s="4"/>
-      <c r="L185" s="20"/>
+      <c r="L185" s="16"/>
       <c r="M185" s="4"/>
       <c r="N185" s="5"/>
       <c r="O185" s="5"/>
@@ -7510,7 +7595,7 @@
       <c r="A186" s="1"/>
       <c r="J186" s="4"/>
       <c r="K186" s="4"/>
-      <c r="L186" s="20"/>
+      <c r="L186" s="16"/>
       <c r="M186" s="4"/>
       <c r="N186" s="5"/>
       <c r="O186" s="5"/>
@@ -7520,7 +7605,7 @@
       <c r="A187" s="1"/>
       <c r="J187" s="4"/>
       <c r="K187" s="4"/>
-      <c r="L187" s="20"/>
+      <c r="L187" s="16"/>
       <c r="M187" s="4"/>
       <c r="N187" s="5"/>
       <c r="O187" s="5"/>
@@ -7530,7 +7615,7 @@
       <c r="A188" s="1"/>
       <c r="J188" s="4"/>
       <c r="K188" s="4"/>
-      <c r="L188" s="20"/>
+      <c r="L188" s="16"/>
       <c r="M188" s="4"/>
       <c r="N188" s="5"/>
       <c r="O188" s="5"/>
@@ -7540,7 +7625,7 @@
       <c r="A189" s="1"/>
       <c r="J189" s="4"/>
       <c r="K189" s="4"/>
-      <c r="L189" s="20"/>
+      <c r="L189" s="16"/>
       <c r="M189" s="4"/>
       <c r="N189" s="5"/>
       <c r="O189" s="5"/>
@@ -7550,7 +7635,7 @@
       <c r="A190" s="1"/>
       <c r="J190" s="4"/>
       <c r="K190" s="4"/>
-      <c r="L190" s="20"/>
+      <c r="L190" s="16"/>
       <c r="M190" s="4"/>
       <c r="N190" s="5"/>
       <c r="O190" s="5"/>
@@ -7560,7 +7645,7 @@
       <c r="A191" s="1"/>
       <c r="J191" s="4"/>
       <c r="K191" s="4"/>
-      <c r="L191" s="20"/>
+      <c r="L191" s="16"/>
       <c r="M191" s="4"/>
       <c r="N191" s="5"/>
       <c r="O191" s="5"/>
@@ -7570,7 +7655,7 @@
       <c r="A192" s="1"/>
       <c r="J192" s="4"/>
       <c r="K192" s="4"/>
-      <c r="L192" s="20"/>
+      <c r="L192" s="16"/>
       <c r="M192" s="4"/>
       <c r="N192" s="5"/>
       <c r="O192" s="5"/>
@@ -7580,7 +7665,7 @@
       <c r="A193" s="1"/>
       <c r="J193" s="4"/>
       <c r="K193" s="4"/>
-      <c r="L193" s="20"/>
+      <c r="L193" s="16"/>
       <c r="M193" s="4"/>
       <c r="N193" s="5"/>
       <c r="O193" s="5"/>
@@ -7590,7 +7675,7 @@
       <c r="A194" s="1"/>
       <c r="J194" s="4"/>
       <c r="K194" s="4"/>
-      <c r="L194" s="20"/>
+      <c r="L194" s="16"/>
       <c r="M194" s="4"/>
       <c r="N194" s="5"/>
       <c r="O194" s="5"/>
@@ -7600,7 +7685,7 @@
       <c r="A195" s="1"/>
       <c r="J195" s="4"/>
       <c r="K195" s="4"/>
-      <c r="L195" s="20"/>
+      <c r="L195" s="16"/>
       <c r="M195" s="4"/>
       <c r="N195" s="5"/>
       <c r="O195" s="5"/>
@@ -7610,7 +7695,7 @@
       <c r="A196" s="1"/>
       <c r="J196" s="4"/>
       <c r="K196" s="4"/>
-      <c r="L196" s="20"/>
+      <c r="L196" s="16"/>
       <c r="M196" s="4"/>
       <c r="N196" s="5"/>
       <c r="O196" s="5"/>
@@ -7620,7 +7705,7 @@
       <c r="A197" s="1"/>
       <c r="J197" s="4"/>
       <c r="K197" s="4"/>
-      <c r="L197" s="20"/>
+      <c r="L197" s="16"/>
       <c r="M197" s="4"/>
       <c r="N197" s="5"/>
       <c r="O197" s="5"/>
@@ -7630,7 +7715,7 @@
       <c r="A198" s="1"/>
       <c r="J198" s="4"/>
       <c r="K198" s="4"/>
-      <c r="L198" s="20"/>
+      <c r="L198" s="16"/>
       <c r="M198" s="4"/>
       <c r="N198" s="5"/>
       <c r="O198" s="5"/>
@@ -7640,7 +7725,7 @@
       <c r="A199" s="1"/>
       <c r="J199" s="4"/>
       <c r="K199" s="4"/>
-      <c r="L199" s="20"/>
+      <c r="L199" s="16"/>
       <c r="M199" s="4"/>
       <c r="N199" s="5"/>
       <c r="O199" s="5"/>
@@ -7650,7 +7735,7 @@
       <c r="A200" s="1"/>
       <c r="J200" s="4"/>
       <c r="K200" s="4"/>
-      <c r="L200" s="20"/>
+      <c r="L200" s="16"/>
       <c r="M200" s="4"/>
       <c r="N200" s="5"/>
       <c r="O200" s="5"/>
@@ -7660,7 +7745,7 @@
       <c r="A201" s="1"/>
       <c r="J201" s="4"/>
       <c r="K201" s="4"/>
-      <c r="L201" s="20"/>
+      <c r="L201" s="16"/>
       <c r="M201" s="4"/>
       <c r="N201" s="5"/>
       <c r="O201" s="5"/>
@@ -7670,7 +7755,7 @@
       <c r="A202" s="1"/>
       <c r="J202" s="4"/>
       <c r="K202" s="4"/>
-      <c r="L202" s="20"/>
+      <c r="L202" s="16"/>
       <c r="M202" s="4"/>
       <c r="N202" s="5"/>
       <c r="O202" s="5"/>
@@ -7680,7 +7765,7 @@
       <c r="A203" s="1"/>
       <c r="J203" s="4"/>
       <c r="K203" s="4"/>
-      <c r="L203" s="20"/>
+      <c r="L203" s="16"/>
       <c r="M203" s="4"/>
       <c r="N203" s="5"/>
       <c r="O203" s="5"/>
@@ -7690,7 +7775,7 @@
       <c r="A204" s="1"/>
       <c r="J204" s="4"/>
       <c r="K204" s="4"/>
-      <c r="L204" s="20"/>
+      <c r="L204" s="16"/>
       <c r="M204" s="4"/>
       <c r="N204" s="5"/>
       <c r="O204" s="5"/>
@@ -7700,7 +7785,7 @@
       <c r="A205" s="1"/>
       <c r="J205" s="4"/>
       <c r="K205" s="4"/>
-      <c r="L205" s="20"/>
+      <c r="L205" s="16"/>
       <c r="M205" s="4"/>
       <c r="N205" s="5"/>
       <c r="O205" s="5"/>
@@ -7710,7 +7795,7 @@
       <c r="A206" s="1"/>
       <c r="J206" s="4"/>
       <c r="K206" s="4"/>
-      <c r="L206" s="20"/>
+      <c r="L206" s="16"/>
       <c r="M206" s="4"/>
       <c r="N206" s="5"/>
       <c r="O206" s="5"/>
@@ -7720,7 +7805,7 @@
       <c r="A207" s="1"/>
       <c r="J207" s="4"/>
       <c r="K207" s="4"/>
-      <c r="L207" s="20"/>
+      <c r="L207" s="16"/>
       <c r="M207" s="4"/>
       <c r="N207" s="5"/>
       <c r="O207" s="5"/>
@@ -7853,7 +7938,7 @@
       <c r="A249" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A7:Q7"/>
+  <autoFilter ref="A7:AD7"/>
   <mergeCells count="4">
     <mergeCell ref="D2:J2"/>
     <mergeCell ref="D3:J3"/>
@@ -7861,7 +7946,7 @@
     <mergeCell ref="A1:B5"/>
   </mergeCells>
   <conditionalFormatting sqref="Q1:Q1048576">
-    <cfRule type="dataBar" priority="4">
+    <cfRule type="dataBar" priority="6">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -7873,7 +7958,7 @@
         </ext>
       </extLst>
     </cfRule>
-    <cfRule type="colorScale" priority="6">
+    <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -7883,15 +7968,15 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1 F5:F1048576">
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
       <formula>"critical"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="7" operator="equal">
       <formula>"blocker"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O1:O1048576">
-    <cfRule type="iconSet" priority="2">
+    <cfRule type="iconSet" priority="4">
       <iconSet iconSet="5Quarters">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="20"/>
@@ -7902,7 +7987,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:L1048576">
-    <cfRule type="dataBar" priority="1">
+    <cfRule type="dataBar" priority="3">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -7913,6 +7998,28 @@
           <x14:id>{FA669B14-1E46-499F-B0A6-FE74CCAC2FBC}</x14:id>
         </ext>
       </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R7:AD7">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF555A"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{674EB489-9018-4162-B020-DDEB2FFA5E4F}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -7947,6 +8054,19 @@
           </x14:cfRule>
           <xm:sqref>L1:L1048576</xm:sqref>
         </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{674EB489-9018-4162-B020-DDEB2FFA5E4F}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FFFF555A"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>R7:AD7</xm:sqref>
+        </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
   </extLst>

</xml_diff>

<commit_message>
Merge [12238] to 4.9.x for #3467
git-svn-id: file:///mnt/ramdisk/d4-svn/branches/releases/4.10.x@12328 484df14f-75d2-4b3f-8ba0-490e05069a01
</commit_message>
<xml_diff>
--- a/businessintelligenceplugin/default-transformation-templates/ticket-list/report-template.xlsx
+++ b/businessintelligenceplugin/default-transformation-templates/ticket-list/report-template.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Analysis" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tickets!$A$7:$Q$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tickets!$A$7:$AD$7</definedName>
     <definedName name="_FilterDatabase_1" localSheetId="0">Tickets!$B$7:$K$7</definedName>
     <definedName name="_FilterDatabase_1_1" localSheetId="0">Tickets!$B$7:$K$7</definedName>
     <definedName name="_FilterDatabase_1_1_1" localSheetId="0">Tickets!#REF!</definedName>
@@ -19,9 +19,9 @@
     <definedName name="Slicer_Priority">#N/A</definedName>
     <definedName name="Slicer_Status">#N/A</definedName>
   </definedNames>
-  <calcPr calcId="145621" iterateDelta="1E-4"/>
+  <calcPr calcId="145621"/>
   <pivotCaches>
-    <pivotCache cacheId="14" r:id="rId3"/>
+    <pivotCache cacheId="9" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
   <si>
     <t>PROJECT:</t>
   </si>
@@ -114,6 +114,45 @@
   <si>
     <t>Days in Status</t>
   </si>
+  <si>
+    <t>assigned</t>
+  </si>
+  <si>
+    <t>accepted</t>
+  </si>
+  <si>
+    <t>review</t>
+  </si>
+  <si>
+    <t>testing</t>
+  </si>
+  <si>
+    <t>integration</t>
+  </si>
+  <si>
+    <t>closed</t>
+  </si>
+  <si>
+    <t>duration_new</t>
+  </si>
+  <si>
+    <t>hours_assigned</t>
+  </si>
+  <si>
+    <t>hours_accepted</t>
+  </si>
+  <si>
+    <t>hours_review</t>
+  </si>
+  <si>
+    <t>hours_testing</t>
+  </si>
+  <si>
+    <t>hours_integration</t>
+  </si>
+  <si>
+    <t>hours_closed</t>
+  </si>
 </sst>
 </file>
 
@@ -123,7 +162,7 @@
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -171,6 +210,13 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -220,8 +266,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2"/>
   </cellStyleXfs>
   <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -241,6 +288,10 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -253,13 +304,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -301,7 +349,6 @@
   </c:pivotSource>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -367,11 +414,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="110800896"/>
-        <c:axId val="110802432"/>
+        <c:axId val="212641664"/>
+        <c:axId val="212643200"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="110800896"/>
+        <c:axId val="212641664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -380,7 +427,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110802432"/>
+        <c:crossAx val="212643200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -388,7 +435,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="110802432"/>
+        <c:axId val="212643200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -399,14 +446,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110800896"/>
+        <c:crossAx val="212641664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -695,7 +741,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="Piper, Nick" refreshedDate="41418.62409085648" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="243">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="Piper, Nick" refreshedDate="41450.44012777778" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="243">
   <cacheSource type="worksheet">
     <worksheetSource ref="A7:P10000" sheet="Tickets"/>
   </cacheSource>
@@ -746,7 +792,7 @@
     <cacheField name="Changed" numFmtId="0">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
-    <cacheField name="Hours in Status" numFmtId="0">
+    <cacheField name="Days in Status" numFmtId="1">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
     <cacheField name="Resolved" numFmtId="0">
@@ -5150,7 +5196,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="B4:D7" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="16">
     <pivotField showAll="0"/>
@@ -5587,7 +5633,7 @@
   <dimension ref="A1:AMM249"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5602,7 +5648,7 @@
     <col min="8" max="8" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="11" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="11.5703125" style="18" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" style="14" customWidth="1"/>
     <col min="13" max="13" width="9.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="14" max="14" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="15" max="15" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
@@ -5611,69 +5657,69 @@
     <col min="18" max="1027" width="8.7109375" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="16"/>
-      <c r="B1" s="16"/>
+    <row r="1" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="20"/>
+      <c r="B1" s="20"/>
       <c r="G1" s="8"/>
-      <c r="L1" s="17"/>
-    </row>
-    <row r="2" spans="1:17" s="2" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
+      <c r="L1" s="13"/>
+    </row>
+    <row r="2" spans="1:30" s="2" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="20"/>
+      <c r="B2" s="20"/>
       <c r="C2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="L2" s="17"/>
-    </row>
-    <row r="3" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="16"/>
-      <c r="B3" s="16"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="L2" s="13"/>
+    </row>
+    <row r="3" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="20"/>
+      <c r="B3" s="20"/>
       <c r="C3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="L3" s="17"/>
-    </row>
-    <row r="4" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="16"/>
-      <c r="B4" s="16"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="L3" s="13"/>
+    </row>
+    <row r="4" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="20"/>
+      <c r="B4" s="20"/>
       <c r="C4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="15"/>
-      <c r="L4" s="17"/>
-    </row>
-    <row r="5" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="16"/>
-      <c r="B5" s="16"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="19"/>
+      <c r="L4" s="13"/>
+    </row>
+    <row r="5" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="20"/>
+      <c r="B5" s="20"/>
       <c r="G5" s="8"/>
-      <c r="L5" s="17"/>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="L5" s="13"/>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="N6" s="6"/>
       <c r="O6" s="6"/>
       <c r="P6" s="6"/>
     </row>
-    <row r="7" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>3</v>
       </c>
@@ -5707,7 +5753,7 @@
       <c r="K7" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="L7" s="19" t="s">
+      <c r="L7" s="15" t="s">
         <v>24</v>
       </c>
       <c r="M7" s="11" t="s">
@@ -5725,92 +5771,131 @@
       <c r="Q7" s="11" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R7" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="S7" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="T7" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="U7" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="V7" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="W7" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="X7" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y7" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z7" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA7" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB7" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC7" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD7" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
-      <c r="L8" s="20"/>
+      <c r="L8" s="16"/>
       <c r="M8" s="4"/>
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
       <c r="P8" s="5"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
-      <c r="L9" s="20"/>
+      <c r="L9" s="16"/>
       <c r="M9" s="4"/>
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
       <c r="P9" s="5"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
-      <c r="L10" s="20"/>
+      <c r="L10" s="16"/>
       <c r="M10" s="4"/>
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
       <c r="P10" s="5"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
-      <c r="L11" s="20"/>
+      <c r="L11" s="16"/>
       <c r="M11" s="4"/>
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
       <c r="P11" s="5"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
-      <c r="L12" s="20"/>
+      <c r="L12" s="16"/>
       <c r="M12" s="4"/>
       <c r="N12" s="5"/>
       <c r="O12" s="5"/>
       <c r="P12" s="5"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
-      <c r="L13" s="20"/>
+      <c r="L13" s="16"/>
       <c r="M13" s="4"/>
       <c r="N13" s="5"/>
       <c r="O13" s="5"/>
       <c r="P13" s="5"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
-      <c r="L14" s="20"/>
+      <c r="L14" s="16"/>
       <c r="M14" s="4"/>
       <c r="N14" s="5"/>
       <c r="O14" s="5"/>
       <c r="P14" s="5"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
-      <c r="L15" s="20"/>
+      <c r="L15" s="16"/>
       <c r="M15" s="4"/>
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
       <c r="P15" s="5"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
-      <c r="L16" s="20"/>
+      <c r="L16" s="16"/>
       <c r="M16" s="4"/>
       <c r="N16" s="5"/>
       <c r="O16" s="5"/>
@@ -5820,7 +5905,7 @@
       <c r="A17" s="1"/>
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
-      <c r="L17" s="20"/>
+      <c r="L17" s="16"/>
       <c r="M17" s="4"/>
       <c r="N17" s="5"/>
       <c r="O17" s="5"/>
@@ -5830,7 +5915,7 @@
       <c r="A18" s="1"/>
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
-      <c r="L18" s="20"/>
+      <c r="L18" s="16"/>
       <c r="M18" s="4"/>
       <c r="N18" s="5"/>
       <c r="O18" s="5"/>
@@ -5840,7 +5925,7 @@
       <c r="A19" s="1"/>
       <c r="J19" s="4"/>
       <c r="K19" s="4"/>
-      <c r="L19" s="20"/>
+      <c r="L19" s="16"/>
       <c r="M19" s="4"/>
       <c r="N19" s="5"/>
       <c r="O19" s="5"/>
@@ -5850,7 +5935,7 @@
       <c r="A20" s="1"/>
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
-      <c r="L20" s="20"/>
+      <c r="L20" s="16"/>
       <c r="M20" s="4"/>
       <c r="N20" s="5"/>
       <c r="O20" s="5"/>
@@ -5860,7 +5945,7 @@
       <c r="A21" s="1"/>
       <c r="J21" s="4"/>
       <c r="K21" s="4"/>
-      <c r="L21" s="20"/>
+      <c r="L21" s="16"/>
       <c r="M21" s="4"/>
       <c r="N21" s="5"/>
       <c r="O21" s="5"/>
@@ -5870,7 +5955,7 @@
       <c r="A22" s="1"/>
       <c r="J22" s="4"/>
       <c r="K22" s="4"/>
-      <c r="L22" s="20"/>
+      <c r="L22" s="16"/>
       <c r="M22" s="4"/>
       <c r="N22" s="5"/>
       <c r="O22" s="5"/>
@@ -5880,7 +5965,7 @@
       <c r="A23" s="1"/>
       <c r="J23" s="4"/>
       <c r="K23" s="4"/>
-      <c r="L23" s="20"/>
+      <c r="L23" s="16"/>
       <c r="M23" s="4"/>
       <c r="N23" s="5"/>
       <c r="O23" s="5"/>
@@ -5890,7 +5975,7 @@
       <c r="A24" s="1"/>
       <c r="J24" s="4"/>
       <c r="K24" s="4"/>
-      <c r="L24" s="20"/>
+      <c r="L24" s="16"/>
       <c r="M24" s="4"/>
       <c r="N24" s="5"/>
       <c r="O24" s="5"/>
@@ -5900,7 +5985,7 @@
       <c r="A25" s="1"/>
       <c r="J25" s="4"/>
       <c r="K25" s="4"/>
-      <c r="L25" s="20"/>
+      <c r="L25" s="16"/>
       <c r="M25" s="4"/>
       <c r="N25" s="5"/>
       <c r="O25" s="5"/>
@@ -5910,7 +5995,7 @@
       <c r="A26" s="1"/>
       <c r="J26" s="4"/>
       <c r="K26" s="4"/>
-      <c r="L26" s="20"/>
+      <c r="L26" s="16"/>
       <c r="M26" s="4"/>
       <c r="N26" s="5"/>
       <c r="O26" s="5"/>
@@ -5920,7 +6005,7 @@
       <c r="A27" s="1"/>
       <c r="J27" s="4"/>
       <c r="K27" s="4"/>
-      <c r="L27" s="20"/>
+      <c r="L27" s="16"/>
       <c r="M27" s="4"/>
       <c r="N27" s="5"/>
       <c r="O27" s="5"/>
@@ -5930,7 +6015,7 @@
       <c r="A28" s="1"/>
       <c r="J28" s="4"/>
       <c r="K28" s="4"/>
-      <c r="L28" s="20"/>
+      <c r="L28" s="16"/>
       <c r="M28" s="4"/>
       <c r="N28" s="5"/>
       <c r="O28" s="5"/>
@@ -5940,7 +6025,7 @@
       <c r="A29" s="1"/>
       <c r="J29" s="4"/>
       <c r="K29" s="4"/>
-      <c r="L29" s="20"/>
+      <c r="L29" s="16"/>
       <c r="M29" s="4"/>
       <c r="N29" s="5"/>
       <c r="O29" s="5"/>
@@ -5950,7 +6035,7 @@
       <c r="A30" s="1"/>
       <c r="J30" s="4"/>
       <c r="K30" s="4"/>
-      <c r="L30" s="20"/>
+      <c r="L30" s="16"/>
       <c r="M30" s="4"/>
       <c r="N30" s="5"/>
       <c r="O30" s="5"/>
@@ -5960,7 +6045,7 @@
       <c r="A31" s="1"/>
       <c r="J31" s="4"/>
       <c r="K31" s="4"/>
-      <c r="L31" s="20"/>
+      <c r="L31" s="16"/>
       <c r="M31" s="4"/>
       <c r="N31" s="5"/>
       <c r="O31" s="5"/>
@@ -5970,7 +6055,7 @@
       <c r="A32" s="1"/>
       <c r="J32" s="4"/>
       <c r="K32" s="4"/>
-      <c r="L32" s="20"/>
+      <c r="L32" s="16"/>
       <c r="M32" s="4"/>
       <c r="N32" s="5"/>
       <c r="O32" s="5"/>
@@ -5980,7 +6065,7 @@
       <c r="A33" s="1"/>
       <c r="J33" s="4"/>
       <c r="K33" s="4"/>
-      <c r="L33" s="20"/>
+      <c r="L33" s="16"/>
       <c r="M33" s="4"/>
       <c r="N33" s="5"/>
       <c r="O33" s="5"/>
@@ -5990,7 +6075,7 @@
       <c r="A34" s="1"/>
       <c r="J34" s="4"/>
       <c r="K34" s="4"/>
-      <c r="L34" s="20"/>
+      <c r="L34" s="16"/>
       <c r="M34" s="4"/>
       <c r="N34" s="5"/>
       <c r="O34" s="5"/>
@@ -6000,7 +6085,7 @@
       <c r="A35" s="1"/>
       <c r="J35" s="4"/>
       <c r="K35" s="4"/>
-      <c r="L35" s="20"/>
+      <c r="L35" s="16"/>
       <c r="M35" s="4"/>
       <c r="N35" s="5"/>
       <c r="O35" s="5"/>
@@ -6010,7 +6095,7 @@
       <c r="A36" s="1"/>
       <c r="J36" s="4"/>
       <c r="K36" s="4"/>
-      <c r="L36" s="20"/>
+      <c r="L36" s="16"/>
       <c r="M36" s="4"/>
       <c r="N36" s="5"/>
       <c r="O36" s="5"/>
@@ -6020,7 +6105,7 @@
       <c r="A37" s="1"/>
       <c r="J37" s="4"/>
       <c r="K37" s="4"/>
-      <c r="L37" s="20"/>
+      <c r="L37" s="16"/>
       <c r="M37" s="4"/>
       <c r="N37" s="5"/>
       <c r="O37" s="5"/>
@@ -6030,7 +6115,7 @@
       <c r="A38" s="1"/>
       <c r="J38" s="4"/>
       <c r="K38" s="4"/>
-      <c r="L38" s="20"/>
+      <c r="L38" s="16"/>
       <c r="M38" s="4"/>
       <c r="N38" s="5"/>
       <c r="O38" s="5"/>
@@ -6040,7 +6125,7 @@
       <c r="A39" s="1"/>
       <c r="J39" s="4"/>
       <c r="K39" s="4"/>
-      <c r="L39" s="20"/>
+      <c r="L39" s="16"/>
       <c r="M39" s="4"/>
       <c r="N39" s="5"/>
       <c r="O39" s="5"/>
@@ -6050,7 +6135,7 @@
       <c r="A40" s="1"/>
       <c r="J40" s="4"/>
       <c r="K40" s="4"/>
-      <c r="L40" s="20"/>
+      <c r="L40" s="16"/>
       <c r="M40" s="4"/>
       <c r="N40" s="5"/>
       <c r="O40" s="5"/>
@@ -6060,7 +6145,7 @@
       <c r="A41" s="1"/>
       <c r="J41" s="4"/>
       <c r="K41" s="4"/>
-      <c r="L41" s="20"/>
+      <c r="L41" s="16"/>
       <c r="M41" s="4"/>
       <c r="N41" s="5"/>
       <c r="O41" s="5"/>
@@ -6070,7 +6155,7 @@
       <c r="A42" s="1"/>
       <c r="J42" s="4"/>
       <c r="K42" s="4"/>
-      <c r="L42" s="20"/>
+      <c r="L42" s="16"/>
       <c r="M42" s="4"/>
       <c r="N42" s="5"/>
       <c r="O42" s="5"/>
@@ -6080,7 +6165,7 @@
       <c r="A43" s="1"/>
       <c r="J43" s="4"/>
       <c r="K43" s="4"/>
-      <c r="L43" s="20"/>
+      <c r="L43" s="16"/>
       <c r="M43" s="4"/>
       <c r="N43" s="5"/>
       <c r="O43" s="5"/>
@@ -6090,7 +6175,7 @@
       <c r="A44" s="1"/>
       <c r="J44" s="4"/>
       <c r="K44" s="4"/>
-      <c r="L44" s="20"/>
+      <c r="L44" s="16"/>
       <c r="M44" s="4"/>
       <c r="N44" s="5"/>
       <c r="O44" s="5"/>
@@ -6100,7 +6185,7 @@
       <c r="A45" s="1"/>
       <c r="J45" s="4"/>
       <c r="K45" s="4"/>
-      <c r="L45" s="20"/>
+      <c r="L45" s="16"/>
       <c r="M45" s="4"/>
       <c r="N45" s="5"/>
       <c r="O45" s="5"/>
@@ -6110,7 +6195,7 @@
       <c r="A46" s="1"/>
       <c r="J46" s="4"/>
       <c r="K46" s="4"/>
-      <c r="L46" s="20"/>
+      <c r="L46" s="16"/>
       <c r="M46" s="4"/>
       <c r="N46" s="5"/>
       <c r="O46" s="5"/>
@@ -6120,7 +6205,7 @@
       <c r="A47" s="1"/>
       <c r="J47" s="4"/>
       <c r="K47" s="4"/>
-      <c r="L47" s="20"/>
+      <c r="L47" s="16"/>
       <c r="M47" s="4"/>
       <c r="N47" s="5"/>
       <c r="O47" s="5"/>
@@ -6130,7 +6215,7 @@
       <c r="A48" s="1"/>
       <c r="J48" s="4"/>
       <c r="K48" s="4"/>
-      <c r="L48" s="20"/>
+      <c r="L48" s="16"/>
       <c r="M48" s="4"/>
       <c r="N48" s="5"/>
       <c r="O48" s="5"/>
@@ -6140,7 +6225,7 @@
       <c r="A49" s="1"/>
       <c r="J49" s="4"/>
       <c r="K49" s="4"/>
-      <c r="L49" s="20"/>
+      <c r="L49" s="16"/>
       <c r="M49" s="4"/>
       <c r="N49" s="5"/>
       <c r="O49" s="5"/>
@@ -6150,7 +6235,7 @@
       <c r="A50" s="1"/>
       <c r="J50" s="4"/>
       <c r="K50" s="4"/>
-      <c r="L50" s="20"/>
+      <c r="L50" s="16"/>
       <c r="M50" s="4"/>
       <c r="N50" s="5"/>
       <c r="O50" s="5"/>
@@ -6160,7 +6245,7 @@
       <c r="A51" s="1"/>
       <c r="J51" s="4"/>
       <c r="K51" s="4"/>
-      <c r="L51" s="20"/>
+      <c r="L51" s="16"/>
       <c r="M51" s="4"/>
       <c r="N51" s="5"/>
       <c r="O51" s="5"/>
@@ -6170,7 +6255,7 @@
       <c r="A52" s="1"/>
       <c r="J52" s="4"/>
       <c r="K52" s="4"/>
-      <c r="L52" s="20"/>
+      <c r="L52" s="16"/>
       <c r="M52" s="4"/>
       <c r="N52" s="5"/>
       <c r="O52" s="5"/>
@@ -6180,7 +6265,7 @@
       <c r="A53" s="1"/>
       <c r="J53" s="4"/>
       <c r="K53" s="4"/>
-      <c r="L53" s="20"/>
+      <c r="L53" s="16"/>
       <c r="M53" s="4"/>
       <c r="N53" s="5"/>
       <c r="O53" s="5"/>
@@ -6190,7 +6275,7 @@
       <c r="A54" s="1"/>
       <c r="J54" s="4"/>
       <c r="K54" s="4"/>
-      <c r="L54" s="20"/>
+      <c r="L54" s="16"/>
       <c r="M54" s="4"/>
       <c r="N54" s="5"/>
       <c r="O54" s="5"/>
@@ -6200,7 +6285,7 @@
       <c r="A55" s="1"/>
       <c r="J55" s="4"/>
       <c r="K55" s="4"/>
-      <c r="L55" s="20"/>
+      <c r="L55" s="16"/>
       <c r="M55" s="4"/>
       <c r="N55" s="5"/>
       <c r="O55" s="5"/>
@@ -6210,7 +6295,7 @@
       <c r="A56" s="1"/>
       <c r="J56" s="4"/>
       <c r="K56" s="4"/>
-      <c r="L56" s="20"/>
+      <c r="L56" s="16"/>
       <c r="M56" s="4"/>
       <c r="N56" s="5"/>
       <c r="O56" s="5"/>
@@ -6220,7 +6305,7 @@
       <c r="A57" s="1"/>
       <c r="J57" s="4"/>
       <c r="K57" s="4"/>
-      <c r="L57" s="20"/>
+      <c r="L57" s="16"/>
       <c r="M57" s="4"/>
       <c r="N57" s="5"/>
       <c r="O57" s="5"/>
@@ -6230,7 +6315,7 @@
       <c r="A58" s="1"/>
       <c r="J58" s="4"/>
       <c r="K58" s="4"/>
-      <c r="L58" s="20"/>
+      <c r="L58" s="16"/>
       <c r="M58" s="4"/>
       <c r="N58" s="5"/>
       <c r="O58" s="5"/>
@@ -6240,7 +6325,7 @@
       <c r="A59" s="1"/>
       <c r="J59" s="4"/>
       <c r="K59" s="4"/>
-      <c r="L59" s="20"/>
+      <c r="L59" s="16"/>
       <c r="M59" s="4"/>
       <c r="N59" s="5"/>
       <c r="O59" s="5"/>
@@ -6250,7 +6335,7 @@
       <c r="A60" s="1"/>
       <c r="J60" s="4"/>
       <c r="K60" s="4"/>
-      <c r="L60" s="20"/>
+      <c r="L60" s="16"/>
       <c r="M60" s="4"/>
       <c r="N60" s="5"/>
       <c r="O60" s="5"/>
@@ -6260,7 +6345,7 @@
       <c r="A61" s="1"/>
       <c r="J61" s="4"/>
       <c r="K61" s="4"/>
-      <c r="L61" s="20"/>
+      <c r="L61" s="16"/>
       <c r="M61" s="4"/>
       <c r="N61" s="5"/>
       <c r="O61" s="5"/>
@@ -6270,7 +6355,7 @@
       <c r="A62" s="1"/>
       <c r="J62" s="4"/>
       <c r="K62" s="4"/>
-      <c r="L62" s="20"/>
+      <c r="L62" s="16"/>
       <c r="M62" s="4"/>
       <c r="N62" s="5"/>
       <c r="O62" s="5"/>
@@ -6280,7 +6365,7 @@
       <c r="A63" s="1"/>
       <c r="J63" s="4"/>
       <c r="K63" s="4"/>
-      <c r="L63" s="20"/>
+      <c r="L63" s="16"/>
       <c r="M63" s="4"/>
       <c r="N63" s="5"/>
       <c r="O63" s="5"/>
@@ -6290,7 +6375,7 @@
       <c r="A64" s="1"/>
       <c r="J64" s="4"/>
       <c r="K64" s="4"/>
-      <c r="L64" s="20"/>
+      <c r="L64" s="16"/>
       <c r="M64" s="4"/>
       <c r="N64" s="5"/>
       <c r="O64" s="5"/>
@@ -6300,7 +6385,7 @@
       <c r="A65" s="1"/>
       <c r="J65" s="4"/>
       <c r="K65" s="4"/>
-      <c r="L65" s="20"/>
+      <c r="L65" s="16"/>
       <c r="M65" s="4"/>
       <c r="N65" s="5"/>
       <c r="O65" s="5"/>
@@ -6310,7 +6395,7 @@
       <c r="A66" s="1"/>
       <c r="J66" s="4"/>
       <c r="K66" s="4"/>
-      <c r="L66" s="20"/>
+      <c r="L66" s="16"/>
       <c r="M66" s="4"/>
       <c r="N66" s="5"/>
       <c r="O66" s="5"/>
@@ -6320,7 +6405,7 @@
       <c r="A67" s="1"/>
       <c r="J67" s="4"/>
       <c r="K67" s="4"/>
-      <c r="L67" s="20"/>
+      <c r="L67" s="16"/>
       <c r="M67" s="4"/>
       <c r="N67" s="5"/>
       <c r="O67" s="5"/>
@@ -6330,7 +6415,7 @@
       <c r="A68" s="1"/>
       <c r="J68" s="4"/>
       <c r="K68" s="4"/>
-      <c r="L68" s="20"/>
+      <c r="L68" s="16"/>
       <c r="M68" s="4"/>
       <c r="N68" s="5"/>
       <c r="O68" s="5"/>
@@ -6340,7 +6425,7 @@
       <c r="A69" s="1"/>
       <c r="J69" s="4"/>
       <c r="K69" s="4"/>
-      <c r="L69" s="20"/>
+      <c r="L69" s="16"/>
       <c r="M69" s="4"/>
       <c r="N69" s="5"/>
       <c r="O69" s="5"/>
@@ -6350,7 +6435,7 @@
       <c r="A70" s="1"/>
       <c r="J70" s="4"/>
       <c r="K70" s="4"/>
-      <c r="L70" s="20"/>
+      <c r="L70" s="16"/>
       <c r="M70" s="4"/>
       <c r="N70" s="5"/>
       <c r="O70" s="5"/>
@@ -6360,7 +6445,7 @@
       <c r="A71" s="1"/>
       <c r="J71" s="4"/>
       <c r="K71" s="4"/>
-      <c r="L71" s="20"/>
+      <c r="L71" s="16"/>
       <c r="M71" s="4"/>
       <c r="N71" s="5"/>
       <c r="O71" s="5"/>
@@ -6370,7 +6455,7 @@
       <c r="A72" s="1"/>
       <c r="J72" s="4"/>
       <c r="K72" s="4"/>
-      <c r="L72" s="20"/>
+      <c r="L72" s="16"/>
       <c r="M72" s="4"/>
       <c r="N72" s="5"/>
       <c r="O72" s="5"/>
@@ -6380,7 +6465,7 @@
       <c r="A73" s="1"/>
       <c r="J73" s="4"/>
       <c r="K73" s="4"/>
-      <c r="L73" s="20"/>
+      <c r="L73" s="16"/>
       <c r="M73" s="4"/>
       <c r="N73" s="5"/>
       <c r="O73" s="5"/>
@@ -6390,7 +6475,7 @@
       <c r="A74" s="1"/>
       <c r="J74" s="4"/>
       <c r="K74" s="4"/>
-      <c r="L74" s="20"/>
+      <c r="L74" s="16"/>
       <c r="M74" s="4"/>
       <c r="N74" s="5"/>
       <c r="O74" s="5"/>
@@ -6400,7 +6485,7 @@
       <c r="A75" s="1"/>
       <c r="J75" s="4"/>
       <c r="K75" s="4"/>
-      <c r="L75" s="20"/>
+      <c r="L75" s="16"/>
       <c r="M75" s="4"/>
       <c r="N75" s="5"/>
       <c r="O75" s="5"/>
@@ -6410,7 +6495,7 @@
       <c r="A76" s="1"/>
       <c r="J76" s="4"/>
       <c r="K76" s="4"/>
-      <c r="L76" s="20"/>
+      <c r="L76" s="16"/>
       <c r="M76" s="4"/>
       <c r="N76" s="5"/>
       <c r="O76" s="5"/>
@@ -6420,7 +6505,7 @@
       <c r="A77" s="1"/>
       <c r="J77" s="4"/>
       <c r="K77" s="4"/>
-      <c r="L77" s="20"/>
+      <c r="L77" s="16"/>
       <c r="M77" s="4"/>
       <c r="N77" s="5"/>
       <c r="O77" s="5"/>
@@ -6430,7 +6515,7 @@
       <c r="A78" s="1"/>
       <c r="J78" s="4"/>
       <c r="K78" s="4"/>
-      <c r="L78" s="20"/>
+      <c r="L78" s="16"/>
       <c r="M78" s="4"/>
       <c r="N78" s="5"/>
       <c r="O78" s="5"/>
@@ -6440,7 +6525,7 @@
       <c r="A79" s="1"/>
       <c r="J79" s="4"/>
       <c r="K79" s="4"/>
-      <c r="L79" s="20"/>
+      <c r="L79" s="16"/>
       <c r="M79" s="4"/>
       <c r="N79" s="5"/>
       <c r="O79" s="5"/>
@@ -6450,7 +6535,7 @@
       <c r="A80" s="1"/>
       <c r="J80" s="4"/>
       <c r="K80" s="4"/>
-      <c r="L80" s="20"/>
+      <c r="L80" s="16"/>
       <c r="M80" s="4"/>
       <c r="N80" s="5"/>
       <c r="O80" s="5"/>
@@ -6460,7 +6545,7 @@
       <c r="A81" s="1"/>
       <c r="J81" s="4"/>
       <c r="K81" s="4"/>
-      <c r="L81" s="20"/>
+      <c r="L81" s="16"/>
       <c r="M81" s="4"/>
       <c r="N81" s="5"/>
       <c r="O81" s="5"/>
@@ -6470,7 +6555,7 @@
       <c r="A82" s="1"/>
       <c r="J82" s="4"/>
       <c r="K82" s="4"/>
-      <c r="L82" s="20"/>
+      <c r="L82" s="16"/>
       <c r="M82" s="4"/>
       <c r="N82" s="5"/>
       <c r="O82" s="5"/>
@@ -6480,7 +6565,7 @@
       <c r="A83" s="1"/>
       <c r="J83" s="4"/>
       <c r="K83" s="4"/>
-      <c r="L83" s="20"/>
+      <c r="L83" s="16"/>
       <c r="M83" s="4"/>
       <c r="N83" s="5"/>
       <c r="O83" s="5"/>
@@ -6490,7 +6575,7 @@
       <c r="A84" s="1"/>
       <c r="J84" s="4"/>
       <c r="K84" s="4"/>
-      <c r="L84" s="20"/>
+      <c r="L84" s="16"/>
       <c r="M84" s="4"/>
       <c r="N84" s="5"/>
       <c r="O84" s="5"/>
@@ -6500,7 +6585,7 @@
       <c r="A85" s="1"/>
       <c r="J85" s="4"/>
       <c r="K85" s="4"/>
-      <c r="L85" s="20"/>
+      <c r="L85" s="16"/>
       <c r="M85" s="4"/>
       <c r="N85" s="5"/>
       <c r="O85" s="5"/>
@@ -6510,7 +6595,7 @@
       <c r="A86" s="1"/>
       <c r="J86" s="4"/>
       <c r="K86" s="4"/>
-      <c r="L86" s="20"/>
+      <c r="L86" s="16"/>
       <c r="M86" s="4"/>
       <c r="N86" s="5"/>
       <c r="O86" s="5"/>
@@ -6520,7 +6605,7 @@
       <c r="A87" s="1"/>
       <c r="J87" s="4"/>
       <c r="K87" s="4"/>
-      <c r="L87" s="20"/>
+      <c r="L87" s="16"/>
       <c r="M87" s="4"/>
       <c r="N87" s="5"/>
       <c r="O87" s="5"/>
@@ -6530,7 +6615,7 @@
       <c r="A88" s="1"/>
       <c r="J88" s="4"/>
       <c r="K88" s="4"/>
-      <c r="L88" s="20"/>
+      <c r="L88" s="16"/>
       <c r="M88" s="4"/>
       <c r="N88" s="5"/>
       <c r="O88" s="5"/>
@@ -6540,7 +6625,7 @@
       <c r="A89" s="1"/>
       <c r="J89" s="4"/>
       <c r="K89" s="4"/>
-      <c r="L89" s="20"/>
+      <c r="L89" s="16"/>
       <c r="M89" s="4"/>
       <c r="N89" s="5"/>
       <c r="O89" s="5"/>
@@ -6550,7 +6635,7 @@
       <c r="A90" s="1"/>
       <c r="J90" s="4"/>
       <c r="K90" s="4"/>
-      <c r="L90" s="20"/>
+      <c r="L90" s="16"/>
       <c r="M90" s="4"/>
       <c r="N90" s="5"/>
       <c r="O90" s="5"/>
@@ -6560,7 +6645,7 @@
       <c r="A91" s="1"/>
       <c r="J91" s="4"/>
       <c r="K91" s="4"/>
-      <c r="L91" s="20"/>
+      <c r="L91" s="16"/>
       <c r="M91" s="4"/>
       <c r="N91" s="5"/>
       <c r="O91" s="5"/>
@@ -6570,7 +6655,7 @@
       <c r="A92" s="1"/>
       <c r="J92" s="4"/>
       <c r="K92" s="4"/>
-      <c r="L92" s="20"/>
+      <c r="L92" s="16"/>
       <c r="M92" s="4"/>
       <c r="N92" s="5"/>
       <c r="O92" s="5"/>
@@ -6580,7 +6665,7 @@
       <c r="A93" s="1"/>
       <c r="J93" s="4"/>
       <c r="K93" s="4"/>
-      <c r="L93" s="20"/>
+      <c r="L93" s="16"/>
       <c r="M93" s="4"/>
       <c r="N93" s="5"/>
       <c r="O93" s="5"/>
@@ -6590,7 +6675,7 @@
       <c r="A94" s="1"/>
       <c r="J94" s="4"/>
       <c r="K94" s="4"/>
-      <c r="L94" s="20"/>
+      <c r="L94" s="16"/>
       <c r="M94" s="4"/>
       <c r="N94" s="5"/>
       <c r="O94" s="5"/>
@@ -6600,7 +6685,7 @@
       <c r="A95" s="1"/>
       <c r="J95" s="4"/>
       <c r="K95" s="4"/>
-      <c r="L95" s="20"/>
+      <c r="L95" s="16"/>
       <c r="M95" s="4"/>
       <c r="N95" s="5"/>
       <c r="O95" s="5"/>
@@ -6610,7 +6695,7 @@
       <c r="A96" s="1"/>
       <c r="J96" s="4"/>
       <c r="K96" s="4"/>
-      <c r="L96" s="20"/>
+      <c r="L96" s="16"/>
       <c r="M96" s="4"/>
       <c r="N96" s="5"/>
       <c r="O96" s="5"/>
@@ -6620,7 +6705,7 @@
       <c r="A97" s="1"/>
       <c r="J97" s="4"/>
       <c r="K97" s="4"/>
-      <c r="L97" s="20"/>
+      <c r="L97" s="16"/>
       <c r="M97" s="4"/>
       <c r="N97" s="5"/>
       <c r="O97" s="5"/>
@@ -6630,7 +6715,7 @@
       <c r="A98" s="1"/>
       <c r="J98" s="4"/>
       <c r="K98" s="4"/>
-      <c r="L98" s="20"/>
+      <c r="L98" s="16"/>
       <c r="M98" s="4"/>
       <c r="N98" s="5"/>
       <c r="O98" s="5"/>
@@ -6640,7 +6725,7 @@
       <c r="A99" s="1"/>
       <c r="J99" s="4"/>
       <c r="K99" s="4"/>
-      <c r="L99" s="20"/>
+      <c r="L99" s="16"/>
       <c r="M99" s="4"/>
       <c r="N99" s="5"/>
       <c r="O99" s="5"/>
@@ -6650,7 +6735,7 @@
       <c r="A100" s="1"/>
       <c r="J100" s="4"/>
       <c r="K100" s="4"/>
-      <c r="L100" s="20"/>
+      <c r="L100" s="16"/>
       <c r="M100" s="4"/>
       <c r="N100" s="5"/>
       <c r="O100" s="5"/>
@@ -6660,7 +6745,7 @@
       <c r="A101" s="1"/>
       <c r="J101" s="4"/>
       <c r="K101" s="4"/>
-      <c r="L101" s="20"/>
+      <c r="L101" s="16"/>
       <c r="M101" s="4"/>
       <c r="N101" s="5"/>
       <c r="O101" s="5"/>
@@ -6670,7 +6755,7 @@
       <c r="A102" s="1"/>
       <c r="J102" s="4"/>
       <c r="K102" s="4"/>
-      <c r="L102" s="20"/>
+      <c r="L102" s="16"/>
       <c r="M102" s="4"/>
       <c r="N102" s="5"/>
       <c r="O102" s="5"/>
@@ -6680,7 +6765,7 @@
       <c r="A103" s="1"/>
       <c r="J103" s="4"/>
       <c r="K103" s="4"/>
-      <c r="L103" s="20"/>
+      <c r="L103" s="16"/>
       <c r="M103" s="4"/>
       <c r="N103" s="5"/>
       <c r="O103" s="5"/>
@@ -6690,7 +6775,7 @@
       <c r="A104" s="1"/>
       <c r="J104" s="4"/>
       <c r="K104" s="4"/>
-      <c r="L104" s="20"/>
+      <c r="L104" s="16"/>
       <c r="M104" s="4"/>
       <c r="N104" s="5"/>
       <c r="O104" s="5"/>
@@ -6700,7 +6785,7 @@
       <c r="A105" s="1"/>
       <c r="J105" s="4"/>
       <c r="K105" s="4"/>
-      <c r="L105" s="20"/>
+      <c r="L105" s="16"/>
       <c r="M105" s="4"/>
       <c r="N105" s="5"/>
       <c r="O105" s="5"/>
@@ -6710,7 +6795,7 @@
       <c r="A106" s="1"/>
       <c r="J106" s="4"/>
       <c r="K106" s="4"/>
-      <c r="L106" s="20"/>
+      <c r="L106" s="16"/>
       <c r="M106" s="4"/>
       <c r="N106" s="5"/>
       <c r="O106" s="5"/>
@@ -6720,7 +6805,7 @@
       <c r="A107" s="1"/>
       <c r="J107" s="4"/>
       <c r="K107" s="4"/>
-      <c r="L107" s="20"/>
+      <c r="L107" s="16"/>
       <c r="M107" s="4"/>
       <c r="N107" s="5"/>
       <c r="O107" s="5"/>
@@ -6730,7 +6815,7 @@
       <c r="A108" s="1"/>
       <c r="J108" s="4"/>
       <c r="K108" s="4"/>
-      <c r="L108" s="20"/>
+      <c r="L108" s="16"/>
       <c r="M108" s="4"/>
       <c r="N108" s="5"/>
       <c r="O108" s="5"/>
@@ -6740,7 +6825,7 @@
       <c r="A109" s="1"/>
       <c r="J109" s="4"/>
       <c r="K109" s="4"/>
-      <c r="L109" s="20"/>
+      <c r="L109" s="16"/>
       <c r="M109" s="4"/>
       <c r="N109" s="5"/>
       <c r="O109" s="5"/>
@@ -6750,7 +6835,7 @@
       <c r="A110" s="1"/>
       <c r="J110" s="4"/>
       <c r="K110" s="4"/>
-      <c r="L110" s="20"/>
+      <c r="L110" s="16"/>
       <c r="M110" s="4"/>
       <c r="N110" s="5"/>
       <c r="O110" s="5"/>
@@ -6760,7 +6845,7 @@
       <c r="A111" s="1"/>
       <c r="J111" s="4"/>
       <c r="K111" s="4"/>
-      <c r="L111" s="20"/>
+      <c r="L111" s="16"/>
       <c r="M111" s="4"/>
       <c r="N111" s="5"/>
       <c r="O111" s="5"/>
@@ -6770,7 +6855,7 @@
       <c r="A112" s="1"/>
       <c r="J112" s="4"/>
       <c r="K112" s="4"/>
-      <c r="L112" s="20"/>
+      <c r="L112" s="16"/>
       <c r="M112" s="4"/>
       <c r="N112" s="5"/>
       <c r="O112" s="5"/>
@@ -6780,7 +6865,7 @@
       <c r="A113" s="1"/>
       <c r="J113" s="4"/>
       <c r="K113" s="4"/>
-      <c r="L113" s="20"/>
+      <c r="L113" s="16"/>
       <c r="M113" s="4"/>
       <c r="N113" s="5"/>
       <c r="O113" s="5"/>
@@ -6790,7 +6875,7 @@
       <c r="A114" s="1"/>
       <c r="J114" s="4"/>
       <c r="K114" s="4"/>
-      <c r="L114" s="20"/>
+      <c r="L114" s="16"/>
       <c r="M114" s="4"/>
       <c r="N114" s="5"/>
       <c r="O114" s="5"/>
@@ -6800,7 +6885,7 @@
       <c r="A115" s="1"/>
       <c r="J115" s="4"/>
       <c r="K115" s="4"/>
-      <c r="L115" s="20"/>
+      <c r="L115" s="16"/>
       <c r="M115" s="4"/>
       <c r="N115" s="5"/>
       <c r="O115" s="5"/>
@@ -6810,7 +6895,7 @@
       <c r="A116" s="1"/>
       <c r="J116" s="4"/>
       <c r="K116" s="4"/>
-      <c r="L116" s="20"/>
+      <c r="L116" s="16"/>
       <c r="M116" s="4"/>
       <c r="N116" s="5"/>
       <c r="O116" s="5"/>
@@ -6820,7 +6905,7 @@
       <c r="A117" s="1"/>
       <c r="J117" s="4"/>
       <c r="K117" s="4"/>
-      <c r="L117" s="20"/>
+      <c r="L117" s="16"/>
       <c r="M117" s="4"/>
       <c r="N117" s="5"/>
       <c r="O117" s="5"/>
@@ -6830,7 +6915,7 @@
       <c r="A118" s="1"/>
       <c r="J118" s="4"/>
       <c r="K118" s="4"/>
-      <c r="L118" s="20"/>
+      <c r="L118" s="16"/>
       <c r="M118" s="4"/>
       <c r="N118" s="5"/>
       <c r="O118" s="5"/>
@@ -6840,7 +6925,7 @@
       <c r="A119" s="1"/>
       <c r="J119" s="4"/>
       <c r="K119" s="4"/>
-      <c r="L119" s="20"/>
+      <c r="L119" s="16"/>
       <c r="M119" s="4"/>
       <c r="N119" s="5"/>
       <c r="O119" s="5"/>
@@ -6850,7 +6935,7 @@
       <c r="A120" s="1"/>
       <c r="J120" s="4"/>
       <c r="K120" s="4"/>
-      <c r="L120" s="20"/>
+      <c r="L120" s="16"/>
       <c r="M120" s="4"/>
       <c r="N120" s="5"/>
       <c r="O120" s="5"/>
@@ -6860,7 +6945,7 @@
       <c r="A121" s="1"/>
       <c r="J121" s="4"/>
       <c r="K121" s="4"/>
-      <c r="L121" s="20"/>
+      <c r="L121" s="16"/>
       <c r="M121" s="4"/>
       <c r="N121" s="5"/>
       <c r="O121" s="5"/>
@@ -6870,7 +6955,7 @@
       <c r="A122" s="1"/>
       <c r="J122" s="4"/>
       <c r="K122" s="4"/>
-      <c r="L122" s="20"/>
+      <c r="L122" s="16"/>
       <c r="M122" s="4"/>
       <c r="N122" s="5"/>
       <c r="O122" s="5"/>
@@ -6880,7 +6965,7 @@
       <c r="A123" s="1"/>
       <c r="J123" s="4"/>
       <c r="K123" s="4"/>
-      <c r="L123" s="20"/>
+      <c r="L123" s="16"/>
       <c r="M123" s="4"/>
       <c r="N123" s="5"/>
       <c r="O123" s="5"/>
@@ -6890,7 +6975,7 @@
       <c r="A124" s="1"/>
       <c r="J124" s="4"/>
       <c r="K124" s="4"/>
-      <c r="L124" s="20"/>
+      <c r="L124" s="16"/>
       <c r="M124" s="4"/>
       <c r="N124" s="5"/>
       <c r="O124" s="5"/>
@@ -6900,7 +6985,7 @@
       <c r="A125" s="1"/>
       <c r="J125" s="4"/>
       <c r="K125" s="4"/>
-      <c r="L125" s="20"/>
+      <c r="L125" s="16"/>
       <c r="M125" s="4"/>
       <c r="N125" s="5"/>
       <c r="O125" s="5"/>
@@ -6910,7 +6995,7 @@
       <c r="A126" s="1"/>
       <c r="J126" s="4"/>
       <c r="K126" s="4"/>
-      <c r="L126" s="20"/>
+      <c r="L126" s="16"/>
       <c r="M126" s="4"/>
       <c r="N126" s="5"/>
       <c r="O126" s="5"/>
@@ -6920,7 +7005,7 @@
       <c r="A127" s="1"/>
       <c r="J127" s="4"/>
       <c r="K127" s="4"/>
-      <c r="L127" s="20"/>
+      <c r="L127" s="16"/>
       <c r="M127" s="4"/>
       <c r="N127" s="5"/>
       <c r="O127" s="5"/>
@@ -6930,7 +7015,7 @@
       <c r="A128" s="1"/>
       <c r="J128" s="4"/>
       <c r="K128" s="4"/>
-      <c r="L128" s="20"/>
+      <c r="L128" s="16"/>
       <c r="M128" s="4"/>
       <c r="N128" s="5"/>
       <c r="O128" s="5"/>
@@ -6940,7 +7025,7 @@
       <c r="A129" s="1"/>
       <c r="J129" s="4"/>
       <c r="K129" s="4"/>
-      <c r="L129" s="20"/>
+      <c r="L129" s="16"/>
       <c r="M129" s="4"/>
       <c r="N129" s="5"/>
       <c r="O129" s="5"/>
@@ -6950,7 +7035,7 @@
       <c r="A130" s="1"/>
       <c r="J130" s="4"/>
       <c r="K130" s="4"/>
-      <c r="L130" s="20"/>
+      <c r="L130" s="16"/>
       <c r="M130" s="4"/>
       <c r="N130" s="5"/>
       <c r="O130" s="5"/>
@@ -6960,7 +7045,7 @@
       <c r="A131" s="1"/>
       <c r="J131" s="4"/>
       <c r="K131" s="4"/>
-      <c r="L131" s="20"/>
+      <c r="L131" s="16"/>
       <c r="M131" s="4"/>
       <c r="N131" s="5"/>
       <c r="O131" s="5"/>
@@ -6970,7 +7055,7 @@
       <c r="A132" s="1"/>
       <c r="J132" s="4"/>
       <c r="K132" s="4"/>
-      <c r="L132" s="20"/>
+      <c r="L132" s="16"/>
       <c r="M132" s="4"/>
       <c r="N132" s="5"/>
       <c r="O132" s="5"/>
@@ -6980,7 +7065,7 @@
       <c r="A133" s="1"/>
       <c r="J133" s="4"/>
       <c r="K133" s="4"/>
-      <c r="L133" s="20"/>
+      <c r="L133" s="16"/>
       <c r="M133" s="4"/>
       <c r="N133" s="5"/>
       <c r="O133" s="5"/>
@@ -6990,7 +7075,7 @@
       <c r="A134" s="1"/>
       <c r="J134" s="4"/>
       <c r="K134" s="4"/>
-      <c r="L134" s="20"/>
+      <c r="L134" s="16"/>
       <c r="M134" s="4"/>
       <c r="N134" s="5"/>
       <c r="O134" s="5"/>
@@ -7000,7 +7085,7 @@
       <c r="A135" s="1"/>
       <c r="J135" s="4"/>
       <c r="K135" s="4"/>
-      <c r="L135" s="20"/>
+      <c r="L135" s="16"/>
       <c r="M135" s="4"/>
       <c r="N135" s="5"/>
       <c r="O135" s="5"/>
@@ -7010,7 +7095,7 @@
       <c r="A136" s="1"/>
       <c r="J136" s="4"/>
       <c r="K136" s="4"/>
-      <c r="L136" s="20"/>
+      <c r="L136" s="16"/>
       <c r="M136" s="4"/>
       <c r="N136" s="5"/>
       <c r="O136" s="5"/>
@@ -7020,7 +7105,7 @@
       <c r="A137" s="1"/>
       <c r="J137" s="4"/>
       <c r="K137" s="4"/>
-      <c r="L137" s="20"/>
+      <c r="L137" s="16"/>
       <c r="M137" s="4"/>
       <c r="N137" s="5"/>
       <c r="O137" s="5"/>
@@ -7030,7 +7115,7 @@
       <c r="A138" s="1"/>
       <c r="J138" s="4"/>
       <c r="K138" s="4"/>
-      <c r="L138" s="20"/>
+      <c r="L138" s="16"/>
       <c r="M138" s="4"/>
       <c r="N138" s="5"/>
       <c r="O138" s="5"/>
@@ -7040,7 +7125,7 @@
       <c r="A139" s="1"/>
       <c r="J139" s="4"/>
       <c r="K139" s="4"/>
-      <c r="L139" s="20"/>
+      <c r="L139" s="16"/>
       <c r="M139" s="4"/>
       <c r="N139" s="5"/>
       <c r="O139" s="5"/>
@@ -7050,7 +7135,7 @@
       <c r="A140" s="1"/>
       <c r="J140" s="4"/>
       <c r="K140" s="4"/>
-      <c r="L140" s="20"/>
+      <c r="L140" s="16"/>
       <c r="M140" s="4"/>
       <c r="N140" s="5"/>
       <c r="O140" s="5"/>
@@ -7060,7 +7145,7 @@
       <c r="A141" s="1"/>
       <c r="J141" s="4"/>
       <c r="K141" s="4"/>
-      <c r="L141" s="20"/>
+      <c r="L141" s="16"/>
       <c r="M141" s="4"/>
       <c r="N141" s="5"/>
       <c r="O141" s="5"/>
@@ -7070,7 +7155,7 @@
       <c r="A142" s="1"/>
       <c r="J142" s="4"/>
       <c r="K142" s="4"/>
-      <c r="L142" s="20"/>
+      <c r="L142" s="16"/>
       <c r="M142" s="4"/>
       <c r="N142" s="5"/>
       <c r="O142" s="5"/>
@@ -7080,7 +7165,7 @@
       <c r="A143" s="1"/>
       <c r="J143" s="4"/>
       <c r="K143" s="4"/>
-      <c r="L143" s="20"/>
+      <c r="L143" s="16"/>
       <c r="M143" s="4"/>
       <c r="N143" s="5"/>
       <c r="O143" s="5"/>
@@ -7090,7 +7175,7 @@
       <c r="A144" s="1"/>
       <c r="J144" s="4"/>
       <c r="K144" s="4"/>
-      <c r="L144" s="20"/>
+      <c r="L144" s="16"/>
       <c r="M144" s="4"/>
       <c r="N144" s="5"/>
       <c r="O144" s="5"/>
@@ -7100,7 +7185,7 @@
       <c r="A145" s="1"/>
       <c r="J145" s="4"/>
       <c r="K145" s="4"/>
-      <c r="L145" s="20"/>
+      <c r="L145" s="16"/>
       <c r="M145" s="4"/>
       <c r="N145" s="5"/>
       <c r="O145" s="5"/>
@@ -7110,7 +7195,7 @@
       <c r="A146" s="1"/>
       <c r="J146" s="4"/>
       <c r="K146" s="4"/>
-      <c r="L146" s="20"/>
+      <c r="L146" s="16"/>
       <c r="M146" s="4"/>
       <c r="N146" s="5"/>
       <c r="O146" s="5"/>
@@ -7120,7 +7205,7 @@
       <c r="A147" s="1"/>
       <c r="J147" s="4"/>
       <c r="K147" s="4"/>
-      <c r="L147" s="20"/>
+      <c r="L147" s="16"/>
       <c r="M147" s="4"/>
       <c r="N147" s="5"/>
       <c r="O147" s="5"/>
@@ -7130,7 +7215,7 @@
       <c r="A148" s="1"/>
       <c r="J148" s="4"/>
       <c r="K148" s="4"/>
-      <c r="L148" s="20"/>
+      <c r="L148" s="16"/>
       <c r="M148" s="4"/>
       <c r="N148" s="5"/>
       <c r="O148" s="5"/>
@@ -7140,7 +7225,7 @@
       <c r="A149" s="1"/>
       <c r="J149" s="4"/>
       <c r="K149" s="4"/>
-      <c r="L149" s="20"/>
+      <c r="L149" s="16"/>
       <c r="M149" s="4"/>
       <c r="N149" s="5"/>
       <c r="O149" s="5"/>
@@ -7150,7 +7235,7 @@
       <c r="A150" s="1"/>
       <c r="J150" s="4"/>
       <c r="K150" s="4"/>
-      <c r="L150" s="20"/>
+      <c r="L150" s="16"/>
       <c r="M150" s="4"/>
       <c r="N150" s="5"/>
       <c r="O150" s="5"/>
@@ -7160,7 +7245,7 @@
       <c r="A151" s="1"/>
       <c r="J151" s="4"/>
       <c r="K151" s="4"/>
-      <c r="L151" s="20"/>
+      <c r="L151" s="16"/>
       <c r="M151" s="4"/>
       <c r="N151" s="5"/>
       <c r="O151" s="5"/>
@@ -7170,7 +7255,7 @@
       <c r="A152" s="1"/>
       <c r="J152" s="4"/>
       <c r="K152" s="4"/>
-      <c r="L152" s="20"/>
+      <c r="L152" s="16"/>
       <c r="M152" s="4"/>
       <c r="N152" s="5"/>
       <c r="O152" s="5"/>
@@ -7180,7 +7265,7 @@
       <c r="A153" s="1"/>
       <c r="J153" s="4"/>
       <c r="K153" s="4"/>
-      <c r="L153" s="20"/>
+      <c r="L153" s="16"/>
       <c r="M153" s="4"/>
       <c r="N153" s="5"/>
       <c r="O153" s="5"/>
@@ -7190,7 +7275,7 @@
       <c r="A154" s="1"/>
       <c r="J154" s="4"/>
       <c r="K154" s="4"/>
-      <c r="L154" s="20"/>
+      <c r="L154" s="16"/>
       <c r="M154" s="4"/>
       <c r="N154" s="5"/>
       <c r="O154" s="5"/>
@@ -7200,7 +7285,7 @@
       <c r="A155" s="1"/>
       <c r="J155" s="4"/>
       <c r="K155" s="4"/>
-      <c r="L155" s="20"/>
+      <c r="L155" s="16"/>
       <c r="M155" s="4"/>
       <c r="N155" s="5"/>
       <c r="O155" s="5"/>
@@ -7210,7 +7295,7 @@
       <c r="A156" s="1"/>
       <c r="J156" s="4"/>
       <c r="K156" s="4"/>
-      <c r="L156" s="20"/>
+      <c r="L156" s="16"/>
       <c r="M156" s="4"/>
       <c r="N156" s="5"/>
       <c r="O156" s="5"/>
@@ -7220,7 +7305,7 @@
       <c r="A157" s="1"/>
       <c r="J157" s="4"/>
       <c r="K157" s="4"/>
-      <c r="L157" s="20"/>
+      <c r="L157" s="16"/>
       <c r="M157" s="4"/>
       <c r="N157" s="5"/>
       <c r="O157" s="5"/>
@@ -7230,7 +7315,7 @@
       <c r="A158" s="1"/>
       <c r="J158" s="4"/>
       <c r="K158" s="4"/>
-      <c r="L158" s="20"/>
+      <c r="L158" s="16"/>
       <c r="M158" s="4"/>
       <c r="N158" s="5"/>
       <c r="O158" s="5"/>
@@ -7240,7 +7325,7 @@
       <c r="A159" s="1"/>
       <c r="J159" s="4"/>
       <c r="K159" s="4"/>
-      <c r="L159" s="20"/>
+      <c r="L159" s="16"/>
       <c r="M159" s="4"/>
       <c r="N159" s="5"/>
       <c r="O159" s="5"/>
@@ -7250,7 +7335,7 @@
       <c r="A160" s="1"/>
       <c r="J160" s="4"/>
       <c r="K160" s="4"/>
-      <c r="L160" s="20"/>
+      <c r="L160" s="16"/>
       <c r="M160" s="4"/>
       <c r="N160" s="5"/>
       <c r="O160" s="5"/>
@@ -7260,7 +7345,7 @@
       <c r="A161" s="1"/>
       <c r="J161" s="4"/>
       <c r="K161" s="4"/>
-      <c r="L161" s="20"/>
+      <c r="L161" s="16"/>
       <c r="M161" s="4"/>
       <c r="N161" s="5"/>
       <c r="O161" s="5"/>
@@ -7270,7 +7355,7 @@
       <c r="A162" s="1"/>
       <c r="J162" s="4"/>
       <c r="K162" s="4"/>
-      <c r="L162" s="20"/>
+      <c r="L162" s="16"/>
       <c r="M162" s="4"/>
       <c r="N162" s="5"/>
       <c r="O162" s="5"/>
@@ -7280,7 +7365,7 @@
       <c r="A163" s="1"/>
       <c r="J163" s="4"/>
       <c r="K163" s="4"/>
-      <c r="L163" s="20"/>
+      <c r="L163" s="16"/>
       <c r="M163" s="4"/>
       <c r="N163" s="5"/>
       <c r="O163" s="5"/>
@@ -7290,7 +7375,7 @@
       <c r="A164" s="1"/>
       <c r="J164" s="4"/>
       <c r="K164" s="4"/>
-      <c r="L164" s="20"/>
+      <c r="L164" s="16"/>
       <c r="M164" s="4"/>
       <c r="N164" s="5"/>
       <c r="O164" s="5"/>
@@ -7300,7 +7385,7 @@
       <c r="A165" s="1"/>
       <c r="J165" s="4"/>
       <c r="K165" s="4"/>
-      <c r="L165" s="20"/>
+      <c r="L165" s="16"/>
       <c r="M165" s="4"/>
       <c r="N165" s="5"/>
       <c r="O165" s="5"/>
@@ -7310,7 +7395,7 @@
       <c r="A166" s="1"/>
       <c r="J166" s="4"/>
       <c r="K166" s="4"/>
-      <c r="L166" s="20"/>
+      <c r="L166" s="16"/>
       <c r="M166" s="4"/>
       <c r="N166" s="5"/>
       <c r="O166" s="5"/>
@@ -7320,7 +7405,7 @@
       <c r="A167" s="1"/>
       <c r="J167" s="4"/>
       <c r="K167" s="4"/>
-      <c r="L167" s="20"/>
+      <c r="L167" s="16"/>
       <c r="M167" s="4"/>
       <c r="N167" s="5"/>
       <c r="O167" s="5"/>
@@ -7330,7 +7415,7 @@
       <c r="A168" s="1"/>
       <c r="J168" s="4"/>
       <c r="K168" s="4"/>
-      <c r="L168" s="20"/>
+      <c r="L168" s="16"/>
       <c r="M168" s="4"/>
       <c r="N168" s="5"/>
       <c r="O168" s="5"/>
@@ -7340,7 +7425,7 @@
       <c r="A169" s="1"/>
       <c r="J169" s="4"/>
       <c r="K169" s="4"/>
-      <c r="L169" s="20"/>
+      <c r="L169" s="16"/>
       <c r="M169" s="4"/>
       <c r="N169" s="5"/>
       <c r="O169" s="5"/>
@@ -7350,7 +7435,7 @@
       <c r="A170" s="1"/>
       <c r="J170" s="4"/>
       <c r="K170" s="4"/>
-      <c r="L170" s="20"/>
+      <c r="L170" s="16"/>
       <c r="M170" s="4"/>
       <c r="N170" s="5"/>
       <c r="O170" s="5"/>
@@ -7360,7 +7445,7 @@
       <c r="A171" s="1"/>
       <c r="J171" s="4"/>
       <c r="K171" s="4"/>
-      <c r="L171" s="20"/>
+      <c r="L171" s="16"/>
       <c r="M171" s="4"/>
       <c r="N171" s="5"/>
       <c r="O171" s="5"/>
@@ -7370,7 +7455,7 @@
       <c r="A172" s="1"/>
       <c r="J172" s="4"/>
       <c r="K172" s="4"/>
-      <c r="L172" s="20"/>
+      <c r="L172" s="16"/>
       <c r="M172" s="4"/>
       <c r="N172" s="5"/>
       <c r="O172" s="5"/>
@@ -7380,7 +7465,7 @@
       <c r="A173" s="1"/>
       <c r="J173" s="4"/>
       <c r="K173" s="4"/>
-      <c r="L173" s="20"/>
+      <c r="L173" s="16"/>
       <c r="M173" s="4"/>
       <c r="N173" s="5"/>
       <c r="O173" s="5"/>
@@ -7390,7 +7475,7 @@
       <c r="A174" s="1"/>
       <c r="J174" s="4"/>
       <c r="K174" s="4"/>
-      <c r="L174" s="20"/>
+      <c r="L174" s="16"/>
       <c r="M174" s="4"/>
       <c r="N174" s="5"/>
       <c r="O174" s="5"/>
@@ -7400,7 +7485,7 @@
       <c r="A175" s="1"/>
       <c r="J175" s="4"/>
       <c r="K175" s="4"/>
-      <c r="L175" s="20"/>
+      <c r="L175" s="16"/>
       <c r="M175" s="4"/>
       <c r="N175" s="5"/>
       <c r="O175" s="5"/>
@@ -7410,7 +7495,7 @@
       <c r="A176" s="1"/>
       <c r="J176" s="4"/>
       <c r="K176" s="4"/>
-      <c r="L176" s="20"/>
+      <c r="L176" s="16"/>
       <c r="M176" s="4"/>
       <c r="N176" s="5"/>
       <c r="O176" s="5"/>
@@ -7420,7 +7505,7 @@
       <c r="A177" s="1"/>
       <c r="J177" s="4"/>
       <c r="K177" s="4"/>
-      <c r="L177" s="20"/>
+      <c r="L177" s="16"/>
       <c r="M177" s="4"/>
       <c r="N177" s="5"/>
       <c r="O177" s="5"/>
@@ -7430,7 +7515,7 @@
       <c r="A178" s="1"/>
       <c r="J178" s="4"/>
       <c r="K178" s="4"/>
-      <c r="L178" s="20"/>
+      <c r="L178" s="16"/>
       <c r="M178" s="4"/>
       <c r="N178" s="5"/>
       <c r="O178" s="5"/>
@@ -7440,7 +7525,7 @@
       <c r="A179" s="1"/>
       <c r="J179" s="4"/>
       <c r="K179" s="4"/>
-      <c r="L179" s="20"/>
+      <c r="L179" s="16"/>
       <c r="M179" s="4"/>
       <c r="N179" s="5"/>
       <c r="O179" s="5"/>
@@ -7450,7 +7535,7 @@
       <c r="A180" s="1"/>
       <c r="J180" s="4"/>
       <c r="K180" s="4"/>
-      <c r="L180" s="20"/>
+      <c r="L180" s="16"/>
       <c r="M180" s="4"/>
       <c r="N180" s="5"/>
       <c r="O180" s="5"/>
@@ -7460,7 +7545,7 @@
       <c r="A181" s="1"/>
       <c r="J181" s="4"/>
       <c r="K181" s="4"/>
-      <c r="L181" s="20"/>
+      <c r="L181" s="16"/>
       <c r="M181" s="4"/>
       <c r="N181" s="5"/>
       <c r="O181" s="5"/>
@@ -7470,7 +7555,7 @@
       <c r="A182" s="1"/>
       <c r="J182" s="4"/>
       <c r="K182" s="4"/>
-      <c r="L182" s="20"/>
+      <c r="L182" s="16"/>
       <c r="M182" s="4"/>
       <c r="N182" s="5"/>
       <c r="O182" s="5"/>
@@ -7480,7 +7565,7 @@
       <c r="A183" s="1"/>
       <c r="J183" s="4"/>
       <c r="K183" s="4"/>
-      <c r="L183" s="20"/>
+      <c r="L183" s="16"/>
       <c r="M183" s="4"/>
       <c r="N183" s="5"/>
       <c r="O183" s="5"/>
@@ -7490,7 +7575,7 @@
       <c r="A184" s="1"/>
       <c r="J184" s="4"/>
       <c r="K184" s="4"/>
-      <c r="L184" s="20"/>
+      <c r="L184" s="16"/>
       <c r="M184" s="4"/>
       <c r="N184" s="5"/>
       <c r="O184" s="5"/>
@@ -7500,7 +7585,7 @@
       <c r="A185" s="1"/>
       <c r="J185" s="4"/>
       <c r="K185" s="4"/>
-      <c r="L185" s="20"/>
+      <c r="L185" s="16"/>
       <c r="M185" s="4"/>
       <c r="N185" s="5"/>
       <c r="O185" s="5"/>
@@ -7510,7 +7595,7 @@
       <c r="A186" s="1"/>
       <c r="J186" s="4"/>
       <c r="K186" s="4"/>
-      <c r="L186" s="20"/>
+      <c r="L186" s="16"/>
       <c r="M186" s="4"/>
       <c r="N186" s="5"/>
       <c r="O186" s="5"/>
@@ -7520,7 +7605,7 @@
       <c r="A187" s="1"/>
       <c r="J187" s="4"/>
       <c r="K187" s="4"/>
-      <c r="L187" s="20"/>
+      <c r="L187" s="16"/>
       <c r="M187" s="4"/>
       <c r="N187" s="5"/>
       <c r="O187" s="5"/>
@@ -7530,7 +7615,7 @@
       <c r="A188" s="1"/>
       <c r="J188" s="4"/>
       <c r="K188" s="4"/>
-      <c r="L188" s="20"/>
+      <c r="L188" s="16"/>
       <c r="M188" s="4"/>
       <c r="N188" s="5"/>
       <c r="O188" s="5"/>
@@ -7540,7 +7625,7 @@
       <c r="A189" s="1"/>
       <c r="J189" s="4"/>
       <c r="K189" s="4"/>
-      <c r="L189" s="20"/>
+      <c r="L189" s="16"/>
       <c r="M189" s="4"/>
       <c r="N189" s="5"/>
       <c r="O189" s="5"/>
@@ -7550,7 +7635,7 @@
       <c r="A190" s="1"/>
       <c r="J190" s="4"/>
       <c r="K190" s="4"/>
-      <c r="L190" s="20"/>
+      <c r="L190" s="16"/>
       <c r="M190" s="4"/>
       <c r="N190" s="5"/>
       <c r="O190" s="5"/>
@@ -7560,7 +7645,7 @@
       <c r="A191" s="1"/>
       <c r="J191" s="4"/>
       <c r="K191" s="4"/>
-      <c r="L191" s="20"/>
+      <c r="L191" s="16"/>
       <c r="M191" s="4"/>
       <c r="N191" s="5"/>
       <c r="O191" s="5"/>
@@ -7570,7 +7655,7 @@
       <c r="A192" s="1"/>
       <c r="J192" s="4"/>
       <c r="K192" s="4"/>
-      <c r="L192" s="20"/>
+      <c r="L192" s="16"/>
       <c r="M192" s="4"/>
       <c r="N192" s="5"/>
       <c r="O192" s="5"/>
@@ -7580,7 +7665,7 @@
       <c r="A193" s="1"/>
       <c r="J193" s="4"/>
       <c r="K193" s="4"/>
-      <c r="L193" s="20"/>
+      <c r="L193" s="16"/>
       <c r="M193" s="4"/>
       <c r="N193" s="5"/>
       <c r="O193" s="5"/>
@@ -7590,7 +7675,7 @@
       <c r="A194" s="1"/>
       <c r="J194" s="4"/>
       <c r="K194" s="4"/>
-      <c r="L194" s="20"/>
+      <c r="L194" s="16"/>
       <c r="M194" s="4"/>
       <c r="N194" s="5"/>
       <c r="O194" s="5"/>
@@ -7600,7 +7685,7 @@
       <c r="A195" s="1"/>
       <c r="J195" s="4"/>
       <c r="K195" s="4"/>
-      <c r="L195" s="20"/>
+      <c r="L195" s="16"/>
       <c r="M195" s="4"/>
       <c r="N195" s="5"/>
       <c r="O195" s="5"/>
@@ -7610,7 +7695,7 @@
       <c r="A196" s="1"/>
       <c r="J196" s="4"/>
       <c r="K196" s="4"/>
-      <c r="L196" s="20"/>
+      <c r="L196" s="16"/>
       <c r="M196" s="4"/>
       <c r="N196" s="5"/>
       <c r="O196" s="5"/>
@@ -7620,7 +7705,7 @@
       <c r="A197" s="1"/>
       <c r="J197" s="4"/>
       <c r="K197" s="4"/>
-      <c r="L197" s="20"/>
+      <c r="L197" s="16"/>
       <c r="M197" s="4"/>
       <c r="N197" s="5"/>
       <c r="O197" s="5"/>
@@ -7630,7 +7715,7 @@
       <c r="A198" s="1"/>
       <c r="J198" s="4"/>
       <c r="K198" s="4"/>
-      <c r="L198" s="20"/>
+      <c r="L198" s="16"/>
       <c r="M198" s="4"/>
       <c r="N198" s="5"/>
       <c r="O198" s="5"/>
@@ -7640,7 +7725,7 @@
       <c r="A199" s="1"/>
       <c r="J199" s="4"/>
       <c r="K199" s="4"/>
-      <c r="L199" s="20"/>
+      <c r="L199" s="16"/>
       <c r="M199" s="4"/>
       <c r="N199" s="5"/>
       <c r="O199" s="5"/>
@@ -7650,7 +7735,7 @@
       <c r="A200" s="1"/>
       <c r="J200" s="4"/>
       <c r="K200" s="4"/>
-      <c r="L200" s="20"/>
+      <c r="L200" s="16"/>
       <c r="M200" s="4"/>
       <c r="N200" s="5"/>
       <c r="O200" s="5"/>
@@ -7660,7 +7745,7 @@
       <c r="A201" s="1"/>
       <c r="J201" s="4"/>
       <c r="K201" s="4"/>
-      <c r="L201" s="20"/>
+      <c r="L201" s="16"/>
       <c r="M201" s="4"/>
       <c r="N201" s="5"/>
       <c r="O201" s="5"/>
@@ -7670,7 +7755,7 @@
       <c r="A202" s="1"/>
       <c r="J202" s="4"/>
       <c r="K202" s="4"/>
-      <c r="L202" s="20"/>
+      <c r="L202" s="16"/>
       <c r="M202" s="4"/>
       <c r="N202" s="5"/>
       <c r="O202" s="5"/>
@@ -7680,7 +7765,7 @@
       <c r="A203" s="1"/>
       <c r="J203" s="4"/>
       <c r="K203" s="4"/>
-      <c r="L203" s="20"/>
+      <c r="L203" s="16"/>
       <c r="M203" s="4"/>
       <c r="N203" s="5"/>
       <c r="O203" s="5"/>
@@ -7690,7 +7775,7 @@
       <c r="A204" s="1"/>
       <c r="J204" s="4"/>
       <c r="K204" s="4"/>
-      <c r="L204" s="20"/>
+      <c r="L204" s="16"/>
       <c r="M204" s="4"/>
       <c r="N204" s="5"/>
       <c r="O204" s="5"/>
@@ -7700,7 +7785,7 @@
       <c r="A205" s="1"/>
       <c r="J205" s="4"/>
       <c r="K205" s="4"/>
-      <c r="L205" s="20"/>
+      <c r="L205" s="16"/>
       <c r="M205" s="4"/>
       <c r="N205" s="5"/>
       <c r="O205" s="5"/>
@@ -7710,7 +7795,7 @@
       <c r="A206" s="1"/>
       <c r="J206" s="4"/>
       <c r="K206" s="4"/>
-      <c r="L206" s="20"/>
+      <c r="L206" s="16"/>
       <c r="M206" s="4"/>
       <c r="N206" s="5"/>
       <c r="O206" s="5"/>
@@ -7720,7 +7805,7 @@
       <c r="A207" s="1"/>
       <c r="J207" s="4"/>
       <c r="K207" s="4"/>
-      <c r="L207" s="20"/>
+      <c r="L207" s="16"/>
       <c r="M207" s="4"/>
       <c r="N207" s="5"/>
       <c r="O207" s="5"/>
@@ -7853,7 +7938,7 @@
       <c r="A249" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A7:Q7"/>
+  <autoFilter ref="A7:AD7"/>
   <mergeCells count="4">
     <mergeCell ref="D2:J2"/>
     <mergeCell ref="D3:J3"/>
@@ -7861,7 +7946,7 @@
     <mergeCell ref="A1:B5"/>
   </mergeCells>
   <conditionalFormatting sqref="Q1:Q1048576">
-    <cfRule type="dataBar" priority="4">
+    <cfRule type="dataBar" priority="6">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -7873,7 +7958,7 @@
         </ext>
       </extLst>
     </cfRule>
-    <cfRule type="colorScale" priority="6">
+    <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -7883,15 +7968,15 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1 F5:F1048576">
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
       <formula>"critical"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="7" operator="equal">
       <formula>"blocker"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O1:O1048576">
-    <cfRule type="iconSet" priority="2">
+    <cfRule type="iconSet" priority="4">
       <iconSet iconSet="5Quarters">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="20"/>
@@ -7902,7 +7987,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:L1048576">
-    <cfRule type="dataBar" priority="1">
+    <cfRule type="dataBar" priority="3">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -7913,6 +7998,28 @@
           <x14:id>{FA669B14-1E46-499F-B0A6-FE74CCAC2FBC}</x14:id>
         </ext>
       </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R7:AD7">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF555A"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{674EB489-9018-4162-B020-DDEB2FFA5E4F}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -7947,6 +8054,19 @@
           </x14:cfRule>
           <xm:sqref>L1:L1048576</xm:sqref>
         </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{674EB489-9018-4162-B020-DDEB2FFA5E4F}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FFFF555A"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>R7:AD7</xm:sqref>
+        </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
   </extLst>

</xml_diff>